<commit_message>
Sales office data gathering
</commit_message>
<xml_diff>
--- a/SalesOffice_archive.xlsx
+++ b/SalesOffice_archive.xlsx
@@ -279,7 +279,7 @@
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="168" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -672,6 +672,41 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -681,41 +716,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -724,161 +724,6 @@
     <cellStyle name="Porcentaje" xfId="3" builtinId="5"/>
   </cellStyles>
   <dxfs count="16">
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -950,6 +795,161 @@
         <scheme val="minor"/>
       </font>
     </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -972,33 +972,33 @@
   <tableColumns count="19">
     <tableColumn id="1" name="No."/>
     <tableColumn id="23" name="Economy "/>
-    <tableColumn id="2" name="QualityBonus" dataDxfId="11" dataCellStyle="Porcentaje"/>
-    <tableColumn id="3" name="Product" dataDxfId="4" dataCellStyle="Moneda"/>
-    <tableColumn id="7" name="Base price1" dataDxfId="10" dataCellStyle="Moneda"/>
-    <tableColumn id="24" name="Req." dataDxfId="9" dataCellStyle="Millares"/>
+    <tableColumn id="2" name="QualityBonus" dataDxfId="15" dataCellStyle="Porcentaje"/>
+    <tableColumn id="3" name="Product" dataDxfId="14" dataCellStyle="Moneda"/>
+    <tableColumn id="7" name="Base price1" dataDxfId="13" dataCellStyle="Moneda"/>
+    <tableColumn id="24" name="Req." dataDxfId="12" dataCellStyle="Millares"/>
     <tableColumn id="4" name="COGS" dataCellStyle="Moneda"/>
     <tableColumn id="5" name="QOGS"/>
-    <tableColumn id="18" name="Product2" dataDxfId="2" dataCellStyle="Moneda"/>
-    <tableColumn id="8" name="Base price2" dataDxfId="8" dataCellStyle="Moneda"/>
-    <tableColumn id="35" name="Req.2" dataDxfId="7" dataCellStyle="Moneda"/>
+    <tableColumn id="18" name="Product2" dataDxfId="11" dataCellStyle="Moneda"/>
+    <tableColumn id="8" name="Base price2" dataDxfId="10" dataCellStyle="Moneda"/>
+    <tableColumn id="35" name="Req.2" dataDxfId="9" dataCellStyle="Moneda"/>
     <tableColumn id="19" name="COGS2" dataCellStyle="Moneda"/>
     <tableColumn id="20" name="Q2"/>
-    <tableColumn id="12" name="Order price" dataDxfId="0" dataCellStyle="Moneda">
+    <tableColumn id="12" name="Order price" dataDxfId="8" dataCellStyle="Moneda">
       <calculatedColumnFormula>Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]+Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="11" name="Bonus" dataCellStyle="Moneda">
       <calculatedColumnFormula>Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[QOGS]]+Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Q2]]*Tabla22[[#This Row],[QualityBonus]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="p1" dataDxfId="3">
+    <tableColumn id="10" name="p1" dataDxfId="7">
       <calculatedColumnFormula>(Tabla22[[#This Row],[Base price1]]*(1+Tabla22[[#This Row],[QOGS]]*Tabla22[[#This Row],[QualityBonus]])-Tabla22[[#This Row],[COGS]])*Tabla22[[#This Row],[Req.]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="9" name="p2" dataDxfId="6">
       <calculatedColumnFormula>(Tabla22[[#This Row],[Base price2]]*(1+Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Q2]])-Tabla22[[#This Row],[COGS2]])*Tabla22[[#This Row],[Req.2]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="30" name="TOTAL PROFIT (no wages, no admin costs)" dataDxfId="1" dataCellStyle="Moneda">
+    <tableColumn id="30" name="TOTAL PROFIT (no wages, no admin costs)" dataDxfId="5" dataCellStyle="Moneda">
       <calculatedColumnFormula>SUM(Tabla22[[#This Row],[p1]:[p2]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="36" name="profit -wages" dataDxfId="5" dataCellStyle="Moneda">
+    <tableColumn id="36" name="profit -wages" dataDxfId="4" dataCellStyle="Moneda">
       <calculatedColumnFormula>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1007,20 +1007,20 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla3" displayName="Tabla3" ref="B8:E19" totalsRowShown="0" dataDxfId="15" dataCellStyle="Moneda">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla3" displayName="Tabla3" ref="B8:E19" totalsRowShown="0" dataDxfId="3" dataCellStyle="Moneda">
   <autoFilter ref="B8:E19"/>
   <sortState ref="B9:E19">
     <sortCondition ref="B8:B19"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" name="Quality"/>
-    <tableColumn id="2" name="Unit price" dataDxfId="14" dataCellStyle="Moneda">
+    <tableColumn id="2" name="Unit price" dataDxfId="2" dataCellStyle="Moneda">
       <calculatedColumnFormula>$C$3*(1+$C$4*B9)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Unit profit" dataDxfId="13" dataCellStyle="Moneda">
+    <tableColumn id="3" name="Unit profit" dataDxfId="1" dataCellStyle="Moneda">
       <calculatedColumnFormula>C9-$C$5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Total profit" dataDxfId="12" dataCellStyle="Moneda">
+    <tableColumn id="4" name="Total profit" dataDxfId="0" dataCellStyle="Moneda">
       <calculatedColumnFormula>D9*$C$6</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1294,7 +1294,7 @@
   <dimension ref="A2:Y63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1323,10 +1323,10 @@
   <sheetData>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="M2" s="46"/>
-      <c r="N2" s="57" t="s">
+      <c r="N2" s="54" t="s">
         <v>73</v>
       </c>
-      <c r="O2" s="66" t="s">
+      <c r="O2" s="60" t="s">
         <v>15</v>
       </c>
       <c r="P2" s="46"/>
@@ -1335,22 +1335,22 @@
       <c r="S2" s="46"/>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="F3" s="62" t="s">
+      <c r="F3" s="72" t="s">
         <v>70</v>
       </c>
-      <c r="G3" s="63"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="63"/>
-      <c r="J3" s="63"/>
-      <c r="K3" s="64"/>
-      <c r="N3" s="62" t="s">
+      <c r="G3" s="73"/>
+      <c r="H3" s="73"/>
+      <c r="I3" s="73"/>
+      <c r="J3" s="73"/>
+      <c r="K3" s="74"/>
+      <c r="N3" s="72" t="s">
         <v>74</v>
       </c>
-      <c r="O3" s="63"/>
-      <c r="P3" s="63"/>
-      <c r="Q3" s="63"/>
-      <c r="R3" s="63"/>
-      <c r="S3" s="64"/>
+      <c r="O3" s="73"/>
+      <c r="P3" s="73"/>
+      <c r="Q3" s="73"/>
+      <c r="R3" s="73"/>
+      <c r="S3" s="74"/>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B4" s="35" t="s">
@@ -1360,48 +1360,48 @@
         <v>35000</v>
       </c>
       <c r="E4" s="50"/>
-      <c r="F4" s="58" t="s">
+      <c r="F4" s="55" t="s">
         <v>62</v>
       </c>
       <c r="G4" s="52" t="s">
         <v>63</v>
       </c>
-      <c r="H4" s="58" t="s">
+      <c r="H4" s="55" t="s">
         <v>64</v>
       </c>
-      <c r="I4" s="58" t="s">
+      <c r="I4" s="55" t="s">
         <v>77</v>
       </c>
-      <c r="J4" s="58" t="s">
+      <c r="J4" s="55" t="s">
         <v>66</v>
       </c>
-      <c r="K4" s="59" t="s">
+      <c r="K4" s="56" t="s">
         <v>67</v>
       </c>
       <c r="M4" s="50"/>
-      <c r="N4" s="58" t="s">
+      <c r="N4" s="55" t="s">
         <v>62</v>
       </c>
       <c r="O4" s="52" t="s">
         <v>63</v>
       </c>
-      <c r="P4" s="58" t="s">
+      <c r="P4" s="55" t="s">
         <v>64</v>
       </c>
-      <c r="Q4" s="58" t="s">
+      <c r="Q4" s="55" t="s">
         <v>77</v>
       </c>
-      <c r="R4" s="58" t="s">
+      <c r="R4" s="55" t="s">
         <v>66</v>
       </c>
-      <c r="S4" s="59" t="s">
+      <c r="S4" s="56" t="s">
         <v>67</v>
       </c>
       <c r="W4" s="46"/>
       <c r="X4" s="46"/>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="E5" s="67" t="s">
+      <c r="E5" s="61" t="s">
         <v>29</v>
       </c>
       <c r="F5" s="49">
@@ -1428,7 +1428,7 @@
         <f>IFERROR((SUMIF(Tabla22[Product],E5,Tabla22[profit -wages])+SUMIF(Tabla22[Product2],E5,Tabla22[profit -wages]))/(COUNTIF(Tabla22[Product],E5)+COUNTIF(Tabla22[Product2],E5)),0)</f>
         <v>0</v>
       </c>
-      <c r="M5" s="67" t="s">
+      <c r="M5" s="61" t="s">
         <v>29</v>
       </c>
       <c r="N5" s="49">
@@ -1459,7 +1459,7 @@
       <c r="X5" s="46"/>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="E6" s="67" t="s">
+      <c r="E6" s="61" t="s">
         <v>60</v>
       </c>
       <c r="F6" s="47">
@@ -1486,7 +1486,7 @@
         <f>IFERROR((SUMIF(Tabla22[Product],E6,Tabla22[profit -wages])+SUMIF(Tabla22[Product2],E6,Tabla22[profit -wages]))/(COUNTIF(Tabla22[Product],E6)+COUNTIF(Tabla22[Product2],E6)),0)</f>
         <v>0</v>
       </c>
-      <c r="M6" s="67" t="s">
+      <c r="M6" s="61" t="s">
         <v>60</v>
       </c>
       <c r="N6" s="47">
@@ -1517,7 +1517,7 @@
       <c r="X6" s="46"/>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="E7" s="67" t="s">
+      <c r="E7" s="61" t="s">
         <v>56</v>
       </c>
       <c r="F7" s="47">
@@ -1544,7 +1544,7 @@
         <f>IFERROR((SUMIF(Tabla22[Product],E7,Tabla22[profit -wages])+SUMIF(Tabla22[Product2],E7,Tabla22[profit -wages]))/(COUNTIF(Tabla22[Product],E7)+COUNTIF(Tabla22[Product2],E7)),0)</f>
         <v>10667.983933333331</v>
       </c>
-      <c r="M7" s="67" t="s">
+      <c r="M7" s="61" t="s">
         <v>56</v>
       </c>
       <c r="N7" s="47">
@@ -1575,7 +1575,7 @@
       <c r="X7" s="46"/>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="E8" s="67" t="s">
+      <c r="E8" s="61" t="s">
         <v>61</v>
       </c>
       <c r="F8" s="47">
@@ -1602,7 +1602,7 @@
         <f>IFERROR((SUMIF(Tabla22[Product],E8,Tabla22[profit -wages])+SUMIF(Tabla22[Product2],E8,Tabla22[profit -wages]))/(COUNTIF(Tabla22[Product],E8)+COUNTIF(Tabla22[Product2],E8)),0)</f>
         <v>31048.23624999998</v>
       </c>
-      <c r="M8" s="67" t="s">
+      <c r="M8" s="61" t="s">
         <v>61</v>
       </c>
       <c r="N8" s="47">
@@ -1636,7 +1636,7 @@
       <c r="B9" s="50" t="s">
         <v>78</v>
       </c>
-      <c r="E9" s="67" t="s">
+      <c r="E9" s="61" t="s">
         <v>58</v>
       </c>
       <c r="F9" s="47">
@@ -1663,7 +1663,7 @@
         <f>IFERROR((SUMIF(Tabla22[Product],E9,Tabla22[profit -wages])+SUMIF(Tabla22[Product2],E9,Tabla22[profit -wages]))/(COUNTIF(Tabla22[Product],E9)+COUNTIF(Tabla22[Product2],E9)),0)</f>
         <v>21291.601259999989</v>
       </c>
-      <c r="M9" s="67" t="s">
+      <c r="M9" s="61" t="s">
         <v>58</v>
       </c>
       <c r="N9" s="47">
@@ -1694,10 +1694,10 @@
       <c r="X9" s="46"/>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B10" s="73" t="s">
+      <c r="B10" s="63" t="s">
         <v>71</v>
       </c>
-      <c r="E10" s="68" t="s">
+      <c r="E10" s="62" t="s">
         <v>57</v>
       </c>
       <c r="F10" s="48">
@@ -1724,7 +1724,7 @@
         <f>IFERROR((SUMIF(Tabla22[Product],E10,Tabla22[profit -wages])+SUMIF(Tabla22[Product2],E10,Tabla22[profit -wages]))/(COUNTIF(Tabla22[Product],E10)+COUNTIF(Tabla22[Product2],E10)),0)</f>
         <v>-6892.3879999999917</v>
       </c>
-      <c r="M10" s="68" t="s">
+      <c r="M10" s="62" t="s">
         <v>57</v>
       </c>
       <c r="N10" s="48">
@@ -1755,7 +1755,7 @@
       <c r="X10" s="46"/>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B11" s="73" t="s">
+      <c r="B11" s="63" t="s">
         <v>15</v>
       </c>
       <c r="E11" s="51" t="s">
@@ -1769,7 +1769,7 @@
         <f>SUM(G5:G10)</f>
         <v>4</v>
       </c>
-      <c r="H11" s="60">
+      <c r="H11" s="57">
         <f>AVERAGE(Tabla22[QualityBonus])</f>
         <v>2.4216666666666675E-2</v>
       </c>
@@ -1781,7 +1781,7 @@
         <f>AVERAGEIF(Tabla22[TOTAL PROFIT (no wages, no admin costs)],"&gt;0")</f>
         <v>51594.269716666669</v>
       </c>
-      <c r="K11" s="61">
+      <c r="K11" s="58">
         <f>AVERAGE(Tabla22[profit -wages])</f>
         <v>16594.269716666658</v>
       </c>
@@ -1797,7 +1797,7 @@
         <f>SUM(O5:O10)</f>
         <v>4</v>
       </c>
-      <c r="P11" s="60">
+      <c r="P11" s="57">
         <f>IFERROR(AVERAGEIFS(Tabla22[QualityBonus],Tabla22[[Economy ]],$O$2),0)</f>
         <v>2.4216666666666675E-2</v>
       </c>
@@ -1809,7 +1809,7 @@
         <f>IFERROR(AVERAGEIFS(Tabla22[TOTAL PROFIT (no wages, no admin costs)],Tabla22[[Economy ]],$O$2),0)</f>
         <v>51594.269716666669</v>
       </c>
-      <c r="S11" s="61">
+      <c r="S11" s="58">
         <f>IFERROR(AVERAGEIFS(Tabla22[profit -wages],Tabla22[[Economy ]],$O$2),0)</f>
         <v>16594.269716666658</v>
       </c>
@@ -1817,7 +1817,7 @@
       <c r="X11" s="46"/>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B12" s="74" t="s">
+      <c r="B12" s="64" t="s">
         <v>72</v>
       </c>
       <c r="S12" s="46"/>
@@ -1841,26 +1841,26 @@
       <c r="W14" s="46"/>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="D15" s="69" t="s">
+      <c r="D15" s="71" t="s">
         <v>48</v>
       </c>
-      <c r="E15" s="70"/>
-      <c r="F15" s="70"/>
-      <c r="G15" s="70"/>
-      <c r="H15" s="71"/>
-      <c r="I15" s="72" t="s">
+      <c r="E15" s="69"/>
+      <c r="F15" s="69"/>
+      <c r="G15" s="69"/>
+      <c r="H15" s="70"/>
+      <c r="I15" s="68" t="s">
         <v>49</v>
       </c>
-      <c r="J15" s="70"/>
-      <c r="K15" s="70"/>
-      <c r="L15" s="70"/>
-      <c r="M15" s="71"/>
-      <c r="N15" s="72" t="s">
+      <c r="J15" s="69"/>
+      <c r="K15" s="69"/>
+      <c r="L15" s="69"/>
+      <c r="M15" s="70"/>
+      <c r="N15" s="68" t="s">
         <v>53</v>
       </c>
-      <c r="O15" s="70"/>
-      <c r="P15" s="70"/>
-      <c r="Q15" s="71"/>
+      <c r="O15" s="69"/>
+      <c r="P15" s="69"/>
+      <c r="Q15" s="70"/>
       <c r="S15" s="46"/>
       <c r="T15" s="46"/>
       <c r="U15" s="46"/>
@@ -1968,7 +1968,7 @@
       <c r="L17" s="3">
         <v>55000</v>
       </c>
-      <c r="M17" s="76">
+      <c r="M17" s="66">
         <v>5</v>
       </c>
       <c r="N17" s="3">
@@ -2038,7 +2038,7 @@
       <c r="L18" s="3">
         <v>55000</v>
       </c>
-      <c r="M18" s="76">
+      <c r="M18" s="66">
         <v>4</v>
       </c>
       <c r="N18" s="3">
@@ -2108,7 +2108,7 @@
       <c r="L19" s="3">
         <v>55000</v>
       </c>
-      <c r="M19" s="76">
+      <c r="M19" s="66">
         <v>4</v>
       </c>
       <c r="N19" s="3">
@@ -2170,7 +2170,7 @@
       <c r="J20" s="3"/>
       <c r="K20" s="4"/>
       <c r="L20" s="3"/>
-      <c r="M20" s="76"/>
+      <c r="M20" s="66"/>
       <c r="N20" s="3">
         <f>Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]+Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]</f>
         <v>179289</v>
@@ -2238,7 +2238,7 @@
       <c r="L21" s="3">
         <v>56000</v>
       </c>
-      <c r="M21" s="76">
+      <c r="M21" s="66">
         <v>4</v>
       </c>
       <c r="N21" s="3">
@@ -2308,7 +2308,7 @@
       <c r="L22" s="39">
         <v>36500</v>
       </c>
-      <c r="M22" s="77">
+      <c r="M22" s="67">
         <v>6</v>
       </c>
       <c r="N22" s="39">
@@ -2356,7 +2356,7 @@
       <c r="J23" s="3"/>
       <c r="K23" s="4"/>
       <c r="L23" s="3"/>
-      <c r="M23" s="76"/>
+      <c r="M23" s="66"/>
       <c r="N23" s="3">
         <f>Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]+Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]</f>
         <v>0</v>
@@ -2402,7 +2402,7 @@
       <c r="J24" s="3"/>
       <c r="K24" s="4"/>
       <c r="L24" s="3"/>
-      <c r="M24" s="76"/>
+      <c r="M24" s="66"/>
       <c r="N24" s="3">
         <f>Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]+Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]</f>
         <v>0</v>
@@ -2448,7 +2448,7 @@
       <c r="J25" s="3"/>
       <c r="K25" s="4"/>
       <c r="L25" s="3"/>
-      <c r="M25" s="76"/>
+      <c r="M25" s="66"/>
       <c r="N25" s="3">
         <f>Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]+Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]</f>
         <v>0</v>
@@ -2494,7 +2494,7 @@
       <c r="J26" s="3"/>
       <c r="K26" s="4"/>
       <c r="L26" s="3"/>
-      <c r="M26" s="76"/>
+      <c r="M26" s="66"/>
       <c r="N26" s="3">
         <f>Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]+Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]</f>
         <v>0</v>
@@ -2540,7 +2540,7 @@
       <c r="J27" s="3"/>
       <c r="K27" s="4"/>
       <c r="L27" s="3"/>
-      <c r="M27" s="76"/>
+      <c r="M27" s="66"/>
       <c r="N27" s="3">
         <f>Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]+Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]</f>
         <v>0</v>
@@ -2586,7 +2586,7 @@
       <c r="J28" s="3"/>
       <c r="K28" s="4"/>
       <c r="L28" s="3"/>
-      <c r="M28" s="76"/>
+      <c r="M28" s="66"/>
       <c r="N28" s="3">
         <f>Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]+Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]</f>
         <v>0</v>
@@ -2632,7 +2632,7 @@
       <c r="J29" s="3"/>
       <c r="K29" s="4"/>
       <c r="L29" s="3"/>
-      <c r="M29" s="76"/>
+      <c r="M29" s="66"/>
       <c r="N29" s="3">
         <f>Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]+Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]</f>
         <v>0</v>
@@ -2678,7 +2678,7 @@
       <c r="J30" s="3"/>
       <c r="K30" s="4"/>
       <c r="L30" s="3"/>
-      <c r="M30" s="76"/>
+      <c r="M30" s="66"/>
       <c r="N30" s="3">
         <f>Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]+Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]</f>
         <v>0</v>
@@ -2724,7 +2724,7 @@
       <c r="J31" s="3"/>
       <c r="K31" s="4"/>
       <c r="L31" s="3"/>
-      <c r="M31" s="76"/>
+      <c r="M31" s="66"/>
       <c r="N31" s="3">
         <f>Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]+Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]</f>
         <v>0</v>
@@ -2770,7 +2770,7 @@
       <c r="J32" s="3"/>
       <c r="K32" s="4"/>
       <c r="L32" s="3"/>
-      <c r="M32" s="76"/>
+      <c r="M32" s="66"/>
       <c r="N32" s="3">
         <f>Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]+Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]</f>
         <v>0</v>
@@ -2816,7 +2816,7 @@
       <c r="J33" s="3"/>
       <c r="K33" s="4"/>
       <c r="L33" s="3"/>
-      <c r="M33" s="76"/>
+      <c r="M33" s="66"/>
       <c r="N33" s="3">
         <f>Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]+Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]</f>
         <v>0</v>
@@ -2861,7 +2861,7 @@
       <c r="J34" s="3"/>
       <c r="K34" s="4"/>
       <c r="L34" s="3"/>
-      <c r="M34" s="76"/>
+      <c r="M34" s="66"/>
       <c r="N34" s="3">
         <f>Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]+Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]</f>
         <v>0</v>
@@ -2906,7 +2906,7 @@
       <c r="J35" s="3"/>
       <c r="K35" s="4"/>
       <c r="L35" s="3"/>
-      <c r="M35" s="76"/>
+      <c r="M35" s="66"/>
       <c r="N35" s="3">
         <f>Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]+Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]</f>
         <v>0</v>
@@ -2951,7 +2951,7 @@
       <c r="J36" s="3"/>
       <c r="K36" s="4"/>
       <c r="L36" s="3"/>
-      <c r="M36" s="76"/>
+      <c r="M36" s="66"/>
       <c r="N36" s="3">
         <f>Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]+Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]</f>
         <v>0</v>
@@ -2996,7 +2996,7 @@
       <c r="J37" s="3"/>
       <c r="K37" s="4"/>
       <c r="L37" s="3"/>
-      <c r="M37" s="76"/>
+      <c r="M37" s="66"/>
       <c r="N37" s="3">
         <f>Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]+Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]</f>
         <v>0</v>
@@ -3041,7 +3041,7 @@
       <c r="J38" s="3"/>
       <c r="K38" s="4"/>
       <c r="L38" s="3"/>
-      <c r="M38" s="76"/>
+      <c r="M38" s="66"/>
       <c r="N38" s="3">
         <f>Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]+Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]</f>
         <v>0</v>
@@ -3086,7 +3086,7 @@
       <c r="J39" s="3"/>
       <c r="K39" s="4"/>
       <c r="L39" s="3"/>
-      <c r="M39" s="76"/>
+      <c r="M39" s="66"/>
       <c r="N39" s="3">
         <f>Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]+Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]</f>
         <v>0</v>
@@ -3127,7 +3127,7 @@
       <c r="J40" s="3"/>
       <c r="K40" s="4"/>
       <c r="L40" s="3"/>
-      <c r="M40" s="76"/>
+      <c r="M40" s="66"/>
       <c r="N40" s="3">
         <f>Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]+Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]</f>
         <v>0</v>
@@ -3168,7 +3168,7 @@
       <c r="J41" s="3"/>
       <c r="K41" s="4"/>
       <c r="L41" s="3"/>
-      <c r="M41" s="76"/>
+      <c r="M41" s="66"/>
       <c r="N41" s="3">
         <f>Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]+Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]</f>
         <v>0</v>
@@ -3209,7 +3209,7 @@
       <c r="J42" s="3"/>
       <c r="K42" s="4"/>
       <c r="L42" s="3"/>
-      <c r="M42" s="76"/>
+      <c r="M42" s="66"/>
       <c r="N42" s="3">
         <f>Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]+Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]</f>
         <v>0</v>
@@ -3250,7 +3250,7 @@
       <c r="J43" s="3"/>
       <c r="K43" s="4"/>
       <c r="L43" s="3"/>
-      <c r="M43" s="76"/>
+      <c r="M43" s="66"/>
       <c r="N43" s="3">
         <f>Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]+Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]</f>
         <v>0</v>
@@ -3291,7 +3291,7 @@
       <c r="J44" s="3"/>
       <c r="K44" s="4"/>
       <c r="L44" s="3"/>
-      <c r="M44" s="76"/>
+      <c r="M44" s="66"/>
       <c r="N44" s="3">
         <f>Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]+Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]</f>
         <v>0</v>
@@ -3332,7 +3332,7 @@
       <c r="J45" s="3"/>
       <c r="K45" s="4"/>
       <c r="L45" s="3"/>
-      <c r="M45" s="76"/>
+      <c r="M45" s="66"/>
       <c r="N45" s="3">
         <f>Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]+Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]</f>
         <v>0</v>
@@ -3373,7 +3373,7 @@
       <c r="J46" s="3"/>
       <c r="K46" s="4"/>
       <c r="L46" s="3"/>
-      <c r="M46" s="76"/>
+      <c r="M46" s="66"/>
       <c r="N46" s="3">
         <f>Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]+Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]</f>
         <v>0</v>
@@ -3414,7 +3414,7 @@
       <c r="J47" s="3"/>
       <c r="K47" s="4"/>
       <c r="L47" s="3"/>
-      <c r="M47" s="76"/>
+      <c r="M47" s="66"/>
       <c r="N47" s="3">
         <f>Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]+Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]</f>
         <v>0</v>
@@ -3455,7 +3455,7 @@
       <c r="J48" s="3"/>
       <c r="K48" s="4"/>
       <c r="L48" s="3"/>
-      <c r="M48" s="76"/>
+      <c r="M48" s="66"/>
       <c r="N48" s="3">
         <f>Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]+Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]</f>
         <v>0</v>
@@ -3496,7 +3496,7 @@
       <c r="J49" s="3"/>
       <c r="K49" s="3"/>
       <c r="L49" s="3"/>
-      <c r="M49" s="76"/>
+      <c r="M49" s="66"/>
       <c r="N49" s="3">
         <f>Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]+Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]</f>
         <v>0</v>
@@ -3537,7 +3537,7 @@
       <c r="J50" s="3"/>
       <c r="K50" s="4"/>
       <c r="L50" s="3"/>
-      <c r="M50" s="76"/>
+      <c r="M50" s="66"/>
       <c r="N50" s="3">
         <f>Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]+Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]</f>
         <v>0</v>
@@ -3578,7 +3578,7 @@
       <c r="J51" s="3"/>
       <c r="K51" s="3"/>
       <c r="L51" s="3"/>
-      <c r="M51" s="76"/>
+      <c r="M51" s="66"/>
       <c r="N51" s="3">
         <f>Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]+Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]</f>
         <v>0</v>
@@ -3619,7 +3619,7 @@
       <c r="J52" s="3"/>
       <c r="K52" s="4"/>
       <c r="L52" s="3"/>
-      <c r="M52" s="76"/>
+      <c r="M52" s="66"/>
       <c r="N52" s="3">
         <f>Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]+Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]</f>
         <v>0</v>
@@ -3660,7 +3660,7 @@
       <c r="J53" s="3"/>
       <c r="K53" s="3"/>
       <c r="L53" s="3"/>
-      <c r="M53" s="76"/>
+      <c r="M53" s="66"/>
       <c r="N53" s="3">
         <f>Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]+Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]</f>
         <v>0</v>
@@ -3701,7 +3701,7 @@
       <c r="J54" s="3"/>
       <c r="K54" s="4"/>
       <c r="L54" s="3"/>
-      <c r="M54" s="76"/>
+      <c r="M54" s="66"/>
       <c r="N54" s="3">
         <f>Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]+Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]</f>
         <v>0</v>
@@ -3742,7 +3742,7 @@
       <c r="J55" s="3"/>
       <c r="K55" s="3"/>
       <c r="L55" s="3"/>
-      <c r="M55" s="76"/>
+      <c r="M55" s="66"/>
       <c r="N55" s="3">
         <f>Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]+Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]</f>
         <v>0</v>
@@ -3783,7 +3783,7 @@
       <c r="J56" s="3"/>
       <c r="K56" s="4"/>
       <c r="L56" s="3"/>
-      <c r="M56" s="76"/>
+      <c r="M56" s="66"/>
       <c r="N56" s="3">
         <f>Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]+Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]</f>
         <v>0</v>
@@ -3824,7 +3824,7 @@
       <c r="J57" s="3"/>
       <c r="K57" s="3"/>
       <c r="L57" s="3"/>
-      <c r="M57" s="76"/>
+      <c r="M57" s="66"/>
       <c r="N57" s="3">
         <f>Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]+Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]</f>
         <v>0</v>
@@ -3865,7 +3865,7 @@
       <c r="J58" s="3"/>
       <c r="K58" s="4"/>
       <c r="L58" s="3"/>
-      <c r="M58" s="76"/>
+      <c r="M58" s="66"/>
       <c r="N58" s="3">
         <f>Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]+Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]</f>
         <v>0</v>
@@ -3906,7 +3906,7 @@
       <c r="J59" s="3"/>
       <c r="K59" s="3"/>
       <c r="L59" s="3"/>
-      <c r="M59" s="76"/>
+      <c r="M59" s="66"/>
       <c r="N59" s="3">
         <f>Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]+Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]</f>
         <v>0</v>
@@ -3947,7 +3947,7 @@
       <c r="J60" s="3"/>
       <c r="K60" s="4"/>
       <c r="L60" s="3"/>
-      <c r="M60" s="76"/>
+      <c r="M60" s="66"/>
       <c r="N60" s="3">
         <f>Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]+Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]</f>
         <v>0</v>
@@ -3988,7 +3988,7 @@
       <c r="J61" s="3"/>
       <c r="K61" s="3"/>
       <c r="L61" s="3"/>
-      <c r="M61" s="76"/>
+      <c r="M61" s="66"/>
       <c r="N61" s="3">
         <f>Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]+Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]</f>
         <v>0</v>
@@ -4029,7 +4029,7 @@
       <c r="J62" s="3"/>
       <c r="K62" s="4"/>
       <c r="L62" s="3"/>
-      <c r="M62" s="76"/>
+      <c r="M62" s="66"/>
       <c r="N62" s="3">
         <f>Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]+Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]</f>
         <v>0</v>
@@ -4070,7 +4070,7 @@
       <c r="J63" s="3"/>
       <c r="K63" s="3"/>
       <c r="L63" s="3"/>
-      <c r="M63" s="76"/>
+      <c r="M63" s="66"/>
       <c r="N63" s="3">
         <f>Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]+Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]</f>
         <v>0</v>
@@ -4287,33 +4287,33 @@
         <v>63</v>
       </c>
       <c r="H5" s="12"/>
-      <c r="I5" s="54" t="s">
+      <c r="I5" s="75" t="s">
         <v>16</v>
       </c>
-      <c r="J5" s="54"/>
-      <c r="K5" s="54"/>
-      <c r="L5" s="54"/>
-      <c r="M5" s="54"/>
-      <c r="N5" s="54"/>
-      <c r="O5" s="54"/>
-      <c r="P5" s="54"/>
-      <c r="Q5" s="54"/>
-      <c r="R5" s="54"/>
-      <c r="S5" s="55"/>
+      <c r="J5" s="75"/>
+      <c r="K5" s="75"/>
+      <c r="L5" s="75"/>
+      <c r="M5" s="75"/>
+      <c r="N5" s="75"/>
+      <c r="O5" s="75"/>
+      <c r="P5" s="75"/>
+      <c r="Q5" s="75"/>
+      <c r="R5" s="75"/>
+      <c r="S5" s="76"/>
       <c r="U5" s="12"/>
-      <c r="V5" s="54" t="s">
+      <c r="V5" s="75" t="s">
         <v>18</v>
       </c>
-      <c r="W5" s="54"/>
-      <c r="X5" s="54"/>
-      <c r="Y5" s="54"/>
-      <c r="Z5" s="54"/>
-      <c r="AA5" s="54"/>
-      <c r="AB5" s="54"/>
-      <c r="AC5" s="54"/>
-      <c r="AD5" s="54"/>
-      <c r="AE5" s="54"/>
-      <c r="AF5" s="55"/>
+      <c r="W5" s="75"/>
+      <c r="X5" s="75"/>
+      <c r="Y5" s="75"/>
+      <c r="Z5" s="75"/>
+      <c r="AA5" s="75"/>
+      <c r="AB5" s="75"/>
+      <c r="AC5" s="75"/>
+      <c r="AD5" s="75"/>
+      <c r="AE5" s="75"/>
+      <c r="AF5" s="76"/>
     </row>
     <row r="6" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
@@ -6654,33 +6654,33 @@
         <v>70.928000000000011</v>
       </c>
       <c r="H30" s="12"/>
-      <c r="I30" s="54" t="s">
+      <c r="I30" s="75" t="s">
         <v>19</v>
       </c>
-      <c r="J30" s="54"/>
-      <c r="K30" s="54"/>
-      <c r="L30" s="54"/>
-      <c r="M30" s="54"/>
-      <c r="N30" s="54"/>
-      <c r="O30" s="54"/>
-      <c r="P30" s="54"/>
-      <c r="Q30" s="54"/>
-      <c r="R30" s="54"/>
-      <c r="S30" s="55"/>
+      <c r="J30" s="75"/>
+      <c r="K30" s="75"/>
+      <c r="L30" s="75"/>
+      <c r="M30" s="75"/>
+      <c r="N30" s="75"/>
+      <c r="O30" s="75"/>
+      <c r="P30" s="75"/>
+      <c r="Q30" s="75"/>
+      <c r="R30" s="75"/>
+      <c r="S30" s="76"/>
       <c r="U30" s="12"/>
-      <c r="V30" s="54" t="s">
+      <c r="V30" s="75" t="s">
         <v>17</v>
       </c>
-      <c r="W30" s="54"/>
-      <c r="X30" s="54"/>
-      <c r="Y30" s="54"/>
-      <c r="Z30" s="54"/>
-      <c r="AA30" s="54"/>
-      <c r="AB30" s="54"/>
-      <c r="AC30" s="54"/>
-      <c r="AD30" s="54"/>
-      <c r="AE30" s="54"/>
-      <c r="AF30" s="55"/>
+      <c r="W30" s="75"/>
+      <c r="X30" s="75"/>
+      <c r="Y30" s="75"/>
+      <c r="Z30" s="75"/>
+      <c r="AA30" s="75"/>
+      <c r="AB30" s="75"/>
+      <c r="AC30" s="75"/>
+      <c r="AD30" s="75"/>
+      <c r="AE30" s="75"/>
+      <c r="AF30" s="76"/>
     </row>
     <row r="31" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B31" s="29" t="s">
@@ -8793,14 +8793,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="77" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
     </row>
     <row r="2" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -8824,7 +8824,7 @@
       <c r="K2" t="s">
         <v>32</v>
       </c>
-      <c r="M2" s="65">
+      <c r="M2" s="59">
         <f>Archive!G11</f>
         <v>4</v>
       </c>
@@ -9226,27 +9226,27 @@
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="75">
+      <c r="B22" s="65">
         <f>1/B21</f>
         <v>3.8987942119447637E-2</v>
       </c>
-      <c r="C22" s="75">
+      <c r="C22" s="65">
         <f t="shared" ref="C22:G22" si="5">1/C21</f>
         <v>6.3494970008711626E-2</v>
       </c>
-      <c r="D22" s="75">
+      <c r="D22" s="65">
         <f t="shared" si="5"/>
         <v>9.5013907917133725E-2</v>
       </c>
-      <c r="E22" s="75">
+      <c r="E22" s="65">
         <f t="shared" si="5"/>
         <v>0.13738249312667331</v>
       </c>
-      <c r="F22" s="75">
+      <c r="F22" s="65">
         <f t="shared" si="5"/>
         <v>0.27325262077035128</v>
       </c>
-      <c r="G22" s="75">
+      <c r="G22" s="65">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Cant afford to pay more than 43k of wages per order
</commit_message>
<xml_diff>
--- a/SalesOffice_archive.xlsx
+++ b/SalesOffice_archive.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="82">
   <si>
     <t>QualityBonus</t>
   </si>
@@ -223,9 +223,6 @@
     <t>Avg profit-w</t>
   </si>
   <si>
-    <t>TOTAL PROFIT (no wages, no admin costs)</t>
-  </si>
-  <si>
     <t>Product2</t>
   </si>
   <si>
@@ -272,6 +269,9 @@
   </si>
   <si>
     <t>Prob</t>
+  </si>
+  <si>
+    <t>P_T</t>
   </si>
 </sst>
 </file>
@@ -366,7 +366,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -604,26 +604,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="0"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color theme="0"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -631,7 +611,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
@@ -711,15 +691,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -731,6 +702,7 @@
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -741,6 +713,13 @@
     <xf numFmtId="164" fontId="0" fillId="7" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -748,7 +727,48 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentaje" xfId="3" builtinId="5"/>
   </cellStyles>
-  <dxfs count="25">
+  <dxfs count="26">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFABAB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -906,18 +926,6 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -936,23 +944,6 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -1156,41 +1147,41 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla22" displayName="Tabla22" ref="A16:P101" totalsRowShown="0">
-  <autoFilter ref="A16:P101"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla22" displayName="Tabla22" ref="A16:P104" totalsRowShown="0">
+  <autoFilter ref="A16:P104"/>
   <sortState ref="A17:R63">
     <sortCondition ref="A16:A63"/>
   </sortState>
   <tableColumns count="16">
     <tableColumn id="1" name="No."/>
     <tableColumn id="23" name="Economy "/>
-    <tableColumn id="2" name="QualityBonus" dataDxfId="24" dataCellStyle="Porcentaje"/>
-    <tableColumn id="3" name="Product" dataDxfId="23" dataCellStyle="Moneda"/>
-    <tableColumn id="7" name="Base price1" dataDxfId="22" dataCellStyle="Moneda"/>
-    <tableColumn id="24" name="Req." dataDxfId="21" dataCellStyle="Millares"/>
-    <tableColumn id="18" name="Product2" dataDxfId="20" dataCellStyle="Moneda"/>
-    <tableColumn id="8" name="Base price2" dataDxfId="15" dataCellStyle="Moneda"/>
-    <tableColumn id="35" name="Req.2" dataDxfId="14" dataCellStyle="Millares"/>
-    <tableColumn id="12" name="Order price" dataDxfId="10" dataCellStyle="Moneda">
+    <tableColumn id="2" name="QualityBonus" dataDxfId="25" dataCellStyle="Porcentaje"/>
+    <tableColumn id="3" name="Product" dataDxfId="24" dataCellStyle="Moneda"/>
+    <tableColumn id="7" name="Base price1" dataDxfId="23" dataCellStyle="Moneda"/>
+    <tableColumn id="24" name="Req." dataDxfId="22" dataCellStyle="Millares"/>
+    <tableColumn id="18" name="Product2" dataDxfId="21" dataCellStyle="Moneda"/>
+    <tableColumn id="8" name="Base price2" dataDxfId="16" dataCellStyle="Moneda"/>
+    <tableColumn id="35" name="Req.2" dataDxfId="15" dataCellStyle="Millares"/>
+    <tableColumn id="12" name="Order price" dataDxfId="12" dataCellStyle="Moneda">
       <calculatedColumnFormula>Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]+Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Bonus1" dataDxfId="13" dataCellStyle="Moneda">
-      <calculatedColumnFormula>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</calculatedColumnFormula>
+    <tableColumn id="4" name="Bonus1" dataDxfId="2" dataCellStyle="Moneda">
+      <calculatedColumnFormula>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="11" name="Bonus2" dataCellStyle="Moneda">
       <calculatedColumnFormula>IF(Tabla22[[#This Row],[Req.2]]&gt;0,LOOKUP(Tabla22[[#This Row],[Product2]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]*Tabla22[[#This Row],[QualityBonus]],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="p1" dataDxfId="9" dataCellStyle="Moneda">
-      <calculatedColumnFormula>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</calculatedColumnFormula>
+    <tableColumn id="10" name="p1" dataDxfId="1" dataCellStyle="Moneda">
+      <calculatedColumnFormula>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="9" name="p2" dataCellStyle="Moneda">
       <calculatedColumnFormula>IF(Tabla22[[#This Row],[Req.2]]&gt;0,(Tabla22[[#This Row],[Base price2]]-LOOKUP(Tabla22[[#This Row],[Product2]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.2]],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="30" name="TOTAL PROFIT (no wages, no admin costs)" dataDxfId="8" dataCellStyle="Moneda">
+    <tableColumn id="30" name="P_T" dataDxfId="11" dataCellStyle="Moneda">
       <calculatedColumnFormula>SUM(Tabla22[[#This Row],[Bonus1]:[p2]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="36" name="profit -wages" dataCellStyle="Moneda">
-      <calculatedColumnFormula>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</calculatedColumnFormula>
+      <calculatedColumnFormula>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1198,35 +1189,35 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="R17:T23" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="R17:T23" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="7">
   <autoFilter ref="R17:T23"/>
   <sortState ref="T18:V23">
     <sortCondition ref="T17:T23"/>
   </sortState>
   <tableColumns count="3">
-    <tableColumn id="1" name="Goods sold" dataDxfId="7"/>
-    <tableColumn id="2" name="COGS" dataDxfId="6"/>
-    <tableColumn id="3" name="Q" dataDxfId="5"/>
+    <tableColumn id="1" name="Goods sold" dataDxfId="10"/>
+    <tableColumn id="2" name="COGS" dataDxfId="9"/>
+    <tableColumn id="3" name="Q" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla3" displayName="Tabla3" ref="B8:E19" totalsRowShown="0" dataDxfId="19" dataCellStyle="Moneda">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla3" displayName="Tabla3" ref="B8:E19" totalsRowShown="0" dataDxfId="20" dataCellStyle="Moneda">
   <autoFilter ref="B8:E19"/>
   <sortState ref="B9:E19">
     <sortCondition ref="B8:B19"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" name="Quality"/>
-    <tableColumn id="2" name="Unit price" dataDxfId="18" dataCellStyle="Moneda">
+    <tableColumn id="2" name="Unit price" dataDxfId="19" dataCellStyle="Moneda">
       <calculatedColumnFormula>$C$3*(1+$C$4*B9)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Unit profit" dataDxfId="17" dataCellStyle="Moneda">
+    <tableColumn id="3" name="Unit profit" dataDxfId="18" dataCellStyle="Moneda">
       <calculatedColumnFormula>C9-$C$5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Total profit" dataDxfId="16" dataCellStyle="Moneda">
+    <tableColumn id="4" name="Total profit" dataDxfId="17" dataCellStyle="Moneda">
       <calculatedColumnFormula>D9*$C$6</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1497,27 +1488,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:Z101"/>
+  <dimension ref="A2:Z104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
     <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.140625" customWidth="1"/>
+    <col min="5" max="5" width="23" customWidth="1"/>
     <col min="6" max="6" width="9.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" customWidth="1"/>
     <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" customWidth="1"/>
     <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.140625" customWidth="1"/>
-    <col min="13" max="13" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.5703125" customWidth="1"/>
     <col min="14" max="14" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="16" customWidth="1"/>
     <col min="16" max="16" width="15.85546875" bestFit="1" customWidth="1"/>
@@ -1530,7 +1521,7 @@
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="M2" s="46"/>
       <c r="N2" s="54" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="O2" s="60" t="s">
         <v>13</v>
@@ -1541,32 +1532,32 @@
       <c r="S2" s="46"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="F3" s="83" t="s">
-        <v>67</v>
-      </c>
-      <c r="G3" s="84"/>
-      <c r="H3" s="84"/>
-      <c r="I3" s="84"/>
-      <c r="J3" s="84"/>
-      <c r="K3" s="84"/>
-      <c r="L3" s="84"/>
-      <c r="N3" s="83" t="s">
-        <v>71</v>
-      </c>
-      <c r="O3" s="84"/>
-      <c r="P3" s="84"/>
-      <c r="Q3" s="84"/>
-      <c r="R3" s="84"/>
-      <c r="S3" s="84"/>
-      <c r="T3" s="84"/>
-      <c r="U3" s="84"/>
+      <c r="F3" s="81" t="s">
+        <v>66</v>
+      </c>
+      <c r="G3" s="82"/>
+      <c r="H3" s="82"/>
+      <c r="I3" s="82"/>
+      <c r="J3" s="82"/>
+      <c r="K3" s="82"/>
+      <c r="L3" s="82"/>
+      <c r="N3" s="81" t="s">
+        <v>70</v>
+      </c>
+      <c r="O3" s="82"/>
+      <c r="P3" s="82"/>
+      <c r="Q3" s="82"/>
+      <c r="R3" s="82"/>
+      <c r="S3" s="82"/>
+      <c r="T3" s="82"/>
+      <c r="U3" s="82"/>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B4" s="35" t="s">
         <v>21</v>
       </c>
       <c r="C4" s="36">
-        <v>37400</v>
+        <v>43000</v>
       </c>
       <c r="E4" s="50"/>
       <c r="F4" s="55" t="s">
@@ -1576,13 +1567,13 @@
         <v>60</v>
       </c>
       <c r="H4" s="52" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I4" s="55" t="s">
         <v>61</v>
       </c>
       <c r="J4" s="55" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K4" s="55" t="s">
         <v>63</v>
@@ -1598,13 +1589,13 @@
         <v>60</v>
       </c>
       <c r="Q4" s="52" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R4" s="55" t="s">
         <v>61</v>
       </c>
       <c r="S4" s="55" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="T4" s="55" t="s">
         <v>63</v>
@@ -1627,7 +1618,7 @@
         <f>F5/COUNTIF(Tabla22[QualityBonus],"&gt;0")</f>
         <v>5.2631578947368418E-2</v>
       </c>
-      <c r="H5" s="81">
+      <c r="H5" s="79">
         <f>G5/$G$11</f>
         <v>1.1235955056179775E-2</v>
       </c>
@@ -1640,12 +1631,12 @@
         <v>835083</v>
       </c>
       <c r="K5" s="23">
-        <f>IFERROR((SUMIF(Tabla22[Product],E5,Tabla22[TOTAL PROFIT (no wages, no admin costs)])+SUMIF(Tabla22[Product2],E5,Tabla22[TOTAL PROFIT (no wages, no admin costs)]))/(COUNTIF(Tabla22[Product],E5)+COUNTIF(Tabla22[Product2],E5)),0)</f>
+        <f>IFERROR((SUMIF(Tabla22[Product],E5,Tabla22[P_T])+SUMIF(Tabla22[Product2],E5,Tabla22[P_T]))/(COUNTIF(Tabla22[Product],E5)+COUNTIF(Tabla22[Product2],E5)),0)</f>
         <v>250346.85399999999</v>
       </c>
       <c r="L5" s="42">
         <f>IFERROR((SUMIF(Tabla22[Product],E5,Tabla22[profit -wages])+SUMIF(Tabla22[Product2],E5,Tabla22[profit -wages]))/(COUNTIF(Tabla22[Product],E5)+COUNTIF(Tabla22[Product2],E5)),0)</f>
-        <v>212946.85399999999</v>
+        <v>207346.85399999999</v>
       </c>
       <c r="N5" s="61" t="s">
         <v>27</v>
@@ -1656,7 +1647,7 @@
       </c>
       <c r="P5" s="47">
         <f>IFERROR(O5/COUNTIF(Tabla22[[Economy ]],$O$2),0)</f>
-        <v>4.7058823529411764E-2</v>
+        <v>4.5454545454545456E-2</v>
       </c>
       <c r="Q5" s="37">
         <f>P5/$P$11</f>
@@ -1671,12 +1662,12 @@
         <v>835083</v>
       </c>
       <c r="T5" s="23">
-        <f>IFERROR((SUMIFS(Tabla22[TOTAL PROFIT (no wages, no admin costs)],Tabla22[Product],N5,Tabla22[[Economy ]],$O$2)+SUMIFS(Tabla22[TOTAL PROFIT (no wages, no admin costs)],Tabla22[Product2],N5,Tabla22[[Economy ]],$O$2))/(COUNTIFS(Tabla22[Product],N5,Tabla22[[Economy ]],$O$2)+COUNTIFS(Tabla22[Product2],N5,Tabla22[[Economy ]],$O$2)),0)</f>
+        <f>IFERROR((SUMIFS(Tabla22[P_T],Tabla22[Product],N5,Tabla22[[Economy ]],$O$2)+SUMIFS(Tabla22[P_T],Tabla22[Product2],N5,Tabla22[[Economy ]],$O$2))/(COUNTIFS(Tabla22[Product],N5,Tabla22[[Economy ]],$O$2)+COUNTIFS(Tabla22[Product2],N5,Tabla22[[Economy ]],$O$2)),0)</f>
         <v>250346.85399999999</v>
       </c>
       <c r="U5" s="42">
         <f>IFERROR((SUMIFS(Tabla22[profit -wages],Tabla22[Product],E5,Tabla22[[Economy ]],$O$2)+SUMIFS(Tabla22[profit -wages],Tabla22[Product2],E5,Tabla22[[Economy ]],$O$2))/(COUNTIFS(Tabla22[Product],E5,Tabla22[[Economy ]],$O$2)+COUNTIFS(Tabla22[Product2],E5,Tabla22[[Economy ]],$O$2)),0)</f>
-        <v>212946.85399999999</v>
+        <v>207346.85399999999</v>
       </c>
       <c r="Y5" s="46"/>
       <c r="Z5" s="46"/>
@@ -1693,7 +1684,7 @@
         <f>F6/COUNTIF(Tabla22[QualityBonus],"&gt;0")</f>
         <v>0.11842105263157894</v>
       </c>
-      <c r="H6" s="81">
+      <c r="H6" s="79">
         <f t="shared" ref="H6:H10" si="0">G6/$G$11</f>
         <v>2.5280898876404494E-2</v>
       </c>
@@ -1706,12 +1697,12 @@
         <v>226108</v>
       </c>
       <c r="K6" s="3">
-        <f>IFERROR((SUMIF(Tabla22[Product],E6,Tabla22[TOTAL PROFIT (no wages, no admin costs)])+SUMIF(Tabla22[Product2],E6,Tabla22[TOTAL PROFIT (no wages, no admin costs)]))/(COUNTIF(Tabla22[Product],E6)+COUNTIF(Tabla22[Product2],E6)),0)</f>
+        <f>IFERROR((SUMIF(Tabla22[Product],E6,Tabla22[P_T])+SUMIF(Tabla22[Product2],E6,Tabla22[P_T]))/(COUNTIF(Tabla22[Product],E6)+COUNTIF(Tabla22[Product2],E6)),0)</f>
         <v>54273.788524999996</v>
       </c>
       <c r="L6" s="43">
         <f>IFERROR((SUMIF(Tabla22[Product],E6,Tabla22[profit -wages])+SUMIF(Tabla22[Product2],E6,Tabla22[profit -wages]))/(COUNTIF(Tabla22[Product],E6)+COUNTIF(Tabla22[Product2],E6)),0)</f>
-        <v>16873.788525000004</v>
+        <v>11273.788525000004</v>
       </c>
       <c r="N6" s="61" t="s">
         <v>57</v>
@@ -1722,11 +1713,11 @@
       </c>
       <c r="P6" s="47">
         <f>IFERROR(O6/COUNTIF(Tabla22[[Economy ]],$O$2),0)</f>
-        <v>0.10588235294117647</v>
+        <v>0.10227272727272728</v>
       </c>
       <c r="Q6" s="37">
         <f t="shared" ref="Q6:Q10" si="1">P6/$P$11</f>
-        <v>2.5280898876404497E-2</v>
+        <v>2.5280898876404501E-2</v>
       </c>
       <c r="R6" s="37">
         <f>IFERROR((SUMIFS(Tabla22[QualityBonus],Tabla22[Product],N6,Tabla22[[Economy ]],$O$2)+SUMIFS(Tabla22[QualityBonus],Tabla22[Product2],N6,Tabla22[[Economy ]],$O$2))/(COUNTIFS(Tabla22[Product],N6,Tabla22[[Economy ]],$O$2)+COUNTIFS(Tabla22[Product2],N6,Tabla22[[Economy ]],$O$2)),0)</f>
@@ -1737,12 +1728,12 @@
         <v>226108</v>
       </c>
       <c r="T6" s="3">
-        <f>IFERROR((SUMIFS(Tabla22[TOTAL PROFIT (no wages, no admin costs)],Tabla22[Product],N6,Tabla22[[Economy ]],$O$2)+SUMIFS(Tabla22[TOTAL PROFIT (no wages, no admin costs)],Tabla22[Product2],N6,Tabla22[[Economy ]],$O$2))/(COUNTIFS(Tabla22[Product],N6,Tabla22[[Economy ]],$O$2)+COUNTIFS(Tabla22[Product2],N6,Tabla22[[Economy ]],$O$2)),0)</f>
+        <f>IFERROR((SUMIFS(Tabla22[P_T],Tabla22[Product],N6,Tabla22[[Economy ]],$O$2)+SUMIFS(Tabla22[P_T],Tabla22[Product2],N6,Tabla22[[Economy ]],$O$2))/(COUNTIFS(Tabla22[Product],N6,Tabla22[[Economy ]],$O$2)+COUNTIFS(Tabla22[Product2],N6,Tabla22[[Economy ]],$O$2)),0)</f>
         <v>54273.788524999996</v>
       </c>
       <c r="U6" s="43">
         <f>IFERROR((SUMIFS(Tabla22[profit -wages],Tabla22[Product],E6,Tabla22[[Economy ]],$O$2)+SUMIFS(Tabla22[profit -wages],Tabla22[Product2],E6,Tabla22[[Economy ]],$O$2))/(COUNTIFS(Tabla22[Product],E6,Tabla22[[Economy ]],$O$2)+COUNTIFS(Tabla22[Product2],E6,Tabla22[[Economy ]],$O$2)),0)</f>
-        <v>16873.788525000004</v>
+        <v>11273.788525000004</v>
       </c>
       <c r="Y6" s="46"/>
       <c r="Z6" s="46"/>
@@ -1759,7 +1750,7 @@
         <f>F7/COUNTIF(Tabla22[QualityBonus],"&gt;0")</f>
         <v>0.52631578947368418</v>
       </c>
-      <c r="H7" s="81">
+      <c r="H7" s="79">
         <f t="shared" si="0"/>
         <v>0.11235955056179775</v>
       </c>
@@ -1772,12 +1763,12 @@
         <v>120382.25</v>
       </c>
       <c r="K7" s="3">
-        <f>IFERROR((SUMIF(Tabla22[Product],E7,Tabla22[TOTAL PROFIT (no wages, no admin costs)])+SUMIF(Tabla22[Product2],E7,Tabla22[TOTAL PROFIT (no wages, no admin costs)]))/(COUNTIF(Tabla22[Product],E7)+COUNTIF(Tabla22[Product2],E7)),0)</f>
+        <f>IFERROR((SUMIF(Tabla22[Product],E7,Tabla22[P_T])+SUMIF(Tabla22[Product2],E7,Tabla22[P_T]))/(COUNTIF(Tabla22[Product],E7)+COUNTIF(Tabla22[Product2],E7)),0)</f>
         <v>53608.653904999999</v>
       </c>
       <c r="L7" s="43">
         <f>IFERROR((SUMIF(Tabla22[Product],E7,Tabla22[profit -wages])+SUMIF(Tabla22[Product2],E7,Tabla22[profit -wages]))/(COUNTIF(Tabla22[Product],E7)+COUNTIF(Tabla22[Product2],E7)),0)</f>
-        <v>16208.653905000003</v>
+        <v>10608.653905000001</v>
       </c>
       <c r="N7" s="61" t="s">
         <v>53</v>
@@ -1788,7 +1779,7 @@
       </c>
       <c r="P7" s="47">
         <f>IFERROR(O7/COUNTIF(Tabla22[[Economy ]],$O$2),0)</f>
-        <v>0.47058823529411764</v>
+        <v>0.45454545454545453</v>
       </c>
       <c r="Q7" s="37">
         <f t="shared" si="1"/>
@@ -1803,12 +1794,12 @@
         <v>120382.25</v>
       </c>
       <c r="T7" s="3">
-        <f>IFERROR((SUMIFS(Tabla22[TOTAL PROFIT (no wages, no admin costs)],Tabla22[Product],N7,Tabla22[[Economy ]],$O$2)+SUMIFS(Tabla22[TOTAL PROFIT (no wages, no admin costs)],Tabla22[Product2],N7,Tabla22[[Economy ]],$O$2))/(COUNTIFS(Tabla22[Product],N7,Tabla22[[Economy ]],$O$2)+COUNTIFS(Tabla22[Product2],N7,Tabla22[[Economy ]],$O$2)),0)</f>
+        <f>IFERROR((SUMIFS(Tabla22[P_T],Tabla22[Product],N7,Tabla22[[Economy ]],$O$2)+SUMIFS(Tabla22[P_T],Tabla22[Product2],N7,Tabla22[[Economy ]],$O$2))/(COUNTIFS(Tabla22[Product],N7,Tabla22[[Economy ]],$O$2)+COUNTIFS(Tabla22[Product2],N7,Tabla22[[Economy ]],$O$2)),0)</f>
         <v>53608.653904999999</v>
       </c>
       <c r="U7" s="43">
         <f>IFERROR((SUMIFS(Tabla22[profit -wages],Tabla22[Product],E7,Tabla22[[Economy ]],$O$2)+SUMIFS(Tabla22[profit -wages],Tabla22[Product2],E7,Tabla22[[Economy ]],$O$2))/(COUNTIFS(Tabla22[Product],E7,Tabla22[[Economy ]],$O$2)+COUNTIFS(Tabla22[Product2],E7,Tabla22[[Economy ]],$O$2)),0)</f>
-        <v>16208.653905000003</v>
+        <v>10608.653905000001</v>
       </c>
       <c r="Y7" s="46"/>
       <c r="Z7" s="46"/>
@@ -1825,7 +1816,7 @@
         <f>F8/COUNTIF(Tabla22[QualityBonus],"&gt;0")</f>
         <v>0.47368421052631576</v>
       </c>
-      <c r="H8" s="81">
+      <c r="H8" s="79">
         <f t="shared" si="0"/>
         <v>0.10112359550561797</v>
       </c>
@@ -1838,12 +1829,12 @@
         <v>84606.2</v>
       </c>
       <c r="K8" s="3">
-        <f>IFERROR((SUMIF(Tabla22[Product],E8,Tabla22[TOTAL PROFIT (no wages, no admin costs)])+SUMIF(Tabla22[Product2],E8,Tabla22[TOTAL PROFIT (no wages, no admin costs)]))/(COUNTIF(Tabla22[Product],E8)+COUNTIF(Tabla22[Product2],E8)),0)</f>
+        <f>IFERROR((SUMIF(Tabla22[Product],E8,Tabla22[P_T])+SUMIF(Tabla22[Product2],E8,Tabla22[P_T]))/(COUNTIF(Tabla22[Product],E8)+COUNTIF(Tabla22[Product2],E8)),0)</f>
         <v>64241.802946666678</v>
       </c>
       <c r="L8" s="43">
         <f>IFERROR((SUMIF(Tabla22[Product],E8,Tabla22[profit -wages])+SUMIF(Tabla22[Product2],E8,Tabla22[profit -wages]))/(COUNTIF(Tabla22[Product],E8)+COUNTIF(Tabla22[Product2],E8)),0)</f>
-        <v>26841.802946666667</v>
+        <v>21241.802946666667</v>
       </c>
       <c r="N8" s="61" t="s">
         <v>58</v>
@@ -1854,11 +1845,11 @@
       </c>
       <c r="P8" s="47">
         <f>IFERROR(O8/COUNTIF(Tabla22[[Economy ]],$O$2),0)</f>
-        <v>0.42352941176470588</v>
+        <v>0.40909090909090912</v>
       </c>
       <c r="Q8" s="37">
         <f t="shared" si="1"/>
-        <v>0.10112359550561799</v>
+        <v>0.101123595505618</v>
       </c>
       <c r="R8" s="37">
         <f>IFERROR((SUMIFS(Tabla22[QualityBonus],Tabla22[Product],N8,Tabla22[[Economy ]],$O$2)+SUMIFS(Tabla22[QualityBonus],Tabla22[Product2],N8,Tabla22[[Economy ]],$O$2))/(COUNTIFS(Tabla22[Product],N8,Tabla22[[Economy ]],$O$2)+COUNTIFS(Tabla22[Product2],N8,Tabla22[[Economy ]],$O$2)),0)</f>
@@ -1869,19 +1860,19 @@
         <v>84606.2</v>
       </c>
       <c r="T8" s="3">
-        <f>IFERROR((SUMIFS(Tabla22[TOTAL PROFIT (no wages, no admin costs)],Tabla22[Product],N8,Tabla22[[Economy ]],$O$2)+SUMIFS(Tabla22[TOTAL PROFIT (no wages, no admin costs)],Tabla22[Product2],N8,Tabla22[[Economy ]],$O$2))/(COUNTIFS(Tabla22[Product],N8,Tabla22[[Economy ]],$O$2)+COUNTIFS(Tabla22[Product2],N8,Tabla22[[Economy ]],$O$2)),0)</f>
+        <f>IFERROR((SUMIFS(Tabla22[P_T],Tabla22[Product],N8,Tabla22[[Economy ]],$O$2)+SUMIFS(Tabla22[P_T],Tabla22[Product2],N8,Tabla22[[Economy ]],$O$2))/(COUNTIFS(Tabla22[Product],N8,Tabla22[[Economy ]],$O$2)+COUNTIFS(Tabla22[Product2],N8,Tabla22[[Economy ]],$O$2)),0)</f>
         <v>64241.802946666678</v>
       </c>
       <c r="U8" s="43">
         <f>IFERROR((SUMIFS(Tabla22[profit -wages],Tabla22[Product],E8,Tabla22[[Economy ]],$O$2)+SUMIFS(Tabla22[profit -wages],Tabla22[Product2],E8,Tabla22[[Economy ]],$O$2))/(COUNTIFS(Tabla22[Product],E8,Tabla22[[Economy ]],$O$2)+COUNTIFS(Tabla22[Product2],E8,Tabla22[[Economy ]],$O$2)),0)</f>
-        <v>26841.802946666667</v>
+        <v>21241.802946666667</v>
       </c>
       <c r="Y8" s="46"/>
       <c r="Z8" s="46"/>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B9" s="50" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E9" s="61" t="s">
         <v>55</v>
@@ -1894,7 +1885,7 @@
         <f>F9/COUNTIF(Tabla22[QualityBonus],"&gt;0")</f>
         <v>1.381578947368421</v>
       </c>
-      <c r="H9" s="81">
+      <c r="H9" s="79">
         <f t="shared" si="0"/>
         <v>0.2949438202247191</v>
       </c>
@@ -1907,12 +1898,12 @@
         <v>61455.022222222222</v>
       </c>
       <c r="K9" s="3">
-        <f>IFERROR((SUMIF(Tabla22[Product],E9,Tabla22[TOTAL PROFIT (no wages, no admin costs)])+SUMIF(Tabla22[Product2],E9,Tabla22[TOTAL PROFIT (no wages, no admin costs)]))/(COUNTIF(Tabla22[Product],E9)+COUNTIF(Tabla22[Product2],E9)),0)</f>
+        <f>IFERROR((SUMIF(Tabla22[Product],E9,Tabla22[P_T])+SUMIF(Tabla22[Product2],E9,Tabla22[P_T]))/(COUNTIF(Tabla22[Product],E9)+COUNTIF(Tabla22[Product2],E9)),0)</f>
         <v>52889.740973333341</v>
       </c>
       <c r="L9" s="43">
         <f>IFERROR((SUMIF(Tabla22[Product],E9,Tabla22[profit -wages])+SUMIF(Tabla22[Product2],E9,Tabla22[profit -wages]))/(COUNTIF(Tabla22[Product],E9)+COUNTIF(Tabla22[Product2],E9)),0)</f>
-        <v>15489.740973333337</v>
+        <v>9889.7409733333334</v>
       </c>
       <c r="N9" s="61" t="s">
         <v>55</v>
@@ -1923,11 +1914,11 @@
       </c>
       <c r="P9" s="47">
         <f>IFERROR(O9/COUNTIF(Tabla22[[Economy ]],$O$2),0)</f>
-        <v>1.2352941176470589</v>
+        <v>1.1931818181818181</v>
       </c>
       <c r="Q9" s="37">
         <f t="shared" si="1"/>
-        <v>0.29494382022471916</v>
+        <v>0.2949438202247191</v>
       </c>
       <c r="R9" s="37">
         <f>IFERROR((SUMIFS(Tabla22[QualityBonus],Tabla22[Product],N9,Tabla22[[Economy ]],$O$2)+SUMIFS(Tabla22[QualityBonus],Tabla22[Product2],N9,Tabla22[[Economy ]],$O$2))/(COUNTIFS(Tabla22[Product],N9,Tabla22[[Economy ]],$O$2)+COUNTIFS(Tabla22[Product2],N9,Tabla22[[Economy ]],$O$2)),0)</f>
@@ -1938,19 +1929,19 @@
         <v>61455.022222222222</v>
       </c>
       <c r="T9" s="3">
-        <f>IFERROR((SUMIFS(Tabla22[TOTAL PROFIT (no wages, no admin costs)],Tabla22[Product],N9,Tabla22[[Economy ]],$O$2)+SUMIFS(Tabla22[TOTAL PROFIT (no wages, no admin costs)],Tabla22[Product2],N9,Tabla22[[Economy ]],$O$2))/(COUNTIFS(Tabla22[Product],N9,Tabla22[[Economy ]],$O$2)+COUNTIFS(Tabla22[Product2],N9,Tabla22[[Economy ]],$O$2)),0)</f>
+        <f>IFERROR((SUMIFS(Tabla22[P_T],Tabla22[Product],N9,Tabla22[[Economy ]],$O$2)+SUMIFS(Tabla22[P_T],Tabla22[Product2],N9,Tabla22[[Economy ]],$O$2))/(COUNTIFS(Tabla22[Product],N9,Tabla22[[Economy ]],$O$2)+COUNTIFS(Tabla22[Product2],N9,Tabla22[[Economy ]],$O$2)),0)</f>
         <v>52889.740973333341</v>
       </c>
       <c r="U9" s="43">
         <f>IFERROR((SUMIFS(Tabla22[profit -wages],Tabla22[Product],E9,Tabla22[[Economy ]],$O$2)+SUMIFS(Tabla22[profit -wages],Tabla22[Product2],E9,Tabla22[[Economy ]],$O$2))/(COUNTIFS(Tabla22[Product],E9,Tabla22[[Economy ]],$O$2)+COUNTIFS(Tabla22[Product2],E9,Tabla22[[Economy ]],$O$2)),0)</f>
-        <v>15489.740973333337</v>
+        <v>9889.7409733333334</v>
       </c>
       <c r="Y9" s="46"/>
       <c r="Z9" s="46"/>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B10" s="63" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E10" s="62" t="s">
         <v>54</v>
@@ -1963,7 +1954,7 @@
         <f>F10/COUNTIF(Tabla22[QualityBonus],"&gt;0")</f>
         <v>2.1315789473684212</v>
       </c>
-      <c r="H10" s="81">
+      <c r="H10" s="79">
         <f t="shared" si="0"/>
         <v>0.45505617977528096</v>
       </c>
@@ -1976,12 +1967,12 @@
         <v>41497.755555555559</v>
       </c>
       <c r="K10" s="39">
-        <f>IFERROR((SUMIF(Tabla22[Product],E10,Tabla22[TOTAL PROFIT (no wages, no admin costs)])+SUMIF(Tabla22[Product2],E10,Tabla22[TOTAL PROFIT (no wages, no admin costs)]))/(COUNTIF(Tabla22[Product],E10)+COUNTIF(Tabla22[Product2],E10)),0)</f>
+        <f>IFERROR((SUMIF(Tabla22[Product],E10,Tabla22[P_T])+SUMIF(Tabla22[Product2],E10,Tabla22[P_T]))/(COUNTIF(Tabla22[Product],E10)+COUNTIF(Tabla22[Product2],E10)),0)</f>
         <v>68111.238277777782</v>
       </c>
       <c r="L10" s="44">
         <f>IFERROR((SUMIF(Tabla22[Product],E10,Tabla22[profit -wages])+SUMIF(Tabla22[Product2],E10,Tabla22[profit -wages]))/(COUNTIF(Tabla22[Product],E10)+COUNTIF(Tabla22[Product2],E10)),0)</f>
-        <v>30711.238277777771</v>
+        <v>25111.238277777775</v>
       </c>
       <c r="N10" s="62" t="s">
         <v>54</v>
@@ -1992,7 +1983,7 @@
       </c>
       <c r="P10" s="48">
         <f>IFERROR(O10/COUNTIF(Tabla22[[Economy ]],$O$2),0)</f>
-        <v>1.9058823529411764</v>
+        <v>1.8409090909090908</v>
       </c>
       <c r="Q10" s="45">
         <f t="shared" si="1"/>
@@ -2007,12 +1998,12 @@
         <v>41497.755555555559</v>
       </c>
       <c r="T10" s="39">
-        <f>IFERROR((SUMIFS(Tabla22[TOTAL PROFIT (no wages, no admin costs)],Tabla22[Product],N10,Tabla22[[Economy ]],$O$2)+SUMIFS(Tabla22[TOTAL PROFIT (no wages, no admin costs)],Tabla22[Product2],N10,Tabla22[[Economy ]],$O$2))/(COUNTIFS(Tabla22[Product],N10,Tabla22[[Economy ]],$O$2)+COUNTIFS(Tabla22[Product2],N10,Tabla22[[Economy ]],$O$2)),0)</f>
+        <f>IFERROR((SUMIFS(Tabla22[P_T],Tabla22[Product],N10,Tabla22[[Economy ]],$O$2)+SUMIFS(Tabla22[P_T],Tabla22[Product2],N10,Tabla22[[Economy ]],$O$2))/(COUNTIFS(Tabla22[Product],N10,Tabla22[[Economy ]],$O$2)+COUNTIFS(Tabla22[Product2],N10,Tabla22[[Economy ]],$O$2)),0)</f>
         <v>68111.238277777782</v>
       </c>
       <c r="U10" s="44">
         <f>IFERROR((SUMIFS(Tabla22[profit -wages],Tabla22[Product],E10,Tabla22[[Economy ]],$O$2)+SUMIFS(Tabla22[profit -wages],Tabla22[Product2],E10,Tabla22[[Economy ]],$O$2))/(COUNTIFS(Tabla22[Product],E10,Tabla22[[Economy ]],$O$2)+COUNTIFS(Tabla22[Product2],E10,Tabla22[[Economy ]],$O$2)),0)</f>
-        <v>30711.238277777771</v>
+        <v>25111.238277777775</v>
       </c>
       <c r="Y10" s="46"/>
       <c r="Z10" s="46"/>
@@ -2032,7 +2023,7 @@
         <f>SUM(G5:G10)</f>
         <v>4.6842105263157894</v>
       </c>
-      <c r="H11" s="82">
+      <c r="H11" s="80">
         <f>SUM(H5:H10)</f>
         <v>1</v>
       </c>
@@ -2045,12 +2036,12 @@
         <v>74190.536329588023</v>
       </c>
       <c r="K11" s="39">
-        <f>AVERAGEIF(Tabla22[TOTAL PROFIT (no wages, no admin costs)],"&gt;0")</f>
+        <f>AVERAGEIF(Tabla22[P_T],"&gt;0")</f>
         <v>58336.130084210527</v>
       </c>
       <c r="L11" s="58">
         <f>AVERAGE(Tabla22[profit -wages])</f>
-        <v>20936.130084210534</v>
+        <v>15336.130084210532</v>
       </c>
       <c r="M11" s="53"/>
       <c r="N11" s="51" t="s">
@@ -2062,9 +2053,9 @@
       </c>
       <c r="P11" s="48">
         <f>SUM(P5:P10)</f>
-        <v>4.1882352941176464</v>
-      </c>
-      <c r="Q11" s="82">
+        <v>4.045454545454545</v>
+      </c>
+      <c r="Q11" s="80">
         <f>SUM(Q5:Q10)</f>
         <v>1.0000000000000002</v>
       </c>
@@ -2077,19 +2068,19 @@
         <v>74190.536329588023</v>
       </c>
       <c r="T11" s="39">
-        <f>IFERROR(AVERAGEIFS(Tabla22[TOTAL PROFIT (no wages, no admin costs)],Tabla22[[Economy ]],$O$2),0)</f>
-        <v>0</v>
+        <f>IFERROR(AVERAGEIFS(Tabla22[P_T],Tabla22[[Economy ]],$O$2),0)</f>
+        <v>50381.203254545457</v>
       </c>
       <c r="U11" s="58">
         <f>IFERROR(AVERAGEIFS(Tabla22[profit -wages],Tabla22[[Economy ]],$O$2),0)</f>
-        <v>20936.130084210534</v>
+        <v>15336.130084210532</v>
       </c>
       <c r="Y11" s="46"/>
       <c r="Z11" s="46"/>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B12" s="64" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="S12" s="46"/>
       <c r="T12" s="46"/>
@@ -2123,15 +2114,15 @@
       </c>
       <c r="H15" s="68"/>
       <c r="I15" s="69"/>
-      <c r="J15" s="71" t="s">
+      <c r="J15" s="83" t="s">
         <v>50</v>
       </c>
-      <c r="K15" s="72"/>
-      <c r="L15" s="72"/>
-      <c r="M15" s="72"/>
-      <c r="N15" s="72"/>
-      <c r="O15" s="73"/>
-      <c r="P15" s="46"/>
+      <c r="K15" s="84"/>
+      <c r="L15" s="84"/>
+      <c r="M15" s="84"/>
+      <c r="N15" s="84"/>
+      <c r="O15" s="84"/>
+      <c r="P15" s="84"/>
       <c r="R15" s="46"/>
       <c r="S15" s="46"/>
       <c r="T15" s="46"/>
@@ -2159,7 +2150,7 @@
         <v>4</v>
       </c>
       <c r="G16" s="66" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H16" s="13" t="s">
         <v>3</v>
@@ -2168,13 +2159,13 @@
         <v>5</v>
       </c>
       <c r="J16" s="66" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K16" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="L16" s="13" t="s">
         <v>79</v>
-      </c>
-      <c r="L16" s="13" t="s">
-        <v>80</v>
       </c>
       <c r="M16" s="1" t="s">
         <v>51</v>
@@ -2183,7 +2174,7 @@
         <v>52</v>
       </c>
       <c r="O16" s="41" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="P16" t="s">
         <v>20</v>
@@ -2227,7 +2218,7 @@
         <v>313724</v>
       </c>
       <c r="K17" s="3">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
         <v>21729.668400000002</v>
       </c>
       <c r="L17" s="3">
@@ -2235,7 +2226,7 @@
         <v>27538.785</v>
       </c>
       <c r="M17" s="2">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
         <v>5454</v>
       </c>
       <c r="N17" s="3">
@@ -2247,17 +2238,17 @@
         <v>78992.453399999999</v>
       </c>
       <c r="P17" s="3">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
-        <v>41592.453399999999</v>
-      </c>
-      <c r="R17" s="80" t="s">
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v>35992.453399999999</v>
+      </c>
+      <c r="R17" s="78" t="s">
+        <v>76</v>
+      </c>
+      <c r="S17" s="78" t="s">
+        <v>2</v>
+      </c>
+      <c r="T17" s="78" t="s">
         <v>77</v>
-      </c>
-      <c r="S17" s="80" t="s">
-        <v>2</v>
-      </c>
-      <c r="T17" s="80" t="s">
-        <v>78</v>
       </c>
       <c r="U17" s="46"/>
       <c r="V17" s="46"/>
@@ -2295,7 +2286,7 @@
         <v>416796</v>
       </c>
       <c r="K18" s="3">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
         <v>14108.670399999999</v>
       </c>
       <c r="L18" s="3">
@@ -2303,7 +2294,7 @@
         <v>25919.343999999997</v>
       </c>
       <c r="M18" s="2">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
         <v>4764</v>
       </c>
       <c r="N18" s="3">
@@ -2315,16 +2306,16 @@
         <v>72824.0144</v>
       </c>
       <c r="P18" s="3">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
-        <v>35424.0144</v>
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v>29824.0144</v>
       </c>
       <c r="R18" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="S18" s="79">
+      <c r="S18" s="77">
         <v>858000</v>
       </c>
-      <c r="T18" s="79">
+      <c r="T18" s="77">
         <v>6</v>
       </c>
       <c r="U18" s="46"/>
@@ -2363,7 +2354,7 @@
         <v>332955</v>
       </c>
       <c r="K19" s="3">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
         <v>9320.7659999999996</v>
       </c>
       <c r="L19" s="3">
@@ -2371,7 +2362,7 @@
         <v>33797.4</v>
       </c>
       <c r="M19" s="2">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
         <v>3355</v>
       </c>
       <c r="N19" s="3">
@@ -2383,16 +2374,16 @@
         <v>74073.165999999997</v>
       </c>
       <c r="P19" s="3">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
-        <v>36673.165999999997</v>
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v>31073.165999999997</v>
       </c>
       <c r="R19" s="46" t="s">
         <v>57</v>
       </c>
-      <c r="S19" s="79">
+      <c r="S19" s="77">
         <v>238000</v>
       </c>
-      <c r="T19" s="79">
+      <c r="T19" s="77">
         <v>4</v>
       </c>
       <c r="U19" s="46"/>
@@ -2425,7 +2416,7 @@
         <v>179289</v>
       </c>
       <c r="K20" s="3">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
         <v>26176.193999999996</v>
       </c>
       <c r="L20" s="3">
@@ -2433,7 +2424,7 @@
         <v>0</v>
       </c>
       <c r="M20" s="2">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
         <v>14289</v>
       </c>
       <c r="N20" s="3">
@@ -2445,16 +2436,16 @@
         <v>40465.193999999996</v>
       </c>
       <c r="P20" s="3">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
-        <v>3065.1939999999959</v>
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v>-2534.8060000000041</v>
       </c>
       <c r="R20" s="46" t="s">
         <v>58</v>
       </c>
-      <c r="S20" s="79">
+      <c r="S20" s="77">
         <v>82000</v>
       </c>
-      <c r="T20" s="79">
+      <c r="T20" s="77">
         <v>4</v>
       </c>
       <c r="U20" s="46"/>
@@ -2493,7 +2484,7 @@
         <v>244351</v>
       </c>
       <c r="K21" s="3">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
         <v>16229.271000000001</v>
       </c>
       <c r="L21" s="3">
@@ -2501,7 +2492,7 @@
         <v>13720.744000000001</v>
       </c>
       <c r="M21" s="2">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
         <v>2295</v>
       </c>
       <c r="N21" s="3">
@@ -2513,16 +2504,16 @@
         <v>45301.014999999999</v>
       </c>
       <c r="P21" s="3">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
-        <v>7901.0149999999994</v>
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v>2301.0149999999994</v>
       </c>
       <c r="R21" s="46" t="s">
         <v>55</v>
       </c>
-      <c r="S21" s="79">
+      <c r="S21" s="77">
         <v>55000</v>
       </c>
-      <c r="T21" s="79">
+      <c r="T21" s="77">
         <v>5</v>
       </c>
       <c r="U21" s="46"/>
@@ -2561,7 +2552,7 @@
         <v>202985</v>
       </c>
       <c r="K22" s="39">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
         <v>11918.709000000001</v>
       </c>
       <c r="L22" s="39">
@@ -2569,7 +2560,7 @@
         <v>8176.8060000000005</v>
       </c>
       <c r="M22" s="38">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
         <v>1391</v>
       </c>
       <c r="N22" s="39">
@@ -2581,16 +2572,16 @@
         <v>29880.514999999999</v>
       </c>
       <c r="P22" s="39">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
-        <v>-7519.4850000000006</v>
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v>-13119.485000000001</v>
       </c>
       <c r="R22" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="S22" s="79">
+      <c r="S22" s="77">
         <v>37100</v>
       </c>
-      <c r="T22" s="79">
+      <c r="T22" s="77">
         <v>6</v>
       </c>
       <c r="U22" s="46"/>
@@ -2623,7 +2614,7 @@
         <v>178722</v>
       </c>
       <c r="K23" s="3">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
         <v>24752.996999999999</v>
       </c>
       <c r="L23" s="3">
@@ -2631,7 +2622,7 @@
         <v>0</v>
       </c>
       <c r="M23" s="2">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
         <v>13722</v>
       </c>
       <c r="N23" s="3">
@@ -2643,16 +2634,16 @@
         <v>38474.997000000003</v>
       </c>
       <c r="P23" s="3">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
-        <v>1074.997000000003</v>
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v>-4525.002999999997</v>
       </c>
       <c r="R23" s="46" t="s">
         <v>53</v>
       </c>
-      <c r="S23" s="79">
+      <c r="S23" s="77">
         <v>119000</v>
       </c>
-      <c r="T23" s="79">
+      <c r="T23" s="77">
         <v>6</v>
       </c>
       <c r="U23" s="46"/>
@@ -2691,7 +2682,7 @@
         <v>463221</v>
       </c>
       <c r="K24" s="3">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
         <v>24691.350000000002</v>
       </c>
       <c r="L24" s="3">
@@ -2699,7 +2690,7 @@
         <v>24356.312000000002</v>
       </c>
       <c r="M24" s="2">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
         <v>26625</v>
       </c>
       <c r="N24" s="3">
@@ -2711,8 +2702,8 @@
         <v>106768.66200000001</v>
       </c>
       <c r="P24" s="3">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
-        <v>69368.662000000011</v>
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v>63768.662000000011</v>
       </c>
       <c r="R24" s="46"/>
       <c r="S24" s="46"/>
@@ -2747,7 +2738,7 @@
         <v>62463</v>
       </c>
       <c r="K25" s="3">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
         <v>9182.0609999999997</v>
       </c>
       <c r="L25" s="3">
@@ -2755,7 +2746,7 @@
         <v>0</v>
       </c>
       <c r="M25" s="2">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
         <v>7463</v>
       </c>
       <c r="N25" s="3">
@@ -2767,8 +2758,8 @@
         <v>16645.061000000002</v>
       </c>
       <c r="P25" s="3">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
-        <v>-20754.938999999998</v>
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v>-26354.938999999998</v>
       </c>
       <c r="R25" s="46"/>
       <c r="S25" s="46"/>
@@ -2809,7 +2800,7 @@
         <v>306761</v>
       </c>
       <c r="K26" s="3">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
         <v>4262.9625000000005</v>
       </c>
       <c r="L26" s="3">
@@ -2817,7 +2808,7 @@
         <v>19732.085999999999</v>
       </c>
       <c r="M26" s="2">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
         <v>8155</v>
       </c>
       <c r="N26" s="3">
@@ -2829,8 +2820,8 @@
         <v>37756.048500000004</v>
       </c>
       <c r="P26" s="3">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
-        <v>356.04850000000442</v>
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v>-5243.9514999999956</v>
       </c>
       <c r="R26" s="46"/>
       <c r="S26" s="46"/>
@@ -2871,7 +2862,7 @@
         <v>306654</v>
       </c>
       <c r="K27" s="3">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
         <v>28764.254399999998</v>
       </c>
       <c r="L27" s="3">
@@ -2879,7 +2870,7 @@
         <v>6081.88</v>
       </c>
       <c r="M27" s="2">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
         <v>6594</v>
       </c>
       <c r="N27" s="3">
@@ -2891,8 +2882,8 @@
         <v>48500.134399999995</v>
       </c>
       <c r="P27" s="3">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
-        <v>11100.134399999995</v>
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v>5500.1343999999954</v>
       </c>
       <c r="R27" s="46"/>
       <c r="S27" s="46"/>
@@ -2927,7 +2918,7 @@
         <v>84120</v>
       </c>
       <c r="K28" s="3">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
         <v>10144.871999999999</v>
       </c>
       <c r="L28" s="3">
@@ -2935,7 +2926,7 @@
         <v>0</v>
       </c>
       <c r="M28" s="2">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
         <v>9920</v>
       </c>
       <c r="N28" s="3">
@@ -2947,8 +2938,8 @@
         <v>20064.871999999999</v>
       </c>
       <c r="P28" s="3">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
-        <v>-17335.128000000001</v>
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v>-22935.128000000001</v>
       </c>
       <c r="R28" s="46"/>
       <c r="S28" s="46"/>
@@ -2989,7 +2980,7 @@
         <v>512699</v>
       </c>
       <c r="K29" s="39">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
         <v>16260.6</v>
       </c>
       <c r="L29" s="39">
@@ -2997,7 +2988,7 @@
         <v>11205.238499999999</v>
       </c>
       <c r="M29" s="38">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
         <v>2500</v>
       </c>
       <c r="N29" s="39">
@@ -3009,8 +3000,8 @@
         <v>47164.838499999998</v>
       </c>
       <c r="P29" s="39">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
-        <v>9764.838499999998</v>
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v>4164.838499999998</v>
       </c>
       <c r="R29" s="46"/>
       <c r="S29" s="46"/>
@@ -3051,7 +3042,7 @@
         <v>660840</v>
       </c>
       <c r="K30" s="3">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
         <v>70806.528000000006</v>
       </c>
       <c r="L30" s="3">
@@ -3059,7 +3050,7 @@
         <v>16236.288</v>
       </c>
       <c r="M30" s="2">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
         <v>15712</v>
       </c>
       <c r="N30" s="3">
@@ -3071,8 +3062,8 @@
         <v>107882.81600000001</v>
       </c>
       <c r="P30" s="3">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
-        <v>70482.816000000006</v>
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v>64882.816000000006</v>
       </c>
       <c r="R30" s="46"/>
       <c r="S30" s="46"/>
@@ -3113,7 +3104,7 @@
         <v>141919</v>
       </c>
       <c r="K31" s="3">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
         <v>6554.1336000000001</v>
       </c>
       <c r="L31" s="3">
@@ -3121,7 +3112,7 @@
         <v>3975.8354999999997</v>
       </c>
       <c r="M31" s="2">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
         <v>7932</v>
       </c>
       <c r="N31" s="3">
@@ -3133,8 +3124,8 @@
         <v>23248.969100000002</v>
       </c>
       <c r="P31" s="3">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
-        <v>-14151.030899999998</v>
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v>-19751.030899999998</v>
       </c>
       <c r="R31" s="46"/>
       <c r="S31" s="46"/>
@@ -3175,7 +3166,7 @@
         <v>443847</v>
       </c>
       <c r="K32" s="3">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
         <v>23384.703000000001</v>
       </c>
       <c r="L32" s="3">
@@ -3183,7 +3174,7 @@
         <v>27480.163199999999</v>
       </c>
       <c r="M32" s="2">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
         <v>18555</v>
       </c>
       <c r="N32" s="3">
@@ -3195,8 +3186,8 @@
         <v>71211.866200000004</v>
       </c>
       <c r="P32" s="3">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
-        <v>33811.866200000004</v>
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v>28211.866200000004</v>
       </c>
       <c r="R32" s="46"/>
       <c r="S32" s="46"/>
@@ -3237,7 +3228,7 @@
         <v>184408</v>
       </c>
       <c r="K33" s="3">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
         <v>18640.736399999998</v>
       </c>
       <c r="L33" s="3">
@@ -3245,7 +3236,7 @@
         <v>7793.665</v>
       </c>
       <c r="M33" s="2">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
         <v>3798</v>
       </c>
       <c r="N33" s="3">
@@ -3257,8 +3248,8 @@
         <v>36842.401400000002</v>
       </c>
       <c r="P33" s="3">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
-        <v>-557.59859999999753</v>
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v>-6157.5985999999975</v>
       </c>
       <c r="S33" s="46"/>
       <c r="T33" s="46"/>
@@ -3298,7 +3289,7 @@
         <v>526494</v>
       </c>
       <c r="K34" s="3">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
         <v>10242.902400000001</v>
       </c>
       <c r="L34" s="3">
@@ -3306,7 +3297,7 @@
         <v>31388.313600000001</v>
       </c>
       <c r="M34" s="2">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
         <v>9022</v>
       </c>
       <c r="N34" s="3">
@@ -3318,8 +3309,8 @@
         <v>47125.216</v>
       </c>
       <c r="P34" s="3">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
-        <v>9725.2160000000003</v>
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v>4125.2160000000003</v>
       </c>
       <c r="S34" s="46"/>
       <c r="T34" s="46"/>
@@ -3359,7 +3350,7 @@
         <v>286699</v>
       </c>
       <c r="K35" s="3">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
         <v>23339.889600000002</v>
       </c>
       <c r="L35" s="3">
@@ -3367,7 +3358,7 @@
         <v>16740.6306</v>
       </c>
       <c r="M35" s="2">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
         <v>18552</v>
       </c>
       <c r="N35" s="3">
@@ -3379,8 +3370,8 @@
         <v>59379.520199999999</v>
       </c>
       <c r="P35" s="3">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
-        <v>21979.520199999999</v>
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v>16379.520199999999</v>
       </c>
       <c r="S35" s="46"/>
       <c r="T35" s="46"/>
@@ -3420,7 +3411,7 @@
         <v>330905</v>
       </c>
       <c r="K36" s="3">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
         <v>26035.424999999999</v>
       </c>
       <c r="L36" s="3">
@@ -3428,7 +3419,7 @@
         <v>12552.48</v>
       </c>
       <c r="M36" s="2">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
         <v>24125</v>
       </c>
       <c r="N36" s="3">
@@ -3440,8 +3431,8 @@
         <v>73992.904999999999</v>
       </c>
       <c r="P36" s="3">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
-        <v>36592.904999999999</v>
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v>30992.904999999999</v>
       </c>
       <c r="S36" s="46"/>
       <c r="T36" s="46"/>
@@ -3481,7 +3472,7 @@
         <v>272625</v>
       </c>
       <c r="K37" s="39">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
         <v>9006.2279999999992</v>
       </c>
       <c r="L37" s="39">
@@ -3489,7 +3480,7 @@
         <v>25546.59</v>
       </c>
       <c r="M37" s="38">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
         <v>1391</v>
       </c>
       <c r="N37" s="39">
@@ -3501,8 +3492,8 @@
         <v>60177.817999999999</v>
       </c>
       <c r="P37" s="39">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
-        <v>22777.817999999999</v>
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v>17177.817999999999</v>
       </c>
       <c r="S37" s="46"/>
       <c r="T37" s="46"/>
@@ -3542,7 +3533,7 @@
         <v>288860</v>
       </c>
       <c r="K38" s="3">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
         <v>7967.7440000000006</v>
       </c>
       <c r="L38" s="3">
@@ -3550,7 +3541,7 @@
         <v>12623.155200000001</v>
       </c>
       <c r="M38" s="2">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
         <v>14496</v>
       </c>
       <c r="N38" s="3">
@@ -3562,8 +3553,8 @@
         <v>51050.8992</v>
       </c>
       <c r="P38" s="3">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
-        <v>13650.8992</v>
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v>8050.8991999999998</v>
       </c>
       <c r="S38" s="46"/>
       <c r="T38" s="46"/>
@@ -3603,7 +3594,7 @@
         <v>391747</v>
       </c>
       <c r="K39" s="3">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
         <v>25170.516000000003</v>
       </c>
       <c r="L39" s="3">
@@ -3611,7 +3602,7 @@
         <v>32318.201999999997</v>
       </c>
       <c r="M39" s="2">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
         <v>24252</v>
       </c>
       <c r="N39" s="3">
@@ -3623,8 +3614,8 @@
         <v>98735.717999999993</v>
       </c>
       <c r="P39" s="3">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
-        <v>61335.717999999993</v>
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v>55735.717999999993</v>
       </c>
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.25">
@@ -3660,7 +3651,7 @@
         <v>652877</v>
       </c>
       <c r="K40" s="3">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
         <v>42172.254400000005</v>
       </c>
       <c r="L40" s="3">
@@ -3668,7 +3659,7 @@
         <v>28013.823</v>
       </c>
       <c r="M40" s="2">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
         <v>-23508</v>
       </c>
       <c r="N40" s="3">
@@ -3680,8 +3671,8 @@
         <v>61563.077400000009</v>
       </c>
       <c r="P40" s="3">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
-        <v>24163.077400000009</v>
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v>18563.077400000009</v>
       </c>
     </row>
     <row r="41" spans="1:22" x14ac:dyDescent="0.25">
@@ -3717,7 +3708,7 @@
         <v>378633</v>
       </c>
       <c r="K41" s="3">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
         <v>20323.029600000002</v>
       </c>
       <c r="L41" s="3">
@@ -3725,7 +3716,7 @@
         <v>27040.771199999999</v>
       </c>
       <c r="M41" s="2">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
         <v>15087</v>
       </c>
       <c r="N41" s="3">
@@ -3737,8 +3728,8 @@
         <v>68696.800799999997</v>
       </c>
       <c r="P41" s="3">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
-        <v>31296.800799999997</v>
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v>25696.800799999997</v>
       </c>
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.25">
@@ -3774,7 +3765,7 @@
         <v>388230</v>
       </c>
       <c r="K42" s="3">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
         <v>35145.512999999999</v>
       </c>
       <c r="L42" s="3">
@@ -3782,7 +3773,7 @@
         <v>25258.387500000001</v>
       </c>
       <c r="M42" s="2">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
         <v>22955</v>
       </c>
       <c r="N42" s="3">
@@ -3794,8 +3785,8 @@
         <v>98133.900500000003</v>
       </c>
       <c r="P42" s="3">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
-        <v>60733.900500000003</v>
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v>55133.900500000003</v>
       </c>
     </row>
     <row r="43" spans="1:22" x14ac:dyDescent="0.25">
@@ -3825,7 +3816,7 @@
         <v>170320</v>
       </c>
       <c r="K43" s="3">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
         <v>25854.575999999997</v>
       </c>
       <c r="L43" s="3">
@@ -3833,7 +3824,7 @@
         <v>0</v>
       </c>
       <c r="M43" s="2">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
         <v>21920</v>
       </c>
       <c r="N43" s="3">
@@ -3845,8 +3836,8 @@
         <v>47774.576000000001</v>
       </c>
       <c r="P43" s="3">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
-        <v>10374.576000000001</v>
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v>4774.5760000000009</v>
       </c>
     </row>
     <row r="44" spans="1:22" x14ac:dyDescent="0.25">
@@ -3882,7 +3873,7 @@
         <v>457412</v>
       </c>
       <c r="K44" s="3">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
         <v>14604.408000000001</v>
       </c>
       <c r="L44" s="3">
@@ -3890,7 +3881,7 @@
         <v>14588.262000000001</v>
       </c>
       <c r="M44" s="2">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
         <v>22540</v>
       </c>
       <c r="N44" s="3">
@@ -3902,8 +3893,8 @@
         <v>81104.67</v>
       </c>
       <c r="P44" s="3">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
-        <v>43704.67</v>
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v>38104.67</v>
       </c>
     </row>
     <row r="45" spans="1:22" x14ac:dyDescent="0.25">
@@ -3933,7 +3924,7 @@
         <v>212225</v>
       </c>
       <c r="K45" s="3">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
         <v>33107.1</v>
       </c>
       <c r="L45" s="3">
@@ -3941,7 +3932,7 @@
         <v>0</v>
       </c>
       <c r="M45" s="2">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
         <v>26725</v>
       </c>
       <c r="N45" s="3">
@@ -3953,8 +3944,8 @@
         <v>59832.1</v>
       </c>
       <c r="P45" s="3">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
-        <v>22432.1</v>
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v>16832.099999999999</v>
       </c>
     </row>
     <row r="46" spans="1:22" x14ac:dyDescent="0.25">
@@ -3990,7 +3981,7 @@
         <v>447172</v>
       </c>
       <c r="K46" s="3">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
         <v>11154.184799999999</v>
       </c>
       <c r="L46" s="3">
@@ -3998,7 +3989,7 @@
         <v>49482.338399999993</v>
       </c>
       <c r="M46" s="2">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
         <v>8058</v>
       </c>
       <c r="N46" s="3">
@@ -4010,8 +4001,8 @@
         <v>76608.523199999996</v>
       </c>
       <c r="P46" s="3">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
-        <v>39208.523199999996</v>
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v>33608.523199999996</v>
       </c>
     </row>
     <row r="47" spans="1:22" x14ac:dyDescent="0.25">
@@ -4047,7 +4038,7 @@
         <v>184008</v>
       </c>
       <c r="K47" s="3">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
         <v>9020.3040000000019</v>
       </c>
       <c r="L47" s="3">
@@ -4055,7 +4046,7 @@
         <v>21855.456000000002</v>
       </c>
       <c r="M47" s="2">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
         <v>5948</v>
       </c>
       <c r="N47" s="3">
@@ -4067,8 +4058,8 @@
         <v>48583.76</v>
       </c>
       <c r="P47" s="3">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
-        <v>11183.760000000002</v>
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v>5583.760000000002</v>
       </c>
     </row>
     <row r="48" spans="1:22" x14ac:dyDescent="0.25">
@@ -4104,7 +4095,7 @@
         <v>477379</v>
       </c>
       <c r="K48" s="3">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
         <v>37301.615999999995</v>
       </c>
       <c r="L48" s="3">
@@ -4112,7 +4103,7 @@
         <v>10924.672</v>
       </c>
       <c r="M48" s="2">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
         <v>-3765</v>
       </c>
       <c r="N48" s="3">
@@ -4124,8 +4115,8 @@
         <v>58605.287999999993</v>
       </c>
       <c r="P48" s="3">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
-        <v>21205.287999999993</v>
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v>15605.287999999993</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
@@ -4155,7 +4146,7 @@
         <v>62999</v>
       </c>
       <c r="K49" s="3">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
         <v>5354.915</v>
       </c>
       <c r="L49" s="3">
@@ -4163,7 +4154,7 @@
         <v>0</v>
       </c>
       <c r="M49" s="2">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
         <v>7999</v>
       </c>
       <c r="N49" s="3">
@@ -4175,8 +4166,8 @@
         <v>13353.915000000001</v>
       </c>
       <c r="P49" s="3">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
-        <v>-24046.084999999999</v>
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v>-29646.084999999999</v>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
@@ -4206,7 +4197,7 @@
         <v>117232</v>
       </c>
       <c r="K50" s="39">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
         <v>19835.654399999999</v>
       </c>
       <c r="L50" s="39">
@@ -4214,7 +4205,7 @@
         <v>0</v>
       </c>
       <c r="M50" s="38">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
         <v>-1768</v>
       </c>
       <c r="N50" s="39">
@@ -4226,8 +4217,8 @@
         <v>18067.654399999999</v>
       </c>
       <c r="P50" s="39">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
-        <v>-19332.345600000001</v>
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v>-24932.345600000001</v>
       </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
@@ -4263,7 +4254,7 @@
         <v>544654</v>
       </c>
       <c r="K51" s="3">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
         <v>35173.343999999997</v>
       </c>
       <c r="L51" s="3">
@@ -4271,7 +4262,7 @@
         <v>33839.97</v>
       </c>
       <c r="M51" s="2">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
         <v>3824</v>
       </c>
       <c r="N51" s="3">
@@ -4283,8 +4274,8 @@
         <v>100167.314</v>
       </c>
       <c r="P51" s="3">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
-        <v>62767.313999999998</v>
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v>57167.313999999998</v>
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.25">
@@ -4314,7 +4305,7 @@
         <v>169316</v>
       </c>
       <c r="K52" s="3">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
         <v>26413.295999999998</v>
       </c>
       <c r="L52" s="3">
@@ -4322,7 +4313,7 @@
         <v>0</v>
       </c>
       <c r="M52" s="2">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
         <v>20916</v>
       </c>
       <c r="N52" s="3">
@@ -4334,8 +4325,8 @@
         <v>47329.296000000002</v>
       </c>
       <c r="P52" s="3">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
-        <v>9929.2960000000021</v>
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v>4329.2960000000021</v>
       </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.25">
@@ -4371,7 +4362,7 @@
         <v>438265</v>
       </c>
       <c r="K53" s="3">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
         <v>12045.704399999999</v>
       </c>
       <c r="L53" s="3">
@@ -4379,7 +4370,7 @@
         <v>51853.332599999994</v>
       </c>
       <c r="M53" s="2">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
         <v>8418</v>
       </c>
       <c r="N53" s="3">
@@ -4391,8 +4382,8 @@
         <v>70964.036999999997</v>
       </c>
       <c r="P53" s="3">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
-        <v>33564.036999999997</v>
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v>27964.036999999997</v>
       </c>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
@@ -4428,7 +4419,7 @@
         <v>211434</v>
       </c>
       <c r="K54" s="3">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
         <v>12610.079999999998</v>
       </c>
       <c r="L54" s="3">
@@ -4436,7 +4427,7 @@
         <v>5801.6448</v>
       </c>
       <c r="M54" s="2">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
         <v>13800</v>
       </c>
       <c r="N54" s="3">
@@ -4448,8 +4439,8 @@
         <v>36545.724799999996</v>
       </c>
       <c r="P54" s="3">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
-        <v>-854.27520000000368</v>
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v>-6454.2752000000037</v>
       </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
@@ -4479,7 +4470,7 @@
         <v>82536</v>
       </c>
       <c r="K55" s="3">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
         <v>11538.532800000001</v>
       </c>
       <c r="L55" s="3">
@@ -4487,7 +4478,7 @@
         <v>0</v>
       </c>
       <c r="M55" s="2">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
         <v>8336</v>
       </c>
       <c r="N55" s="3">
@@ -4499,8 +4490,8 @@
         <v>19874.532800000001</v>
       </c>
       <c r="P55" s="3">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
-        <v>-17525.467199999999</v>
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v>-23125.467199999999</v>
       </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.25">
@@ -4536,7 +4527,7 @@
         <v>552269</v>
       </c>
       <c r="K56" s="3">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
         <v>29834.9568</v>
       </c>
       <c r="L56" s="3">
@@ -4544,7 +4535,7 @@
         <v>27484.35</v>
       </c>
       <c r="M56" s="2">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
         <v>14144</v>
       </c>
       <c r="N56" s="3">
@@ -4556,8 +4547,8 @@
         <v>96088.306799999991</v>
       </c>
       <c r="P56" s="3">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
-        <v>58688.306799999991</v>
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v>53088.306799999991</v>
       </c>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.25">
@@ -4593,7 +4584,7 @@
         <v>206348</v>
       </c>
       <c r="K57" s="3">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
         <v>12098.394</v>
       </c>
       <c r="L57" s="3">
@@ -4601,7 +4592,7 @@
         <v>9996.0696000000007</v>
       </c>
       <c r="M57" s="2">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
         <v>12206</v>
       </c>
       <c r="N57" s="3">
@@ -4613,8 +4604,8 @@
         <v>44242.463600000003</v>
       </c>
       <c r="P57" s="3">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
-        <v>6842.4636000000028</v>
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v>1242.4636000000028</v>
       </c>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
@@ -4644,7 +4635,7 @@
         <v>79988</v>
       </c>
       <c r="K58" s="39">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
         <v>4895.2656000000006</v>
       </c>
       <c r="L58" s="39">
@@ -4652,7 +4643,7 @@
         <v>0</v>
       </c>
       <c r="M58" s="38">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
         <v>5788</v>
       </c>
       <c r="N58" s="39">
@@ -4664,8 +4655,8 @@
         <v>10683.265600000001</v>
       </c>
       <c r="P58" s="39">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
-        <v>-26716.734400000001</v>
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v>-32316.734400000001</v>
       </c>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.25">
@@ -4701,7 +4692,7 @@
         <v>519698</v>
       </c>
       <c r="K59" s="3">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
         <v>22482.806400000001</v>
       </c>
       <c r="L59" s="3">
@@ -4709,7 +4700,7 @@
         <v>48611.880000000005</v>
       </c>
       <c r="M59" s="2">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
         <v>15948</v>
       </c>
       <c r="N59" s="3">
@@ -4721,8 +4712,8 @@
         <v>85392.686400000006</v>
       </c>
       <c r="P59" s="3">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
-        <v>47992.686400000006</v>
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v>42392.686400000006</v>
       </c>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.25">
@@ -4752,7 +4743,7 @@
         <v>201450</v>
       </c>
       <c r="K60" s="3">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
         <v>21031.379999999997</v>
       </c>
       <c r="L60" s="3">
@@ -4760,7 +4751,7 @@
         <v>0</v>
       </c>
       <c r="M60" s="2">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
         <v>15950</v>
       </c>
       <c r="N60" s="3">
@@ -4772,8 +4763,8 @@
         <v>36981.379999999997</v>
       </c>
       <c r="P60" s="3">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
-        <v>-418.62000000000262</v>
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v>-6018.6200000000026</v>
       </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">
@@ -4803,7 +4794,7 @@
         <v>183468</v>
       </c>
       <c r="K61" s="3">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
         <v>26602.86</v>
       </c>
       <c r="L61" s="3">
@@ -4811,7 +4802,7 @@
         <v>0</v>
       </c>
       <c r="M61" s="2">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
         <v>18468</v>
       </c>
       <c r="N61" s="3">
@@ -4823,8 +4814,8 @@
         <v>45070.86</v>
       </c>
       <c r="P61" s="3">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
-        <v>7670.8600000000006</v>
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v>2070.8600000000006</v>
       </c>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.25">
@@ -4860,7 +4851,7 @@
         <v>463631</v>
       </c>
       <c r="K62" s="3">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
         <v>11247.6114</v>
       </c>
       <c r="L62" s="3">
@@ -4868,7 +4859,7 @@
         <v>20875.809600000001</v>
       </c>
       <c r="M62" s="2">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
         <v>11223</v>
       </c>
       <c r="N62" s="3">
@@ -4880,8 +4871,8 @@
         <v>56454.421000000002</v>
       </c>
       <c r="P62" s="3">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
-        <v>19054.421000000002</v>
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v>13454.421000000002</v>
       </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">
@@ -4911,7 +4902,7 @@
         <v>124584</v>
       </c>
       <c r="K63" s="3">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
         <v>13019.028</v>
       </c>
       <c r="L63" s="3">
@@ -4919,7 +4910,7 @@
         <v>0</v>
       </c>
       <c r="M63" s="2">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
         <v>14584</v>
       </c>
       <c r="N63" s="3">
@@ -4931,8 +4922,8 @@
         <v>27603.027999999998</v>
       </c>
       <c r="P63" s="3">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
-        <v>-9796.9720000000016</v>
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v>-15396.972000000002</v>
       </c>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.25">
@@ -4942,13 +4933,13 @@
       <c r="B64" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C64" s="77">
+      <c r="C64" s="74">
         <v>2.5999999999999999E-2</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E64" s="78">
+      <c r="E64" s="75">
         <v>62770</v>
       </c>
       <c r="F64" s="5">
@@ -4968,7 +4959,7 @@
         <v>335796</v>
       </c>
       <c r="K64" s="3">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
         <v>32640.400000000001</v>
       </c>
       <c r="L64" s="3">
@@ -4976,7 +4967,7 @@
         <v>8810.4639999999999</v>
       </c>
       <c r="M64" s="2">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
         <v>31080</v>
       </c>
       <c r="N64" s="3">
@@ -4987,9 +4978,9 @@
         <f>SUM(Tabla22[[#This Row],[Bonus1]:[p2]])</f>
         <v>75246.864000000001</v>
       </c>
-      <c r="P64" s="78">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
-        <v>37846.864000000001</v>
+      <c r="P64" s="75">
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v>32246.864000000001</v>
       </c>
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.25">
@@ -4999,13 +4990,13 @@
       <c r="B65" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C65" s="77">
+      <c r="C65" s="74">
         <v>1.7100000000000001E-2</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E65" s="78">
+      <c r="E65" s="75">
         <v>42582</v>
       </c>
       <c r="F65" s="5">
@@ -5025,7 +5016,7 @@
         <v>337884</v>
       </c>
       <c r="K65" s="3">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
         <v>21844.565999999999</v>
       </c>
       <c r="L65" s="3">
@@ -5033,7 +5024,7 @@
         <v>10685.277</v>
       </c>
       <c r="M65" s="2">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
         <v>27410</v>
       </c>
       <c r="N65" s="3">
@@ -5044,9 +5035,9 @@
         <f>SUM(Tabla22[[#This Row],[Bonus1]:[p2]])</f>
         <v>74913.842999999993</v>
       </c>
-      <c r="P65" s="78">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
-        <v>37513.842999999993</v>
+      <c r="P65" s="75">
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v>31913.842999999993</v>
       </c>
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.25">
@@ -5056,13 +5047,13 @@
       <c r="B66" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C66" s="77">
+      <c r="C66" s="74">
         <v>1.0200000000000001E-2</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E66" s="78">
+      <c r="E66" s="75">
         <v>59416</v>
       </c>
       <c r="F66" s="5">
@@ -5076,7 +5067,7 @@
         <v>118832</v>
       </c>
       <c r="K66" s="3">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
         <v>6060.4320000000007</v>
       </c>
       <c r="L66" s="3">
@@ -5084,7 +5075,7 @@
         <v>0</v>
       </c>
       <c r="M66" s="2">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
         <v>8832</v>
       </c>
       <c r="N66" s="3">
@@ -5095,9 +5086,9 @@
         <f>SUM(Tabla22[[#This Row],[Bonus1]:[p2]])</f>
         <v>14892.432000000001</v>
       </c>
-      <c r="P66" s="78">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
-        <v>-22507.567999999999</v>
+      <c r="P66" s="75">
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v>-28107.567999999999</v>
       </c>
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.25">
@@ -5107,13 +5098,13 @@
       <c r="B67" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C67" s="77">
+      <c r="C67" s="74">
         <v>2.7099999999999999E-2</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E67" s="78">
+      <c r="E67" s="75">
         <v>42602</v>
       </c>
       <c r="F67" s="5">
@@ -5127,7 +5118,7 @@
         <v>213010</v>
       </c>
       <c r="K67" s="3">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
         <v>34635.425999999999</v>
       </c>
       <c r="L67" s="3">
@@ -5135,7 +5126,7 @@
         <v>0</v>
       </c>
       <c r="M67" s="2">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
         <v>27510</v>
       </c>
       <c r="N67" s="3">
@@ -5146,9 +5137,9 @@
         <f>SUM(Tabla22[[#This Row],[Bonus1]:[p2]])</f>
         <v>62145.425999999999</v>
       </c>
-      <c r="P67" s="78">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
-        <v>24745.425999999999</v>
+      <c r="P67" s="75">
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v>19145.425999999999</v>
       </c>
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.25">
@@ -5158,13 +5149,13 @@
       <c r="B68" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C68" s="77">
+      <c r="C68" s="74">
         <v>2.9399999999999999E-2</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E68" s="78">
+      <c r="E68" s="75">
         <v>825825</v>
       </c>
       <c r="F68" s="5">
@@ -5184,7 +5175,7 @@
         <v>2677980</v>
       </c>
       <c r="K68" s="3">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
         <v>437026.58999999997</v>
       </c>
       <c r="L68" s="3">
@@ -5192,7 +5183,7 @@
         <v>35369.082000000002</v>
       </c>
       <c r="M68" s="2">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
         <v>-96525</v>
       </c>
       <c r="N68" s="3">
@@ -5203,9 +5194,9 @@
         <f>SUM(Tabla22[[#This Row],[Bonus1]:[p2]])</f>
         <v>390875.67199999996</v>
       </c>
-      <c r="P68" s="78">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
-        <v>353475.67199999996</v>
+      <c r="P68" s="75">
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v>347875.67199999996</v>
       </c>
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.25">
@@ -5215,13 +5206,13 @@
       <c r="B69" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C69" s="77">
+      <c r="C69" s="74">
         <v>2.9600000000000001E-2</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E69" s="78">
+      <c r="E69" s="75">
         <v>61467</v>
       </c>
       <c r="F69" s="5">
@@ -5235,7 +5226,7 @@
         <v>61467</v>
       </c>
       <c r="K69" s="3">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
         <v>9097.1160000000018</v>
       </c>
       <c r="L69" s="3">
@@ -5243,7 +5234,7 @@
         <v>0</v>
       </c>
       <c r="M69" s="2">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
         <v>6467</v>
       </c>
       <c r="N69" s="3">
@@ -5254,9 +5245,9 @@
         <f>SUM(Tabla22[[#This Row],[Bonus1]:[p2]])</f>
         <v>15564.116000000002</v>
       </c>
-      <c r="P69" s="78">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
-        <v>-21835.883999999998</v>
+      <c r="P69" s="75">
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v>-27435.883999999998</v>
       </c>
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.25">
@@ -5266,13 +5257,13 @@
       <c r="B70" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C70" s="77">
+      <c r="C70" s="74">
         <v>1.9099999999999999E-2</v>
       </c>
       <c r="D70" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E70" s="78">
+      <c r="E70" s="75">
         <v>119307</v>
       </c>
       <c r="F70" s="5">
@@ -5292,7 +5283,7 @@
         <v>247017</v>
       </c>
       <c r="K70" s="3">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
         <v>13672.582199999999</v>
       </c>
       <c r="L70" s="3">
@@ -5300,7 +5291,7 @@
         <v>14635.565999999999</v>
       </c>
       <c r="M70" s="2">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
         <v>307</v>
       </c>
       <c r="N70" s="3">
@@ -5311,9 +5302,9 @@
         <f>SUM(Tabla22[[#This Row],[Bonus1]:[p2]])</f>
         <v>45025.148199999996</v>
       </c>
-      <c r="P70" s="78">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
-        <v>7625.148199999996</v>
+      <c r="P70" s="75">
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v>2025.148199999996</v>
       </c>
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.25">
@@ -5323,7 +5314,7 @@
       <c r="B71" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C71" s="77">
+      <c r="C71" s="74">
         <v>1.61E-2</v>
       </c>
       <c r="D71" s="2" t="s">
@@ -5343,7 +5334,7 @@
         <v>61283</v>
       </c>
       <c r="K71" s="3">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
         <v>4933.2815000000001</v>
       </c>
       <c r="L71" s="3">
@@ -5351,7 +5342,7 @@
         <v>0</v>
       </c>
       <c r="M71" s="2">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
         <v>6283</v>
       </c>
       <c r="N71" s="3">
@@ -5363,8 +5354,8 @@
         <v>11216.281500000001</v>
       </c>
       <c r="P71" s="3">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
-        <v>-26183.718499999999</v>
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v>-31783.718499999999</v>
       </c>
     </row>
     <row r="72" spans="1:16" x14ac:dyDescent="0.25">
@@ -5400,7 +5391,7 @@
         <v>143504</v>
       </c>
       <c r="K72" s="39">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
         <v>7380.7379999999994</v>
       </c>
       <c r="L72" s="39">
@@ -5408,7 +5399,7 @@
         <v>6487.7654999999995</v>
       </c>
       <c r="M72" s="38">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
         <v>2255</v>
       </c>
       <c r="N72" s="39">
@@ -5420,8 +5411,8 @@
         <v>20372.503499999999</v>
       </c>
       <c r="P72" s="39">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
-        <v>-17027.496500000001</v>
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v>-22627.496500000001</v>
       </c>
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.25">
@@ -5431,13 +5422,13 @@
       <c r="B73" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C73" s="77">
+      <c r="C73" s="74">
         <v>1.5800000000000002E-2</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E73" s="78">
+      <c r="E73" s="75">
         <v>62381</v>
       </c>
       <c r="F73" s="5">
@@ -5457,7 +5448,7 @@
         <v>250348</v>
       </c>
       <c r="K73" s="3">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
         <v>9856.1980000000021</v>
       </c>
       <c r="L73" s="3">
@@ -5465,7 +5456,7 @@
         <v>11905.552800000001</v>
       </c>
       <c r="M73" s="2">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
         <v>14762</v>
       </c>
       <c r="N73" s="3">
@@ -5476,9 +5467,9 @@
         <f>SUM(Tabla22[[#This Row],[Bonus1]:[p2]])</f>
         <v>50809.750800000002</v>
       </c>
-      <c r="P73" s="78">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
-        <v>13409.750800000002</v>
+      <c r="P73" s="75">
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v>7809.7508000000016</v>
       </c>
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.25">
@@ -5488,13 +5479,13 @@
       <c r="B74" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C74" s="77">
+      <c r="C74" s="74">
         <v>1.21E-2</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E74" s="78">
+      <c r="E74" s="75">
         <v>40404</v>
       </c>
       <c r="F74" s="5">
@@ -5514,7 +5505,7 @@
         <v>323568</v>
       </c>
       <c r="K74" s="3">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
         <v>5866.6607999999997</v>
       </c>
       <c r="L74" s="3">
@@ -5522,7 +5513,7 @@
         <v>17624.376</v>
       </c>
       <c r="M74" s="2">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
         <v>6608</v>
       </c>
       <c r="N74" s="3">
@@ -5533,9 +5524,9 @@
         <f>SUM(Tabla22[[#This Row],[Bonus1]:[p2]])</f>
         <v>34859.036800000002</v>
       </c>
-      <c r="P74" s="78">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
-        <v>-2540.9631999999983</v>
+      <c r="P74" s="75">
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v>-8140.9631999999983</v>
       </c>
     </row>
     <row r="75" spans="1:16" x14ac:dyDescent="0.25">
@@ -5545,13 +5536,13 @@
       <c r="B75" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C75" s="77">
+      <c r="C75" s="74">
         <v>1.1599999999999999E-2</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E75" s="78">
+      <c r="E75" s="75">
         <v>62536</v>
       </c>
       <c r="F75" s="5">
@@ -5571,7 +5562,7 @@
         <v>333968</v>
       </c>
       <c r="K75" s="3">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
         <v>14508.351999999999</v>
       </c>
       <c r="L75" s="3">
@@ -5579,7 +5570,7 @@
         <v>5834.1503999999995</v>
       </c>
       <c r="M75" s="2">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
         <v>30144</v>
       </c>
       <c r="N75" s="3">
@@ -5590,9 +5581,9 @@
         <f>SUM(Tabla22[[#This Row],[Bonus1]:[p2]])</f>
         <v>60110.502399999998</v>
       </c>
-      <c r="P75" s="78">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
-        <v>22710.502399999998</v>
+      <c r="P75" s="75">
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v>17110.502399999998</v>
       </c>
     </row>
     <row r="76" spans="1:16" x14ac:dyDescent="0.25">
@@ -5602,13 +5593,13 @@
       <c r="B76" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C76" s="77">
+      <c r="C76" s="74">
         <v>2.0299999999999999E-2</v>
       </c>
       <c r="D76" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E76" s="78">
+      <c r="E76" s="75">
         <v>40580</v>
       </c>
       <c r="F76" s="5">
@@ -5628,7 +5619,7 @@
         <v>221705</v>
       </c>
       <c r="K76" s="3">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
         <v>19770.575999999997</v>
       </c>
       <c r="L76" s="3">
@@ -5636,7 +5627,7 @@
         <v>6027.5774999999994</v>
       </c>
       <c r="M76" s="2">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
         <v>13920</v>
       </c>
       <c r="N76" s="3">
@@ -5647,9 +5638,9 @@
         <f>SUM(Tabla22[[#This Row],[Bonus1]:[p2]])</f>
         <v>44103.1535</v>
       </c>
-      <c r="P76" s="78">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
-        <v>6703.1535000000003</v>
+      <c r="P76" s="75">
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v>1103.1535000000003</v>
       </c>
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.25">
@@ -5659,13 +5650,13 @@
       <c r="B77" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C77" s="77">
+      <c r="C77" s="74">
         <v>2.2200000000000001E-2</v>
       </c>
       <c r="D77" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E77" s="78">
+      <c r="E77" s="75">
         <v>222195</v>
       </c>
       <c r="F77" s="5">
@@ -5674,7 +5665,7 @@
       <c r="G77" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="H77" s="78">
+      <c r="H77" s="75">
         <v>117614</v>
       </c>
       <c r="I77" s="5">
@@ -5685,7 +5676,7 @@
         <v>575037</v>
       </c>
       <c r="K77" s="3">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
         <v>19730.916000000001</v>
       </c>
       <c r="L77" s="3">
@@ -5693,7 +5684,7 @@
         <v>46998.554400000001</v>
       </c>
       <c r="M77" s="2">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
         <v>-15805</v>
       </c>
       <c r="N77" s="3">
@@ -5704,9 +5695,9 @@
         <f>SUM(Tabla22[[#This Row],[Bonus1]:[p2]])</f>
         <v>46766.470400000006</v>
       </c>
-      <c r="P77" s="78">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
-        <v>9366.4704000000056</v>
+      <c r="P77" s="75">
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v>3766.4704000000056</v>
       </c>
     </row>
     <row r="78" spans="1:16" x14ac:dyDescent="0.25">
@@ -5716,13 +5707,13 @@
       <c r="B78" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C78" s="77">
+      <c r="C78" s="74">
         <v>2.1299999999999999E-2</v>
       </c>
       <c r="D78" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E78" s="78">
+      <c r="E78" s="75">
         <v>120518</v>
       </c>
       <c r="F78" s="5">
@@ -5731,7 +5722,7 @@
       <c r="G78" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="H78" s="78">
+      <c r="H78" s="75">
         <v>40446</v>
       </c>
       <c r="I78" s="5">
@@ -5742,7 +5733,7 @@
         <v>241856</v>
       </c>
       <c r="K78" s="3">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
         <v>15402.2004</v>
       </c>
       <c r="L78" s="3">
@@ -5750,7 +5741,7 @@
         <v>15506.9964</v>
       </c>
       <c r="M78" s="2">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
         <v>1518</v>
       </c>
       <c r="N78" s="3">
@@ -5761,9 +5752,9 @@
         <f>SUM(Tabla22[[#This Row],[Bonus1]:[p2]])</f>
         <v>42465.196799999998</v>
       </c>
-      <c r="P78" s="78">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
-        <v>5065.1967999999979</v>
+      <c r="P78" s="75">
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v>-534.80320000000211</v>
       </c>
     </row>
     <row r="79" spans="1:16" x14ac:dyDescent="0.25">
@@ -5773,13 +5764,13 @@
       <c r="B79" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C79" s="77">
+      <c r="C79" s="74">
         <v>2.75E-2</v>
       </c>
       <c r="D79" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E79" s="78">
+      <c r="E79" s="75">
         <v>40932</v>
       </c>
       <c r="F79" s="5">
@@ -5788,7 +5779,7 @@
       <c r="G79" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="H79" s="78">
+      <c r="H79" s="75">
         <v>59663</v>
       </c>
       <c r="I79" s="5">
@@ -5799,7 +5790,7 @@
         <v>320516</v>
       </c>
       <c r="K79" s="3">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
         <v>13507.560000000001</v>
       </c>
       <c r="L79" s="3">
@@ -5807,7 +5798,7 @@
         <v>32814.65</v>
       </c>
       <c r="M79" s="2">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
         <v>7664</v>
       </c>
       <c r="N79" s="3">
@@ -5818,9 +5809,9 @@
         <f>SUM(Tabla22[[#This Row],[Bonus1]:[p2]])</f>
         <v>72638.210000000006</v>
       </c>
-      <c r="P79" s="78">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
-        <v>35238.210000000006</v>
+      <c r="P79" s="75">
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v>29638.210000000006</v>
       </c>
     </row>
     <row r="80" spans="1:16" x14ac:dyDescent="0.25">
@@ -5830,13 +5821,13 @@
       <c r="B80" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C80" s="77">
+      <c r="C80" s="74">
         <v>2.0400000000000001E-2</v>
       </c>
       <c r="D80" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E80" s="78">
+      <c r="E80" s="75">
         <v>40605</v>
       </c>
       <c r="F80" s="5">
@@ -5845,7 +5836,7 @@
       <c r="G80" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="H80" s="78">
+      <c r="H80" s="75">
         <v>62919</v>
       </c>
       <c r="I80" s="5">
@@ -5856,7 +5847,7 @@
         <v>184734</v>
       </c>
       <c r="K80" s="3">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
         <v>14910.156000000003</v>
       </c>
       <c r="L80" s="3">
@@ -5864,7 +5855,7 @@
         <v>6417.7380000000003</v>
       </c>
       <c r="M80" s="2">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
         <v>10515</v>
       </c>
       <c r="N80" s="3">
@@ -5875,9 +5866,9 @@
         <f>SUM(Tabla22[[#This Row],[Bonus1]:[p2]])</f>
         <v>39761.894</v>
       </c>
-      <c r="P80" s="78">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
-        <v>2361.8940000000002</v>
+      <c r="P80" s="75">
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v>-3238.1059999999998</v>
       </c>
     </row>
     <row r="81" spans="1:16" x14ac:dyDescent="0.25">
@@ -5887,13 +5878,13 @@
       <c r="B81" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C81" s="77">
+      <c r="C81" s="74">
         <v>1.9699999999999999E-2</v>
       </c>
       <c r="D81" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E81" s="78">
+      <c r="E81" s="75">
         <v>41913</v>
       </c>
       <c r="F81" s="5">
@@ -5902,7 +5893,7 @@
       <c r="G81" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="H81" s="78">
+      <c r="H81" s="75">
         <v>59770</v>
       </c>
       <c r="I81" s="5">
@@ -5913,7 +5904,7 @@
         <v>143596</v>
       </c>
       <c r="K81" s="3">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
         <v>9908.2332000000006</v>
       </c>
       <c r="L81" s="3">
@@ -5921,7 +5912,7 @@
         <v>5887.3449999999993</v>
       </c>
       <c r="M81" s="2">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
         <v>9626</v>
       </c>
       <c r="N81" s="3">
@@ -5932,9 +5923,9 @@
         <f>SUM(Tabla22[[#This Row],[Bonus1]:[p2]])</f>
         <v>30191.5782</v>
       </c>
-      <c r="P81" s="78">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
-        <v>-7208.4218000000001</v>
+      <c r="P81" s="75">
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v>-12808.4218</v>
       </c>
     </row>
     <row r="82" spans="1:16" x14ac:dyDescent="0.25">
@@ -5944,13 +5935,13 @@
       <c r="B82" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C82" s="77">
+      <c r="C82" s="74">
         <v>2.5700000000000001E-2</v>
       </c>
       <c r="D82" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E82" s="78">
+      <c r="E82" s="75">
         <v>59654</v>
       </c>
       <c r="F82" s="5">
@@ -5959,7 +5950,7 @@
       <c r="G82" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="H82" s="78">
+      <c r="H82" s="75">
         <v>42145</v>
       </c>
       <c r="I82" s="5">
@@ -5969,8 +5960,8 @@
         <f>Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]+Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]</f>
         <v>365051</v>
       </c>
-      <c r="K82" s="78">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
+      <c r="K82" s="75">
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
         <v>30662.155999999999</v>
       </c>
       <c r="L82" s="3">
@@ -5978,7 +5969,7 @@
         <v>19496.277000000002</v>
       </c>
       <c r="M82" s="2">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
         <v>18616</v>
       </c>
       <c r="N82" s="3">
@@ -5989,9 +5980,9 @@
         <f>SUM(Tabla22[[#This Row],[Bonus1]:[p2]])</f>
         <v>83909.433000000005</v>
       </c>
-      <c r="P82" s="78">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
-        <v>46509.433000000005</v>
+      <c r="P82" s="75">
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v>40909.433000000005</v>
       </c>
     </row>
     <row r="83" spans="1:16" x14ac:dyDescent="0.25">
@@ -6001,13 +5992,13 @@
       <c r="B83" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C83" s="77">
+      <c r="C83" s="74">
         <v>2.3199999999999998E-2</v>
       </c>
       <c r="D83" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E83" s="78">
+      <c r="E83" s="75">
         <v>42232</v>
       </c>
       <c r="F83" s="5">
@@ -6016,7 +6007,7 @@
       <c r="G83" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="H83" s="78">
+      <c r="H83" s="75">
         <v>61628</v>
       </c>
       <c r="I83" s="5">
@@ -6026,8 +6017,8 @@
         <f>Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]+Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]</f>
         <v>373208</v>
       </c>
-      <c r="K83" s="78">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
+      <c r="K83" s="75">
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
         <v>17636.083199999997</v>
       </c>
       <c r="L83" s="3">
@@ -6035,7 +6026,7 @@
         <v>28595.392</v>
       </c>
       <c r="M83" s="2">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
         <v>15396</v>
       </c>
       <c r="N83" s="3">
@@ -6046,9 +6037,9 @@
         <f>SUM(Tabla22[[#This Row],[Bonus1]:[p2]])</f>
         <v>88139.475200000001</v>
       </c>
-      <c r="P83" s="78">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
-        <v>50739.475200000001</v>
+      <c r="P83" s="75">
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v>45139.475200000001</v>
       </c>
     </row>
     <row r="84" spans="1:16" x14ac:dyDescent="0.25">
@@ -6058,27 +6049,27 @@
       <c r="B84" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C84" s="77">
+      <c r="C84" s="74">
         <v>2.8000000000000001E-2</v>
       </c>
       <c r="D84" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E84" s="78">
+      <c r="E84" s="75">
         <v>61156</v>
       </c>
       <c r="F84" s="5">
         <v>2</v>
       </c>
       <c r="G84" s="2"/>
-      <c r="H84" s="78"/>
+      <c r="H84" s="75"/>
       <c r="I84" s="5"/>
       <c r="J84" s="2">
         <f>Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]+Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]</f>
         <v>122312</v>
       </c>
-      <c r="K84" s="78">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
+      <c r="K84" s="75">
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
         <v>17123.68</v>
       </c>
       <c r="L84" s="3">
@@ -6086,7 +6077,7 @@
         <v>0</v>
       </c>
       <c r="M84" s="2">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
         <v>12312</v>
       </c>
       <c r="N84" s="3">
@@ -6097,9 +6088,9 @@
         <f>SUM(Tabla22[[#This Row],[Bonus1]:[p2]])</f>
         <v>29435.68</v>
       </c>
-      <c r="P84" s="78">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
-        <v>-7964.32</v>
+      <c r="P84" s="75">
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v>-13564.32</v>
       </c>
     </row>
     <row r="85" spans="1:16" x14ac:dyDescent="0.25">
@@ -6109,13 +6100,13 @@
       <c r="B85" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C85" s="77">
+      <c r="C85" s="74">
         <v>2.7799999999999998E-2</v>
       </c>
       <c r="D85" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E85" s="78">
+      <c r="E85" s="75">
         <v>85384</v>
       </c>
       <c r="F85" s="5">
@@ -6124,7 +6115,7 @@
       <c r="G85" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="H85" s="78">
+      <c r="H85" s="75">
         <v>61275</v>
       </c>
       <c r="I85" s="5">
@@ -6134,8 +6125,8 @@
         <f>Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]+Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]</f>
         <v>378702</v>
       </c>
-      <c r="K85" s="78">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
+      <c r="K85" s="75">
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
         <v>28484.102399999996</v>
       </c>
       <c r="L85" s="3">
@@ -6143,7 +6134,7 @@
         <v>17034.45</v>
       </c>
       <c r="M85" s="2">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
         <v>10152</v>
       </c>
       <c r="N85" s="3">
@@ -6154,9 +6145,9 @@
         <f>SUM(Tabla22[[#This Row],[Bonus1]:[p2]])</f>
         <v>68220.5524</v>
       </c>
-      <c r="P85" s="78">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
-        <v>30820.5524</v>
+      <c r="P85" s="75">
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v>25220.5524</v>
       </c>
     </row>
     <row r="86" spans="1:16" x14ac:dyDescent="0.25">
@@ -6166,27 +6157,27 @@
       <c r="B86" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C86" s="77">
+      <c r="C86" s="74">
         <v>2.98E-2</v>
       </c>
       <c r="D86" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E86" s="78">
+      <c r="E86" s="75">
         <v>42066</v>
       </c>
       <c r="F86" s="5">
         <v>5</v>
       </c>
       <c r="G86" s="2"/>
-      <c r="H86" s="78"/>
+      <c r="H86" s="75"/>
       <c r="I86" s="5"/>
       <c r="J86" s="2">
         <f>Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]+Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]</f>
         <v>210330</v>
       </c>
-      <c r="K86" s="78">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
+      <c r="K86" s="75">
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
         <v>37607.004000000001</v>
       </c>
       <c r="L86" s="3">
@@ -6194,7 +6185,7 @@
         <v>0</v>
       </c>
       <c r="M86" s="2">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
         <v>24830</v>
       </c>
       <c r="N86" s="3">
@@ -6205,9 +6196,9 @@
         <f>SUM(Tabla22[[#This Row],[Bonus1]:[p2]])</f>
         <v>62437.004000000001</v>
       </c>
-      <c r="P86" s="78">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
-        <v>25037.004000000001</v>
+      <c r="P86" s="75">
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v>19437.004000000001</v>
       </c>
     </row>
     <row r="87" spans="1:16" x14ac:dyDescent="0.25">
@@ -6217,13 +6208,13 @@
       <c r="B87" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C87" s="77">
+      <c r="C87" s="74">
         <v>2.3400000000000001E-2</v>
       </c>
       <c r="D87" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E87" s="78">
+      <c r="E87" s="75">
         <v>42607</v>
       </c>
       <c r="F87" s="5">
@@ -6232,7 +6223,7 @@
       <c r="G87" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="H87" s="78">
+      <c r="H87" s="75">
         <v>59386</v>
       </c>
       <c r="I87" s="5">
@@ -6242,8 +6233,8 @@
         <f>Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]+Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]</f>
         <v>391193</v>
       </c>
-      <c r="K87" s="78">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
+      <c r="K87" s="75">
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
         <v>29910.113999999998</v>
       </c>
       <c r="L87" s="3">
@@ -6251,7 +6242,7 @@
         <v>20844.486000000001</v>
       </c>
       <c r="M87" s="2">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
         <v>27535</v>
       </c>
       <c r="N87" s="3">
@@ -6262,9 +6253,9 @@
         <f>SUM(Tabla22[[#This Row],[Bonus1]:[p2]])</f>
         <v>91447.6</v>
       </c>
-      <c r="P87" s="78">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
-        <v>54047.600000000006</v>
+      <c r="P87" s="75">
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v>48447.600000000006</v>
       </c>
     </row>
     <row r="88" spans="1:16" x14ac:dyDescent="0.25">
@@ -6274,27 +6265,27 @@
       <c r="B88" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C88" s="77">
+      <c r="C88" s="74">
         <v>1.7100000000000001E-2</v>
       </c>
       <c r="D88" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E88" s="78">
+      <c r="E88" s="75">
         <v>121779</v>
       </c>
       <c r="F88" s="5">
         <v>2</v>
       </c>
       <c r="G88" s="2"/>
-      <c r="H88" s="78"/>
+      <c r="H88" s="75"/>
       <c r="I88" s="5"/>
       <c r="J88" s="2">
         <f>Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]+Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]</f>
         <v>243558</v>
       </c>
-      <c r="K88" s="78">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
+      <c r="K88" s="75">
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
         <v>24989.050800000001</v>
       </c>
       <c r="L88" s="3">
@@ -6302,7 +6293,7 @@
         <v>0</v>
       </c>
       <c r="M88" s="2">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
         <v>5558</v>
       </c>
       <c r="N88" s="3">
@@ -6313,9 +6304,9 @@
         <f>SUM(Tabla22[[#This Row],[Bonus1]:[p2]])</f>
         <v>30547.050800000001</v>
       </c>
-      <c r="P88" s="78">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
-        <v>-6852.9491999999991</v>
+      <c r="P88" s="75">
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v>-12452.949199999999</v>
       </c>
     </row>
     <row r="89" spans="1:16" x14ac:dyDescent="0.25">
@@ -6325,13 +6316,13 @@
       <c r="B89" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C89" s="77">
+      <c r="C89" s="74">
         <v>1.7899999999999999E-2</v>
       </c>
       <c r="D89" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E89" s="78">
+      <c r="E89" s="75">
         <v>228495</v>
       </c>
       <c r="F89" s="5">
@@ -6340,7 +6331,7 @@
       <c r="G89" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="H89" s="78">
+      <c r="H89" s="75">
         <v>62131</v>
       </c>
       <c r="I89" s="5">
@@ -6350,8 +6341,8 @@
         <f>Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]+Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]</f>
         <v>871878</v>
       </c>
-      <c r="K89" s="78">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
+      <c r="K89" s="75">
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
         <v>49080.726000000002</v>
       </c>
       <c r="L89" s="3">
@@ -6359,7 +6350,7 @@
         <v>16682.173500000001</v>
       </c>
       <c r="M89" s="2">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
         <v>-28515</v>
       </c>
       <c r="N89" s="3">
@@ -6370,9 +6361,9 @@
         <f>SUM(Tabla22[[#This Row],[Bonus1]:[p2]])</f>
         <v>58640.8995</v>
       </c>
-      <c r="P89" s="78">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
-        <v>21240.8995</v>
+      <c r="P89" s="75">
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v>15640.8995</v>
       </c>
     </row>
     <row r="90" spans="1:16" x14ac:dyDescent="0.25">
@@ -6382,13 +6373,13 @@
       <c r="B90" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C90" s="77">
+      <c r="C90" s="74">
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="D90" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E90" s="78">
+      <c r="E90" s="75">
         <v>40769</v>
       </c>
       <c r="F90" s="5">
@@ -6397,7 +6388,7 @@
       <c r="G90" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="H90" s="78">
+      <c r="H90" s="75">
         <v>844341</v>
       </c>
       <c r="I90" s="5">
@@ -6407,8 +6398,8 @@
         <f>Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]+Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]</f>
         <v>1007417</v>
       </c>
-      <c r="K90" s="78">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
+      <c r="K90" s="75">
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
         <v>17612.207999999999</v>
       </c>
       <c r="L90" s="3">
@@ -6416,7 +6407,7 @@
         <v>91188.827999999994</v>
       </c>
       <c r="M90" s="2">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
         <v>14676</v>
       </c>
       <c r="N90" s="3">
@@ -6427,9 +6418,9 @@
         <f>SUM(Tabla22[[#This Row],[Bonus1]:[p2]])</f>
         <v>109818.03599999999</v>
       </c>
-      <c r="P90" s="78">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
-        <v>72418.035999999993</v>
+      <c r="P90" s="75">
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v>66818.035999999993</v>
       </c>
     </row>
     <row r="91" spans="1:16" x14ac:dyDescent="0.25">
@@ -6465,7 +6456,7 @@
         <v>869055</v>
       </c>
       <c r="K91" s="3">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
         <v>15298.494000000002</v>
       </c>
       <c r="L91" s="3">
@@ -6473,7 +6464,7 @@
         <v>44771.212800000001</v>
       </c>
       <c r="M91" s="2">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
         <v>21567</v>
       </c>
       <c r="N91" s="3">
@@ -6485,8 +6476,8 @@
         <v>50124.7068</v>
       </c>
       <c r="P91" s="3">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
-        <v>12724.7068</v>
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v>7124.7067999999999</v>
       </c>
     </row>
     <row r="92" spans="1:16" x14ac:dyDescent="0.25">
@@ -6522,7 +6513,7 @@
         <v>313573</v>
       </c>
       <c r="K92" s="39">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
         <v>4742.2479999999996</v>
       </c>
       <c r="L92" s="39">
@@ -6530,7 +6521,7 @@
         <v>15271.44</v>
       </c>
       <c r="M92" s="38">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
         <v>7398</v>
       </c>
       <c r="N92" s="39">
@@ -6542,8 +6533,8 @@
         <v>32586.688000000002</v>
       </c>
       <c r="P92" s="39">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
-        <v>-4813.3119999999981</v>
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v>-10413.311999999998</v>
       </c>
     </row>
     <row r="93" spans="1:16" x14ac:dyDescent="0.25">
@@ -6553,38 +6544,38 @@
       <c r="B93" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C93" s="77"/>
+      <c r="C93" s="74"/>
       <c r="D93" s="2"/>
-      <c r="E93" s="78"/>
+      <c r="E93" s="75"/>
       <c r="G93" s="2"/>
-      <c r="H93" s="78"/>
+      <c r="H93" s="75"/>
       <c r="I93" s="5"/>
       <c r="J93" s="2">
         <f>Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]+Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]</f>
         <v>0</v>
       </c>
-      <c r="K93" s="78" t="e">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
-        <v>#N/A</v>
+      <c r="K93" s="3">
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
+        <v>0</v>
       </c>
       <c r="L93" s="3">
         <f>IF(Tabla22[[#This Row],[Req.2]]&gt;0,LOOKUP(Tabla22[[#This Row],[Product2]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]*Tabla22[[#This Row],[QualityBonus]],0)</f>
         <v>0</v>
       </c>
-      <c r="M93" s="2" t="e">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
-        <v>#N/A</v>
+      <c r="M93" s="85">
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
+        <v>0</v>
       </c>
       <c r="N93" s="3">
         <f>IF(Tabla22[[#This Row],[Req.2]]&gt;0,(Tabla22[[#This Row],[Base price2]]-LOOKUP(Tabla22[[#This Row],[Product2]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.2]],0)</f>
         <v>0</v>
       </c>
-      <c r="O93" s="2" t="e">
+      <c r="O93" s="2">
         <f>SUM(Tabla22[[#This Row],[Bonus1]:[p2]])</f>
-        <v>#N/A</v>
-      </c>
-      <c r="P93" s="78" t="str">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
+        <v>0</v>
+      </c>
+      <c r="P93" s="3" t="str">
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
         <v/>
       </c>
     </row>
@@ -6595,38 +6586,38 @@
       <c r="B94" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C94" s="77"/>
+      <c r="C94" s="74"/>
       <c r="D94" s="2"/>
-      <c r="E94" s="78"/>
+      <c r="E94" s="75"/>
       <c r="G94" s="2"/>
-      <c r="H94" s="78"/>
+      <c r="H94" s="75"/>
       <c r="I94" s="5"/>
       <c r="J94" s="2">
         <f>Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]+Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]</f>
         <v>0</v>
       </c>
-      <c r="K94" s="78" t="e">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
-        <v>#N/A</v>
+      <c r="K94" s="3">
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
+        <v>0</v>
       </c>
       <c r="L94" s="3">
         <f>IF(Tabla22[[#This Row],[Req.2]]&gt;0,LOOKUP(Tabla22[[#This Row],[Product2]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]*Tabla22[[#This Row],[QualityBonus]],0)</f>
         <v>0</v>
       </c>
-      <c r="M94" s="2" t="e">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
-        <v>#N/A</v>
+      <c r="M94" s="2">
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
+        <v>0</v>
       </c>
       <c r="N94" s="3">
         <f>IF(Tabla22[[#This Row],[Req.2]]&gt;0,(Tabla22[[#This Row],[Base price2]]-LOOKUP(Tabla22[[#This Row],[Product2]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.2]],0)</f>
         <v>0</v>
       </c>
-      <c r="O94" s="2" t="e">
+      <c r="O94" s="2">
         <f>SUM(Tabla22[[#This Row],[Bonus1]:[p2]])</f>
-        <v>#N/A</v>
-      </c>
-      <c r="P94" s="78" t="str">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
+        <v>0</v>
+      </c>
+      <c r="P94" s="3" t="str">
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
         <v/>
       </c>
     </row>
@@ -6637,38 +6628,38 @@
       <c r="B95" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C95" s="77"/>
+      <c r="C95" s="74"/>
       <c r="D95" s="2"/>
-      <c r="E95" s="78"/>
+      <c r="E95" s="75"/>
       <c r="G95" s="2"/>
-      <c r="H95" s="78"/>
+      <c r="H95" s="75"/>
       <c r="I95" s="5"/>
       <c r="J95" s="2">
         <f>Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]+Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]</f>
         <v>0</v>
       </c>
-      <c r="K95" s="78" t="e">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
-        <v>#N/A</v>
+      <c r="K95" s="3">
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
+        <v>0</v>
       </c>
       <c r="L95" s="3">
         <f>IF(Tabla22[[#This Row],[Req.2]]&gt;0,LOOKUP(Tabla22[[#This Row],[Product2]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]*Tabla22[[#This Row],[QualityBonus]],0)</f>
         <v>0</v>
       </c>
-      <c r="M95" s="2" t="e">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
-        <v>#N/A</v>
+      <c r="M95" s="2">
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
+        <v>0</v>
       </c>
       <c r="N95" s="3">
         <f>IF(Tabla22[[#This Row],[Req.2]]&gt;0,(Tabla22[[#This Row],[Base price2]]-LOOKUP(Tabla22[[#This Row],[Product2]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.2]],0)</f>
         <v>0</v>
       </c>
-      <c r="O95" s="2" t="e">
+      <c r="O95" s="2">
         <f>SUM(Tabla22[[#This Row],[Bonus1]:[p2]])</f>
-        <v>#N/A</v>
-      </c>
-      <c r="P95" s="78" t="str">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
+        <v>0</v>
+      </c>
+      <c r="P95" s="3" t="str">
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
         <v/>
       </c>
     </row>
@@ -6679,38 +6670,38 @@
       <c r="B96" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C96" s="77"/>
+      <c r="C96" s="74"/>
       <c r="D96" s="2"/>
-      <c r="E96" s="78"/>
+      <c r="E96" s="75"/>
       <c r="G96" s="2"/>
-      <c r="H96" s="78"/>
+      <c r="H96" s="75"/>
       <c r="I96" s="5"/>
       <c r="J96" s="2">
         <f>Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]+Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]</f>
         <v>0</v>
       </c>
-      <c r="K96" s="78" t="e">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
-        <v>#N/A</v>
+      <c r="K96" s="3">
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
+        <v>0</v>
       </c>
       <c r="L96" s="3">
         <f>IF(Tabla22[[#This Row],[Req.2]]&gt;0,LOOKUP(Tabla22[[#This Row],[Product2]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]*Tabla22[[#This Row],[QualityBonus]],0)</f>
         <v>0</v>
       </c>
-      <c r="M96" s="2" t="e">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
-        <v>#N/A</v>
+      <c r="M96" s="2">
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
+        <v>0</v>
       </c>
       <c r="N96" s="3">
         <f>IF(Tabla22[[#This Row],[Req.2]]&gt;0,(Tabla22[[#This Row],[Base price2]]-LOOKUP(Tabla22[[#This Row],[Product2]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.2]],0)</f>
         <v>0</v>
       </c>
-      <c r="O96" s="2" t="e">
+      <c r="O96" s="2">
         <f>SUM(Tabla22[[#This Row],[Bonus1]:[p2]])</f>
-        <v>#N/A</v>
-      </c>
-      <c r="P96" s="78" t="str">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
+        <v>0</v>
+      </c>
+      <c r="P96" s="3" t="str">
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
         <v/>
       </c>
     </row>
@@ -6721,38 +6712,38 @@
       <c r="B97" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C97" s="77"/>
+      <c r="C97" s="74"/>
       <c r="D97" s="2"/>
-      <c r="E97" s="78"/>
+      <c r="E97" s="75"/>
       <c r="G97" s="2"/>
-      <c r="H97" s="78"/>
+      <c r="H97" s="75"/>
       <c r="I97" s="5"/>
       <c r="J97" s="2">
         <f>Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]+Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]</f>
         <v>0</v>
       </c>
-      <c r="K97" s="78" t="e">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
-        <v>#N/A</v>
+      <c r="K97" s="3">
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
+        <v>0</v>
       </c>
       <c r="L97" s="3">
         <f>IF(Tabla22[[#This Row],[Req.2]]&gt;0,LOOKUP(Tabla22[[#This Row],[Product2]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]*Tabla22[[#This Row],[QualityBonus]],0)</f>
         <v>0</v>
       </c>
-      <c r="M97" s="2" t="e">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
-        <v>#N/A</v>
+      <c r="M97" s="2">
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
+        <v>0</v>
       </c>
       <c r="N97" s="3">
         <f>IF(Tabla22[[#This Row],[Req.2]]&gt;0,(Tabla22[[#This Row],[Base price2]]-LOOKUP(Tabla22[[#This Row],[Product2]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.2]],0)</f>
         <v>0</v>
       </c>
-      <c r="O97" s="2" t="e">
+      <c r="O97" s="2">
         <f>SUM(Tabla22[[#This Row],[Bonus1]:[p2]])</f>
-        <v>#N/A</v>
-      </c>
-      <c r="P97" s="78" t="str">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
+        <v>0</v>
+      </c>
+      <c r="P97" s="3" t="str">
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
         <v/>
       </c>
     </row>
@@ -6763,38 +6754,38 @@
       <c r="B98" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C98" s="77"/>
+      <c r="C98" s="74"/>
       <c r="D98" s="2"/>
-      <c r="E98" s="78"/>
+      <c r="E98" s="75"/>
       <c r="G98" s="2"/>
-      <c r="H98" s="78"/>
+      <c r="H98" s="75"/>
       <c r="I98" s="5"/>
       <c r="J98" s="2">
         <f>Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]+Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]</f>
         <v>0</v>
       </c>
-      <c r="K98" s="78" t="e">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
-        <v>#N/A</v>
+      <c r="K98" s="3">
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
+        <v>0</v>
       </c>
       <c r="L98" s="3">
         <f>IF(Tabla22[[#This Row],[Req.2]]&gt;0,LOOKUP(Tabla22[[#This Row],[Product2]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]*Tabla22[[#This Row],[QualityBonus]],0)</f>
         <v>0</v>
       </c>
-      <c r="M98" s="2" t="e">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
-        <v>#N/A</v>
+      <c r="M98" s="2">
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
+        <v>0</v>
       </c>
       <c r="N98" s="3">
         <f>IF(Tabla22[[#This Row],[Req.2]]&gt;0,(Tabla22[[#This Row],[Base price2]]-LOOKUP(Tabla22[[#This Row],[Product2]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.2]],0)</f>
         <v>0</v>
       </c>
-      <c r="O98" s="2" t="e">
+      <c r="O98" s="2">
         <f>SUM(Tabla22[[#This Row],[Bonus1]:[p2]])</f>
-        <v>#N/A</v>
-      </c>
-      <c r="P98" s="78" t="str">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
+        <v>0</v>
+      </c>
+      <c r="P98" s="3" t="str">
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
         <v/>
       </c>
     </row>
@@ -6805,38 +6796,38 @@
       <c r="B99" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C99" s="77"/>
+      <c r="C99" s="74"/>
       <c r="D99" s="2"/>
-      <c r="E99" s="78"/>
+      <c r="E99" s="75"/>
       <c r="G99" s="2"/>
-      <c r="H99" s="78"/>
+      <c r="H99" s="75"/>
       <c r="I99" s="5"/>
       <c r="J99" s="2">
         <f>Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]+Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]</f>
         <v>0</v>
       </c>
-      <c r="K99" s="78" t="e">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
-        <v>#N/A</v>
+      <c r="K99" s="3">
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
+        <v>0</v>
       </c>
       <c r="L99" s="3">
         <f>IF(Tabla22[[#This Row],[Req.2]]&gt;0,LOOKUP(Tabla22[[#This Row],[Product2]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]*Tabla22[[#This Row],[QualityBonus]],0)</f>
         <v>0</v>
       </c>
-      <c r="M99" s="2" t="e">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
-        <v>#N/A</v>
+      <c r="M99" s="2">
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
+        <v>0</v>
       </c>
       <c r="N99" s="3">
         <f>IF(Tabla22[[#This Row],[Req.2]]&gt;0,(Tabla22[[#This Row],[Base price2]]-LOOKUP(Tabla22[[#This Row],[Product2]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.2]],0)</f>
         <v>0</v>
       </c>
-      <c r="O99" s="2" t="e">
+      <c r="O99" s="2">
         <f>SUM(Tabla22[[#This Row],[Bonus1]:[p2]])</f>
-        <v>#N/A</v>
-      </c>
-      <c r="P99" s="78" t="str">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
+        <v>0</v>
+      </c>
+      <c r="P99" s="3" t="str">
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
         <v/>
       </c>
     </row>
@@ -6847,38 +6838,38 @@
       <c r="B100" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C100" s="77"/>
+      <c r="C100" s="74"/>
       <c r="D100" s="2"/>
-      <c r="E100" s="78"/>
+      <c r="E100" s="75"/>
       <c r="G100" s="2"/>
-      <c r="H100" s="78"/>
+      <c r="H100" s="75"/>
       <c r="I100" s="5"/>
       <c r="J100" s="2">
         <f>Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]+Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]</f>
         <v>0</v>
       </c>
-      <c r="K100" s="78" t="e">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
-        <v>#N/A</v>
+      <c r="K100" s="3">
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
+        <v>0</v>
       </c>
       <c r="L100" s="3">
         <f>IF(Tabla22[[#This Row],[Req.2]]&gt;0,LOOKUP(Tabla22[[#This Row],[Product2]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]*Tabla22[[#This Row],[QualityBonus]],0)</f>
         <v>0</v>
       </c>
-      <c r="M100" s="2" t="e">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
-        <v>#N/A</v>
+      <c r="M100" s="2">
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
+        <v>0</v>
       </c>
       <c r="N100" s="3">
         <f>IF(Tabla22[[#This Row],[Req.2]]&gt;0,(Tabla22[[#This Row],[Base price2]]-LOOKUP(Tabla22[[#This Row],[Product2]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.2]],0)</f>
         <v>0</v>
       </c>
-      <c r="O100" s="2" t="e">
+      <c r="O100" s="2">
         <f>SUM(Tabla22[[#This Row],[Bonus1]:[p2]])</f>
-        <v>#N/A</v>
-      </c>
-      <c r="P100" s="78" t="str">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
+        <v>0</v>
+      </c>
+      <c r="P100" s="3" t="str">
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
         <v/>
       </c>
     </row>
@@ -6889,38 +6880,164 @@
       <c r="B101" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C101" s="77"/>
+      <c r="C101" s="74"/>
       <c r="D101" s="2"/>
-      <c r="E101" s="78"/>
+      <c r="E101" s="75"/>
       <c r="G101" s="2"/>
-      <c r="H101" s="78"/>
+      <c r="H101" s="75"/>
       <c r="I101" s="5"/>
       <c r="J101" s="2">
         <f>Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]+Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]</f>
         <v>0</v>
       </c>
-      <c r="K101" s="78" t="e">
-        <f>LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]</f>
-        <v>#N/A</v>
+      <c r="K101" s="3">
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
+        <v>0</v>
       </c>
       <c r="L101" s="3">
         <f>IF(Tabla22[[#This Row],[Req.2]]&gt;0,LOOKUP(Tabla22[[#This Row],[Product2]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]*Tabla22[[#This Row],[QualityBonus]],0)</f>
         <v>0</v>
       </c>
-      <c r="M101" s="2" t="e">
-        <f>(Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]]</f>
-        <v>#N/A</v>
+      <c r="M101" s="2">
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
+        <v>0</v>
       </c>
       <c r="N101" s="3">
         <f>IF(Tabla22[[#This Row],[Req.2]]&gt;0,(Tabla22[[#This Row],[Base price2]]-LOOKUP(Tabla22[[#This Row],[Product2]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.2]],0)</f>
         <v>0</v>
       </c>
-      <c r="O101" s="2" t="e">
+      <c r="O101" s="2">
         <f>SUM(Tabla22[[#This Row],[Bonus1]:[p2]])</f>
-        <v>#N/A</v>
-      </c>
-      <c r="P101" s="78" t="str">
-        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[TOTAL PROFIT (no wages, no admin costs)]]-$C$4,"")</f>
+        <v>0</v>
+      </c>
+      <c r="P101" s="3" t="str">
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="102" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A102" s="13">
+        <v>86</v>
+      </c>
+      <c r="B102" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C102" s="74"/>
+      <c r="D102" s="2"/>
+      <c r="E102" s="75"/>
+      <c r="G102" s="2"/>
+      <c r="H102" s="75"/>
+      <c r="I102" s="5"/>
+      <c r="J102" s="2">
+        <f>Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]+Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]</f>
+        <v>0</v>
+      </c>
+      <c r="K102" s="6">
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="L102" s="75">
+        <f>IF(Tabla22[[#This Row],[Req.2]]&gt;0,LOOKUP(Tabla22[[#This Row],[Product2]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]*Tabla22[[#This Row],[QualityBonus]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="M102" s="76">
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="N102" s="75">
+        <f>IF(Tabla22[[#This Row],[Req.2]]&gt;0,(Tabla22[[#This Row],[Base price2]]-LOOKUP(Tabla22[[#This Row],[Product2]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.2]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="O102" s="76">
+        <f>SUM(Tabla22[[#This Row],[Bonus1]:[p2]])</f>
+        <v>0</v>
+      </c>
+      <c r="P102" s="75" t="str">
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A103" s="13">
+        <v>87</v>
+      </c>
+      <c r="B103" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C103" s="74"/>
+      <c r="D103" s="2"/>
+      <c r="E103" s="75"/>
+      <c r="G103" s="2"/>
+      <c r="H103" s="75"/>
+      <c r="I103" s="5"/>
+      <c r="J103" s="2">
+        <f>Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]+Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]</f>
+        <v>0</v>
+      </c>
+      <c r="K103" s="6">
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="L103" s="75">
+        <f>IF(Tabla22[[#This Row],[Req.2]]&gt;0,LOOKUP(Tabla22[[#This Row],[Product2]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]*Tabla22[[#This Row],[QualityBonus]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="M103" s="76">
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="N103" s="75">
+        <f>IF(Tabla22[[#This Row],[Req.2]]&gt;0,(Tabla22[[#This Row],[Base price2]]-LOOKUP(Tabla22[[#This Row],[Product2]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.2]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="O103" s="76">
+        <f>SUM(Tabla22[[#This Row],[Bonus1]:[p2]])</f>
+        <v>0</v>
+      </c>
+      <c r="P103" s="75" t="str">
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="104" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A104" s="13">
+        <v>88</v>
+      </c>
+      <c r="B104" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C104" s="74"/>
+      <c r="D104" s="2"/>
+      <c r="E104" s="75"/>
+      <c r="G104" s="2"/>
+      <c r="H104" s="75"/>
+      <c r="I104" s="5"/>
+      <c r="J104" s="2">
+        <f>Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]+Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]</f>
+        <v>0</v>
+      </c>
+      <c r="K104" s="6">
+        <f>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="L104" s="75">
+        <f>IF(Tabla22[[#This Row],[Req.2]]&gt;0,LOOKUP(Tabla22[[#This Row],[Product2]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]*Tabla22[[#This Row],[QualityBonus]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="M104" s="76">
+        <f>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="N104" s="75">
+        <f>IF(Tabla22[[#This Row],[Req.2]]&gt;0,(Tabla22[[#This Row],[Base price2]]-LOOKUP(Tabla22[[#This Row],[Product2]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.2]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="O104" s="76">
+        <f>SUM(Tabla22[[#This Row],[Bonus1]:[p2]])</f>
+        <v>0</v>
+      </c>
+      <c r="P104" s="75" t="str">
+        <f>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[P_T]]-$C$4,"")</f>
         <v/>
       </c>
     </row>
@@ -6928,9 +7045,9 @@
   <mergeCells count="5">
     <mergeCell ref="D15:F15"/>
     <mergeCell ref="G15:I15"/>
-    <mergeCell ref="J15:O15"/>
     <mergeCell ref="F3:L3"/>
     <mergeCell ref="N3:U3"/>
+    <mergeCell ref="J15:P15"/>
   </mergeCells>
   <conditionalFormatting sqref="G5:H10">
     <cfRule type="colorScale" priority="35">
@@ -7052,8 +7169,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P17:P101">
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="lessThan">
+  <conditionalFormatting sqref="P17:P104">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7078,10 +7195,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2 B17:B101">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2 B17:B104">
       <formula1>$B$10:$B$12</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D17:D101 G17:G101">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D17:D104 G17:G104">
       <formula1>$E$5:$E$10</formula1>
     </dataValidation>
   </dataValidations>
@@ -7141,33 +7258,33 @@
         <v>63</v>
       </c>
       <c r="H5" s="12"/>
-      <c r="I5" s="74" t="s">
+      <c r="I5" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="J5" s="74"/>
-      <c r="K5" s="74"/>
-      <c r="L5" s="74"/>
-      <c r="M5" s="74"/>
-      <c r="N5" s="74"/>
-      <c r="O5" s="74"/>
-      <c r="P5" s="74"/>
-      <c r="Q5" s="74"/>
-      <c r="R5" s="74"/>
-      <c r="S5" s="75"/>
+      <c r="J5" s="71"/>
+      <c r="K5" s="71"/>
+      <c r="L5" s="71"/>
+      <c r="M5" s="71"/>
+      <c r="N5" s="71"/>
+      <c r="O5" s="71"/>
+      <c r="P5" s="71"/>
+      <c r="Q5" s="71"/>
+      <c r="R5" s="71"/>
+      <c r="S5" s="72"/>
       <c r="U5" s="12"/>
-      <c r="V5" s="74" t="s">
+      <c r="V5" s="71" t="s">
         <v>16</v>
       </c>
-      <c r="W5" s="74"/>
-      <c r="X5" s="74"/>
-      <c r="Y5" s="74"/>
-      <c r="Z5" s="74"/>
-      <c r="AA5" s="74"/>
-      <c r="AB5" s="74"/>
-      <c r="AC5" s="74"/>
-      <c r="AD5" s="74"/>
-      <c r="AE5" s="74"/>
-      <c r="AF5" s="75"/>
+      <c r="W5" s="71"/>
+      <c r="X5" s="71"/>
+      <c r="Y5" s="71"/>
+      <c r="Z5" s="71"/>
+      <c r="AA5" s="71"/>
+      <c r="AB5" s="71"/>
+      <c r="AC5" s="71"/>
+      <c r="AD5" s="71"/>
+      <c r="AE5" s="71"/>
+      <c r="AF5" s="72"/>
     </row>
     <row r="6" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
@@ -9508,33 +9625,33 @@
         <v>70.928000000000011</v>
       </c>
       <c r="H30" s="12"/>
-      <c r="I30" s="74" t="s">
+      <c r="I30" s="71" t="s">
         <v>17</v>
       </c>
-      <c r="J30" s="74"/>
-      <c r="K30" s="74"/>
-      <c r="L30" s="74"/>
-      <c r="M30" s="74"/>
-      <c r="N30" s="74"/>
-      <c r="O30" s="74"/>
-      <c r="P30" s="74"/>
-      <c r="Q30" s="74"/>
-      <c r="R30" s="74"/>
-      <c r="S30" s="75"/>
+      <c r="J30" s="71"/>
+      <c r="K30" s="71"/>
+      <c r="L30" s="71"/>
+      <c r="M30" s="71"/>
+      <c r="N30" s="71"/>
+      <c r="O30" s="71"/>
+      <c r="P30" s="71"/>
+      <c r="Q30" s="71"/>
+      <c r="R30" s="71"/>
+      <c r="S30" s="72"/>
       <c r="U30" s="12"/>
-      <c r="V30" s="74" t="s">
+      <c r="V30" s="71" t="s">
         <v>15</v>
       </c>
-      <c r="W30" s="74"/>
-      <c r="X30" s="74"/>
-      <c r="Y30" s="74"/>
-      <c r="Z30" s="74"/>
-      <c r="AA30" s="74"/>
-      <c r="AB30" s="74"/>
-      <c r="AC30" s="74"/>
-      <c r="AD30" s="74"/>
-      <c r="AE30" s="74"/>
-      <c r="AF30" s="75"/>
+      <c r="W30" s="71"/>
+      <c r="X30" s="71"/>
+      <c r="Y30" s="71"/>
+      <c r="Z30" s="71"/>
+      <c r="AA30" s="71"/>
+      <c r="AB30" s="71"/>
+      <c r="AC30" s="71"/>
+      <c r="AD30" s="71"/>
+      <c r="AE30" s="71"/>
+      <c r="AF30" s="72"/>
     </row>
     <row r="31" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B31" s="29" t="s">
@@ -11647,14 +11764,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B1" s="76" t="s">
+      <c r="B1" s="73" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="76"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="73"/>
     </row>
     <row r="2" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -12076,7 +12193,7 @@
         <v>1</v>
       </c>
       <c r="H21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
@@ -12105,7 +12222,7 @@
         <v>1</v>
       </c>
       <c r="H22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Will not produce SATs
</commit_message>
<xml_diff>
--- a/SalesOffice_archive.xlsx
+++ b/SalesOffice_archive.xlsx
@@ -318,7 +318,7 @@
     <numFmt numFmtId="165" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="0.0%"/>
     <numFmt numFmtId="167" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="0.000"/>
+    <numFmt numFmtId="168" formatCode="0.000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -737,6 +737,12 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="7" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -770,12 +776,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -784,6 +784,16 @@
     <cellStyle name="Porcentaje" xfId="3" builtinId="5"/>
   </cellStyles>
   <dxfs count="24">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFABAB"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1110,16 +1120,6 @@
       </font>
       <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFABAB"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -1147,32 +1147,32 @@
   <tableColumns count="16">
     <tableColumn id="1" name="No."/>
     <tableColumn id="23" name="Economy "/>
-    <tableColumn id="2" name="QualityBonus" dataDxfId="22" dataCellStyle="Porcentaje"/>
-    <tableColumn id="3" name="Product" dataDxfId="21" dataCellStyle="Moneda"/>
-    <tableColumn id="7" name="Base price1" dataDxfId="20" dataCellStyle="Moneda"/>
-    <tableColumn id="24" name="Req." dataDxfId="19" dataCellStyle="Millares"/>
-    <tableColumn id="18" name="Product2" dataDxfId="18" dataCellStyle="Moneda"/>
-    <tableColumn id="8" name="Base price2" dataDxfId="17" dataCellStyle="Moneda"/>
-    <tableColumn id="35" name="Req.2" dataDxfId="16" dataCellStyle="Millares"/>
-    <tableColumn id="12" name="Order price" dataDxfId="15" dataCellStyle="Moneda">
+    <tableColumn id="2" name="QualityBonus" dataDxfId="23" dataCellStyle="Porcentaje"/>
+    <tableColumn id="3" name="Product" dataDxfId="22" dataCellStyle="Moneda"/>
+    <tableColumn id="7" name="Base price1" dataDxfId="21" dataCellStyle="Moneda"/>
+    <tableColumn id="24" name="Req." dataDxfId="20" dataCellStyle="Millares"/>
+    <tableColumn id="18" name="Product2" dataDxfId="19" dataCellStyle="Moneda"/>
+    <tableColumn id="8" name="Base price2" dataDxfId="18" dataCellStyle="Moneda"/>
+    <tableColumn id="35" name="Req.2" dataDxfId="17" dataCellStyle="Millares"/>
+    <tableColumn id="12" name="Order price" dataDxfId="16" dataCellStyle="Moneda">
       <calculatedColumnFormula>Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]]+Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Bonus1" dataDxfId="14" dataCellStyle="Moneda">
+    <tableColumn id="4" name="Bonus1" dataDxfId="15" dataCellStyle="Moneda">
       <calculatedColumnFormula>IFERROR(LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[QualityBonus]]*Tabla22[[#This Row],[Base price1]]*Tabla22[[#This Row],[Req.]],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="Bonus2" dataDxfId="13" dataCellStyle="Moneda">
+    <tableColumn id="11" name="Bonus2" dataDxfId="14" dataCellStyle="Moneda">
       <calculatedColumnFormula>IF(Tabla22[[#This Row],[Req.2]]&gt;0,LOOKUP(Tabla22[[#This Row],[Product2]],$R$18:$R$23,$T$18:$T$23)*Tabla22[[#This Row],[Base price2]]*Tabla22[[#This Row],[Req.2]]*Tabla22[[#This Row],[QualityBonus]],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="p1" dataDxfId="12" dataCellStyle="Moneda">
+    <tableColumn id="10" name="p1" dataDxfId="13" dataCellStyle="Moneda">
       <calculatedColumnFormula>IFERROR((Tabla22[[#This Row],[Base price1]]-LOOKUP(Tabla22[[#This Row],[Product]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.]],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="p2" dataDxfId="11" dataCellStyle="Moneda">
+    <tableColumn id="9" name="p2" dataDxfId="12" dataCellStyle="Moneda">
       <calculatedColumnFormula>IF(Tabla22[[#This Row],[Req.2]]&gt;0,(Tabla22[[#This Row],[Base price2]]-LOOKUP(Tabla22[[#This Row],[Product2]],$R$18:$R$23,$S$18:$S$23))*Tabla22[[#This Row],[Req.2]],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="30" name="No wages" dataDxfId="10" dataCellStyle="Moneda">
+    <tableColumn id="30" name="No wages" dataDxfId="11" dataCellStyle="Moneda">
       <calculatedColumnFormula>SUM(Tabla22[[#This Row],[Bonus1]:[p2]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="36" name="profit -wages" dataDxfId="9" dataCellStyle="Moneda">
+    <tableColumn id="36" name="profit -wages" dataDxfId="10" dataCellStyle="Moneda">
       <calculatedColumnFormula>IF(Tabla22[[#This Row],[QualityBonus]]&gt;0,Tabla22[[#This Row],[No wages]]-$C$4,"")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1181,35 +1181,35 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="R17:T23" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="R17:T23" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8">
   <autoFilter ref="R17:T23"/>
   <sortState ref="T18:V23">
     <sortCondition ref="T17:T23"/>
   </sortState>
   <tableColumns count="3">
-    <tableColumn id="1" name="Goods sold" dataDxfId="6"/>
-    <tableColumn id="2" name="COGS" dataDxfId="5"/>
-    <tableColumn id="3" name="Q" dataDxfId="4"/>
+    <tableColumn id="1" name="Goods sold" dataDxfId="7"/>
+    <tableColumn id="2" name="COGS" dataDxfId="6"/>
+    <tableColumn id="3" name="Q" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla3" displayName="Tabla3" ref="B8:E19" totalsRowShown="0" dataDxfId="3" dataCellStyle="Moneda">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla3" displayName="Tabla3" ref="B8:E19" totalsRowShown="0" dataDxfId="4" dataCellStyle="Moneda">
   <autoFilter ref="B8:E19"/>
   <sortState ref="B9:E19">
     <sortCondition ref="B8:B19"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" name="Quality"/>
-    <tableColumn id="2" name="Unit price" dataDxfId="2" dataCellStyle="Moneda">
+    <tableColumn id="2" name="Unit price" dataDxfId="3" dataCellStyle="Moneda">
       <calculatedColumnFormula>$C$3*(1+$C$4*B9)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Unit profit" dataDxfId="1" dataCellStyle="Moneda">
+    <tableColumn id="3" name="Unit profit" dataDxfId="2" dataCellStyle="Moneda">
       <calculatedColumnFormula>C9-$C$5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Total profit" dataDxfId="0" dataCellStyle="Moneda">
+    <tableColumn id="4" name="Total profit" dataDxfId="1" dataCellStyle="Moneda">
       <calculatedColumnFormula>D9*$C$6</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1530,35 +1530,35 @@
       <c r="AB2" s="46"/>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="F3" s="90" t="s">
+      <c r="F3" s="96" t="s">
         <v>65</v>
       </c>
-      <c r="G3" s="91"/>
-      <c r="H3" s="91"/>
-      <c r="I3" s="91"/>
-      <c r="J3" s="91"/>
-      <c r="K3" s="91"/>
-      <c r="L3" s="91"/>
-      <c r="N3" s="90" t="s">
+      <c r="G3" s="97"/>
+      <c r="H3" s="97"/>
+      <c r="I3" s="97"/>
+      <c r="J3" s="97"/>
+      <c r="K3" s="97"/>
+      <c r="L3" s="97"/>
+      <c r="N3" s="96" t="s">
         <v>69</v>
       </c>
-      <c r="O3" s="91"/>
-      <c r="P3" s="91"/>
-      <c r="Q3" s="91"/>
-      <c r="R3" s="91"/>
-      <c r="S3" s="91"/>
-      <c r="T3" s="91"/>
-      <c r="U3" s="91"/>
-      <c r="W3" s="90" t="s">
+      <c r="O3" s="97"/>
+      <c r="P3" s="97"/>
+      <c r="Q3" s="97"/>
+      <c r="R3" s="97"/>
+      <c r="S3" s="97"/>
+      <c r="T3" s="97"/>
+      <c r="U3" s="97"/>
+      <c r="W3" s="96" t="s">
         <v>69</v>
       </c>
-      <c r="X3" s="91"/>
-      <c r="Y3" s="91"/>
-      <c r="Z3" s="91"/>
-      <c r="AA3" s="91"/>
-      <c r="AB3" s="91"/>
-      <c r="AC3" s="91"/>
-      <c r="AD3" s="91"/>
+      <c r="X3" s="97"/>
+      <c r="Y3" s="97"/>
+      <c r="Z3" s="97"/>
+      <c r="AA3" s="97"/>
+      <c r="AB3" s="97"/>
+      <c r="AC3" s="97"/>
+      <c r="AD3" s="97"/>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B4" s="35" t="s">
@@ -2336,25 +2336,25 @@
       <c r="W14" s="46"/>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="D15" s="92" t="s">
+      <c r="D15" s="98" t="s">
         <v>45</v>
       </c>
-      <c r="E15" s="93"/>
-      <c r="F15" s="94"/>
-      <c r="G15" s="95" t="s">
+      <c r="E15" s="99"/>
+      <c r="F15" s="100"/>
+      <c r="G15" s="101" t="s">
         <v>46</v>
       </c>
-      <c r="H15" s="93"/>
-      <c r="I15" s="94"/>
-      <c r="J15" s="96" t="s">
+      <c r="H15" s="99"/>
+      <c r="I15" s="100"/>
+      <c r="J15" s="102" t="s">
         <v>49</v>
       </c>
-      <c r="K15" s="97"/>
-      <c r="L15" s="97"/>
-      <c r="M15" s="97"/>
-      <c r="N15" s="97"/>
-      <c r="O15" s="97"/>
-      <c r="P15" s="97"/>
+      <c r="K15" s="103"/>
+      <c r="L15" s="103"/>
+      <c r="M15" s="103"/>
+      <c r="N15" s="103"/>
+      <c r="O15" s="103"/>
+      <c r="P15" s="103"/>
       <c r="R15" s="46"/>
       <c r="S15" s="46"/>
       <c r="T15" s="46"/>
@@ -12195,7 +12195,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P17:P200">
-    <cfRule type="cellIs" dxfId="23" priority="17" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="17" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12353,33 +12353,33 @@
         <v>63</v>
       </c>
       <c r="H5" s="12"/>
-      <c r="I5" s="98" t="s">
+      <c r="I5" s="104" t="s">
         <v>14</v>
       </c>
-      <c r="J5" s="98"/>
-      <c r="K5" s="98"/>
-      <c r="L5" s="98"/>
-      <c r="M5" s="98"/>
-      <c r="N5" s="98"/>
-      <c r="O5" s="98"/>
-      <c r="P5" s="98"/>
-      <c r="Q5" s="98"/>
-      <c r="R5" s="98"/>
-      <c r="S5" s="99"/>
+      <c r="J5" s="104"/>
+      <c r="K5" s="104"/>
+      <c r="L5" s="104"/>
+      <c r="M5" s="104"/>
+      <c r="N5" s="104"/>
+      <c r="O5" s="104"/>
+      <c r="P5" s="104"/>
+      <c r="Q5" s="104"/>
+      <c r="R5" s="104"/>
+      <c r="S5" s="105"/>
       <c r="U5" s="12"/>
-      <c r="V5" s="98" t="s">
+      <c r="V5" s="104" t="s">
         <v>16</v>
       </c>
-      <c r="W5" s="98"/>
-      <c r="X5" s="98"/>
-      <c r="Y5" s="98"/>
-      <c r="Z5" s="98"/>
-      <c r="AA5" s="98"/>
-      <c r="AB5" s="98"/>
-      <c r="AC5" s="98"/>
-      <c r="AD5" s="98"/>
-      <c r="AE5" s="98"/>
-      <c r="AF5" s="99"/>
+      <c r="W5" s="104"/>
+      <c r="X5" s="104"/>
+      <c r="Y5" s="104"/>
+      <c r="Z5" s="104"/>
+      <c r="AA5" s="104"/>
+      <c r="AB5" s="104"/>
+      <c r="AC5" s="104"/>
+      <c r="AD5" s="104"/>
+      <c r="AE5" s="104"/>
+      <c r="AF5" s="105"/>
     </row>
     <row r="6" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
@@ -14720,33 +14720,33 @@
         <v>70.928000000000011</v>
       </c>
       <c r="H30" s="12"/>
-      <c r="I30" s="98" t="s">
+      <c r="I30" s="104" t="s">
         <v>17</v>
       </c>
-      <c r="J30" s="98"/>
-      <c r="K30" s="98"/>
-      <c r="L30" s="98"/>
-      <c r="M30" s="98"/>
-      <c r="N30" s="98"/>
-      <c r="O30" s="98"/>
-      <c r="P30" s="98"/>
-      <c r="Q30" s="98"/>
-      <c r="R30" s="98"/>
-      <c r="S30" s="99"/>
+      <c r="J30" s="104"/>
+      <c r="K30" s="104"/>
+      <c r="L30" s="104"/>
+      <c r="M30" s="104"/>
+      <c r="N30" s="104"/>
+      <c r="O30" s="104"/>
+      <c r="P30" s="104"/>
+      <c r="Q30" s="104"/>
+      <c r="R30" s="104"/>
+      <c r="S30" s="105"/>
       <c r="U30" s="12"/>
-      <c r="V30" s="98" t="s">
+      <c r="V30" s="104" t="s">
         <v>15</v>
       </c>
-      <c r="W30" s="98"/>
-      <c r="X30" s="98"/>
-      <c r="Y30" s="98"/>
-      <c r="Z30" s="98"/>
-      <c r="AA30" s="98"/>
-      <c r="AB30" s="98"/>
-      <c r="AC30" s="98"/>
-      <c r="AD30" s="98"/>
-      <c r="AE30" s="98"/>
-      <c r="AF30" s="99"/>
+      <c r="W30" s="104"/>
+      <c r="X30" s="104"/>
+      <c r="Y30" s="104"/>
+      <c r="Z30" s="104"/>
+      <c r="AA30" s="104"/>
+      <c r="AB30" s="104"/>
+      <c r="AC30" s="104"/>
+      <c r="AD30" s="104"/>
+      <c r="AE30" s="104"/>
+      <c r="AF30" s="105"/>
     </row>
     <row r="31" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B31" s="29" t="s">
@@ -16846,998 +16846,958 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M51"/>
+  <dimension ref="A1:N51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="K49" sqref="K49"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="G56" sqref="G56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="3" max="6" width="15.85546875" customWidth="1"/>
-    <col min="7" max="8" width="11.7109375" customWidth="1"/>
-    <col min="9" max="9" width="23" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" customWidth="1"/>
+    <col min="4" max="7" width="15.85546875" customWidth="1"/>
+    <col min="8" max="9" width="11.7109375" customWidth="1"/>
+    <col min="10" max="10" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B1" s="100" t="s">
+    <row r="1" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C1" s="106" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="100"/>
-      <c r="D1" s="100"/>
-      <c r="E1" s="100"/>
-      <c r="F1" s="100"/>
-      <c r="G1" s="100"/>
-    </row>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+      <c r="D1" s="106"/>
+      <c r="E1" s="106"/>
+      <c r="F1" s="106"/>
+      <c r="G1" s="106"/>
+      <c r="H1" s="106"/>
+    </row>
+    <row r="2" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
         <v>22</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>23</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>24</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>25</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>26</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>29</v>
       </c>
-      <c r="M2" s="59">
+      <c r="N2" s="59">
         <f>Archive!G11</f>
         <v>4.6956521739130439</v>
       </c>
     </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B3">
+    <row r="3" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C3">
         <v>18445</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>20460</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>7336</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>9072</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>4574</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>635</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>30</v>
       </c>
-      <c r="M3" s="7">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B4">
+      <c r="N3" s="7">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C4">
         <v>29891</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>9445</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>13242</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>4651</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>2510</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>1188</v>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B5">
+    <row r="5" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C5">
         <v>19315</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>19653</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>6885</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>9083</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>3910</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>600</v>
       </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B6">
+    <row r="6" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C6">
         <v>29235</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>9778</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>13148</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>4597</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>3034</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>1508</v>
       </c>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B7">
+    <row r="7" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C7">
         <v>21002</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>18773</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>7065</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>8771</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>4191</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>640</v>
       </c>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B8">
+    <row r="8" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C8">
         <v>27283</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>11070</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>14108</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>5558</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>2836</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>1088</v>
       </c>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B9">
+    <row r="9" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C9">
         <v>22479</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>19404</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>6940</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>8009</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>4114</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>820</v>
       </c>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B10">
+    <row r="10" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C10">
         <v>27783</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>12290</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>13147</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>6203</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>3097</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>1316</v>
       </c>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B11">
+    <row r="11" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C11">
         <v>22991</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>18022</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>6987</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>8034</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>4352</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>726</v>
       </c>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B12">
+    <row r="12" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C12">
         <v>25478</v>
       </c>
-      <c r="C12">
+      <c r="D12">
         <v>11329</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>14167</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>5533</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>2912</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>924</v>
       </c>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B13">
+    <row r="13" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C13">
         <v>23336</v>
       </c>
-      <c r="C13">
+      <c r="D13">
         <v>16534</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <v>6269</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>7335</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>3293</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>987</v>
       </c>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B14" s="24">
+    <row r="14" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C14" s="24">
         <v>26263</v>
       </c>
-      <c r="C14" s="24">
+      <c r="D14" s="24">
         <v>13461</v>
       </c>
-      <c r="D14" s="24">
+      <c r="E14" s="24">
         <v>11141</v>
       </c>
-      <c r="E14" s="24">
+      <c r="F14" s="24">
         <v>6447</v>
       </c>
-      <c r="F14" s="24">
+      <c r="G14" s="24">
         <v>3054</v>
       </c>
-      <c r="G14" s="24">
+      <c r="H14" s="24">
         <v>1011</v>
       </c>
-      <c r="H14" s="24"/>
-    </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B15" s="25">
-        <f>SUM(B3:B14)</f>
+      <c r="I14" s="24"/>
+    </row>
+    <row r="15" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C15" s="25">
+        <f>SUM(C3:C14)</f>
         <v>293501</v>
       </c>
-      <c r="C15" s="25">
-        <f t="shared" ref="C15:G15" si="0">SUM(C3:C14)</f>
+      <c r="D15" s="25">
+        <f t="shared" ref="D15:H15" si="0">SUM(D3:D14)</f>
         <v>180219</v>
       </c>
-      <c r="D15" s="25">
+      <c r="E15" s="25">
         <f t="shared" si="0"/>
         <v>120435</v>
       </c>
-      <c r="E15" s="25">
+      <c r="F15" s="25">
         <f t="shared" si="0"/>
         <v>83293</v>
       </c>
-      <c r="F15" s="25">
+      <c r="G15" s="25">
         <f t="shared" si="0"/>
         <v>41877</v>
       </c>
-      <c r="G15" s="25">
+      <c r="H15" s="25">
         <f t="shared" si="0"/>
         <v>11443</v>
       </c>
-      <c r="H15" s="26">
-        <f>SUM(B15:G15)</f>
+      <c r="I15" s="26">
+        <f>SUM(C15:H15)</f>
         <v>730768</v>
       </c>
-      <c r="I15" t="s">
+      <c r="J15" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B16" s="27">
-        <f>B15/$H$15</f>
+    <row r="16" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C16" s="27">
+        <f>C15/$I$15</f>
         <v>0.40163362380399797</v>
       </c>
-      <c r="C16" s="27">
-        <f t="shared" ref="C16:G16" si="1">C15/$H$15</f>
+      <c r="D16" s="27">
+        <f t="shared" ref="D16:H16" si="1">D15/$I$15</f>
         <v>0.24661588903728679</v>
       </c>
-      <c r="D16" s="27">
+      <c r="E16" s="27">
         <f t="shared" si="1"/>
         <v>0.16480606704179712</v>
       </c>
-      <c r="E16" s="27">
+      <c r="F16" s="27">
         <f t="shared" si="1"/>
         <v>0.11398008670330392</v>
       </c>
-      <c r="F16" s="27">
+      <c r="G16" s="27">
         <f t="shared" si="1"/>
         <v>5.7305464935519891E-2</v>
       </c>
-      <c r="G16" s="27">
+      <c r="H16" s="27">
         <f t="shared" si="1"/>
         <v>1.5658868478094279E-2</v>
       </c>
-      <c r="H16" t="s">
+      <c r="I16" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B18" s="25">
-        <f t="shared" ref="B18:G18" si="2">B16*$M$2*$M$3</f>
-        <v>39.604567773368153</v>
-      </c>
+    <row r="18" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C18" s="25">
-        <f t="shared" si="2"/>
-        <v>24.318471145068109</v>
+        <f t="shared" ref="C18:H18" si="2">C16*$N$2*$N$3</f>
+        <v>79.209135546736306</v>
       </c>
       <c r="D18" s="25">
         <f t="shared" si="2"/>
-        <v>16.251311306556342</v>
+        <v>48.636942290136219</v>
       </c>
       <c r="E18" s="25">
         <f t="shared" si="2"/>
-        <v>11.239427680134492</v>
+        <v>32.502622613112685</v>
       </c>
       <c r="F18" s="25">
         <f t="shared" si="2"/>
-        <v>5.6508171510330056</v>
+        <v>22.478855360268984</v>
       </c>
       <c r="G18" s="25">
         <f t="shared" si="2"/>
-        <v>1.5441005960138185</v>
-      </c>
-      <c r="H18" t="s">
+        <v>11.301634302066011</v>
+      </c>
+      <c r="H18" s="25">
+        <f t="shared" si="2"/>
+        <v>3.0882011920276371</v>
+      </c>
+      <c r="I18" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="25">
-        <f>B18/2</f>
-        <v>19.802283886684076</v>
-      </c>
+    <row r="19" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C19" s="25">
-        <f t="shared" ref="C19:F19" si="3">C18/2</f>
-        <v>12.159235572534055</v>
+        <f>C18/2</f>
+        <v>39.604567773368153</v>
       </c>
       <c r="D19" s="25">
-        <f t="shared" si="3"/>
-        <v>8.1256556532781712</v>
+        <f t="shared" ref="D19:G19" si="3">D18/2</f>
+        <v>24.318471145068109</v>
       </c>
       <c r="E19" s="25">
         <f t="shared" si="3"/>
-        <v>5.6197138400672459</v>
+        <v>16.251311306556342</v>
       </c>
       <c r="F19" s="25">
         <f t="shared" si="3"/>
-        <v>2.8254085755165028</v>
+        <v>11.239427680134492</v>
       </c>
       <c r="G19" s="25">
-        <f>G18/2</f>
-        <v>0.77205029800690927</v>
-      </c>
-      <c r="H19" t="s">
+        <f t="shared" si="3"/>
+        <v>5.6508171510330056</v>
+      </c>
+      <c r="H19" s="25">
+        <f>H18/2</f>
+        <v>1.5441005960138185</v>
+      </c>
+      <c r="I19" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B21" s="10">
-        <f>B16/$G$16</f>
+    <row r="21" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C21" s="10">
+        <f>C16/$H$16</f>
         <v>25.648955693437035</v>
       </c>
-      <c r="C21" s="10">
-        <f t="shared" ref="C21:G21" si="4">C16/$G$16</f>
+      <c r="D21" s="10">
+        <f t="shared" ref="D21:H21" si="4">D16/$H$16</f>
         <v>15.749279035218036</v>
       </c>
-      <c r="D21" s="10">
+      <c r="E21" s="10">
         <f t="shared" si="4"/>
         <v>10.524774971598356</v>
       </c>
-      <c r="E21" s="10">
+      <c r="F21" s="10">
         <f t="shared" si="4"/>
         <v>7.2789478283666869</v>
       </c>
-      <c r="F21" s="10">
+      <c r="G21" s="10">
         <f t="shared" si="4"/>
         <v>3.6596172332430306</v>
       </c>
-      <c r="G21" s="10">
+      <c r="H21" s="10">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="H21" t="s">
+      <c r="I21" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B22" s="65">
-        <f>1/B21</f>
+    <row r="22" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C22" s="65">
+        <f>1/C21</f>
         <v>3.8987942119447637E-2</v>
       </c>
-      <c r="C22" s="65">
-        <f t="shared" ref="C22:G22" si="5">1/C21</f>
+      <c r="D22" s="65">
+        <f t="shared" ref="D22:H22" si="5">1/D21</f>
         <v>6.3494970008711626E-2</v>
       </c>
-      <c r="D22" s="65">
+      <c r="E22" s="65">
         <f t="shared" si="5"/>
         <v>9.5013907917133725E-2</v>
       </c>
-      <c r="E22" s="65">
+      <c r="F22" s="65">
         <f t="shared" si="5"/>
         <v>0.13738249312667331</v>
       </c>
-      <c r="F22" s="65">
+      <c r="G22" s="65">
         <f t="shared" si="5"/>
         <v>0.27325262077035128</v>
       </c>
-      <c r="G22" s="65">
+      <c r="H22" s="65">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="H22" t="s">
+      <c r="I22" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B24" s="83" t="s">
+    <row r="24" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C24" s="83" t="s">
         <v>81</v>
       </c>
-      <c r="C24" s="84"/>
       <c r="D24" s="84"/>
       <c r="E24" s="84"/>
       <c r="F24" s="84"/>
       <c r="G24" s="84"/>
-      <c r="H24" s="21"/>
-      <c r="I24" s="31"/>
-    </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B25" s="1">
+      <c r="H24" s="84"/>
+      <c r="I24" s="21"/>
+      <c r="J24" s="31"/>
+    </row>
+    <row r="25" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C25" s="1">
         <v>25.36</v>
       </c>
-      <c r="C25" s="13">
+      <c r="D25" s="13">
         <v>15.5</v>
       </c>
-      <c r="D25" s="13">
+      <c r="E25" s="13">
         <v>10.47</v>
       </c>
-      <c r="E25" s="13">
+      <c r="F25" s="13">
         <v>7.12</v>
       </c>
-      <c r="F25" s="13">
+      <c r="G25" s="13">
         <v>3.65</v>
       </c>
-      <c r="G25" s="85">
+      <c r="H25" s="85">
         <v>1</v>
       </c>
-      <c r="H25" s="13" t="s">
+      <c r="I25" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="I25" s="14"/>
-    </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B26" s="86">
-        <f>B25/SUM($B$25:$G$25)</f>
+      <c r="J25" s="14"/>
+    </row>
+    <row r="26" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C26" s="86">
+        <f>C25/SUM($C$25:$H$25)</f>
         <v>0.40190174326465927</v>
       </c>
-      <c r="C26" s="37">
-        <f t="shared" ref="C26:G26" si="6">C25/SUM($B$25:$G$25)</f>
+      <c r="D26" s="37">
+        <f t="shared" ref="D26:H26" si="6">D25/SUM($C$25:$H$25)</f>
         <v>0.24564183835182252</v>
       </c>
-      <c r="D26" s="37">
+      <c r="E26" s="37">
         <f t="shared" si="6"/>
         <v>0.16592709984152143</v>
       </c>
-      <c r="E26" s="37">
+      <c r="F26" s="37">
         <f t="shared" si="6"/>
         <v>0.1128367670364501</v>
       </c>
-      <c r="F26" s="37">
+      <c r="G26" s="37">
         <f t="shared" si="6"/>
         <v>5.7844690966719493E-2</v>
       </c>
-      <c r="G26" s="37">
+      <c r="H26" s="37">
         <f t="shared" si="6"/>
         <v>1.5847860538827259E-2</v>
       </c>
-      <c r="H26" s="13"/>
-      <c r="I26" s="14"/>
-    </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B27" s="87">
-        <f>B26*$M$2*$M$3</f>
-        <v>39.631006683662925</v>
-      </c>
-      <c r="C27" s="88">
-        <f t="shared" ref="C27:G27" si="7">C26*$M$2*$M$3</f>
-        <v>24.222421277475373</v>
+      <c r="I26" s="13"/>
+      <c r="J26" s="14"/>
+    </row>
+    <row r="27" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C27" s="87">
+        <f>C26*$N$2*$N$3</f>
+        <v>79.262013367325849</v>
       </c>
       <c r="D27" s="88">
-        <f t="shared" si="7"/>
-        <v>16.361854888720462</v>
+        <f t="shared" ref="D27:H27" si="7">D26*$N$2*$N$3</f>
+        <v>48.444842554950746</v>
       </c>
       <c r="E27" s="88">
         <f t="shared" si="7"/>
-        <v>11.126686419072559</v>
+        <v>32.723709777440924</v>
       </c>
       <c r="F27" s="88">
         <f t="shared" si="7"/>
-        <v>5.7039895266312968</v>
+        <v>22.253372838145118</v>
       </c>
       <c r="G27" s="88">
         <f t="shared" si="7"/>
-        <v>1.5627368566113142</v>
-      </c>
-      <c r="H27" s="13" t="s">
+        <v>11.407979053262594</v>
+      </c>
+      <c r="H27" s="88">
+        <f t="shared" si="7"/>
+        <v>3.1254737132226285</v>
+      </c>
+      <c r="I27" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="I27" s="14"/>
-    </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B28" s="89">
-        <f>B27/47*24</f>
-        <v>20.237109795912982</v>
-      </c>
+      <c r="J27" s="14"/>
+    </row>
+    <row r="28" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C28" s="89">
-        <f t="shared" ref="C28:G28" si="8">C27/47*24</f>
-        <v>12.368895971476785</v>
+        <f>C27/47*24</f>
+        <v>40.474219591825964</v>
       </c>
       <c r="D28" s="89">
-        <f t="shared" si="8"/>
-        <v>8.3549897304104483</v>
+        <f t="shared" ref="D28:H28" si="8">D27/47*24</f>
+        <v>24.737791942953571</v>
       </c>
       <c r="E28" s="89">
         <f t="shared" si="8"/>
-        <v>5.6817122139944978</v>
+        <v>16.709979460820897</v>
       </c>
       <c r="F28" s="89">
         <f t="shared" si="8"/>
-        <v>2.9126755029606621</v>
+        <v>11.363424427988996</v>
       </c>
       <c r="G28" s="89">
         <f t="shared" si="8"/>
-        <v>0.79799328848237328</v>
-      </c>
-      <c r="H28" s="24" t="s">
+        <v>5.8253510059213243</v>
+      </c>
+      <c r="H28" s="89">
+        <f t="shared" si="8"/>
+        <v>1.5959865769647466</v>
+      </c>
+      <c r="I28" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="I28" s="34"/>
-    </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
+      <c r="J28" s="34"/>
+    </row>
+    <row r="32" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
         <v>85</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>88</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
         <v>89</v>
       </c>
-      <c r="E32" t="s">
+      <c r="F32" t="s">
         <v>90</v>
       </c>
-      <c r="F32" t="s">
+      <c r="G32" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
         <v>22</v>
       </c>
-      <c r="C33">
+      <c r="D33">
         <v>0.17</v>
       </c>
-      <c r="D33">
+      <c r="E33">
         <v>0.24</v>
       </c>
-      <c r="E33">
+      <c r="F33">
         <v>0.44</v>
       </c>
-      <c r="F33">
+      <c r="G33">
         <v>0.61</v>
       </c>
-      <c r="I33">
-        <f>C33/24</f>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>23</v>
+      </c>
+      <c r="D34">
+        <v>1.64</v>
+      </c>
+      <c r="F34">
+        <f>1.49+0.62+8.06</f>
+        <v>10.17</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>86</v>
+      </c>
+      <c r="D35">
+        <v>2.72</v>
+      </c>
+      <c r="E35">
+        <v>0.24</v>
+      </c>
+      <c r="F35">
+        <v>0.44</v>
+      </c>
+      <c r="G35">
+        <v>5.88</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>87</v>
+      </c>
+      <c r="D36">
+        <v>4.54</v>
+      </c>
+      <c r="E36">
+        <v>1.23</v>
+      </c>
+      <c r="F36">
+        <v>0.88</v>
+      </c>
+      <c r="G36">
+        <v>14.28</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>92</v>
+      </c>
+      <c r="D38" t="s">
+        <v>88</v>
+      </c>
+      <c r="E38" t="s">
+        <v>89</v>
+      </c>
+      <c r="F38" t="s">
+        <v>90</v>
+      </c>
+      <c r="G38" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>22</v>
+      </c>
+      <c r="D39">
+        <f>D33*$C$28/24</f>
+        <v>0.28669238877543396</v>
+      </c>
+      <c r="E39">
+        <f t="shared" ref="E39:G39" si="9">E33*$C$28/24</f>
+        <v>0.40474219591825961</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="9"/>
+        <v>0.74202735918347607</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="9"/>
+        <v>1.0287197479589099</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>23</v>
+      </c>
+      <c r="D40">
+        <f>D34*$D$28/24</f>
+        <v>1.690415782768494</v>
+      </c>
+      <c r="E40">
+        <f t="shared" ref="E40:G40" si="10">E34*$D$28/24</f>
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="10"/>
+        <v>10.482639335826576</v>
+      </c>
+      <c r="G40">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>86</v>
+      </c>
+      <c r="D41">
+        <f>D35*$E$28/24</f>
+        <v>1.8937976722263683</v>
+      </c>
+      <c r="E41">
+        <f t="shared" ref="E41:G41" si="11">E35*$E$28/24</f>
+        <v>0.16709979460820898</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="11"/>
+        <v>0.30634962344838312</v>
+      </c>
+      <c r="G41">
+        <f t="shared" si="11"/>
+        <v>4.0939449679011197</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
+        <v>87</v>
+      </c>
+      <c r="D42" s="24">
+        <f>D36*$G$28/24</f>
+        <v>1.1019622319534506</v>
+      </c>
+      <c r="E42" s="24">
+        <f t="shared" ref="E42:G42" si="12">E36*$G$28/24</f>
+        <v>0.29854923905346786</v>
+      </c>
+      <c r="F42" s="24">
+        <f t="shared" si="12"/>
+        <v>0.21359620355044853</v>
+      </c>
+      <c r="G42" s="24">
+        <f t="shared" si="12"/>
+        <v>3.4660838485231875</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D43">
+        <f>SUM(D39:D42)</f>
+        <v>4.9728680757237473</v>
+      </c>
+      <c r="E43">
+        <f t="shared" ref="E43:G43" si="13">SUM(E39:E42)</f>
+        <v>0.87039122957993642</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="13"/>
+        <v>11.744612522008884</v>
+      </c>
+      <c r="G43">
+        <f t="shared" si="13"/>
+        <v>8.5887485643832164</v>
+      </c>
+      <c r="H43">
+        <f>SUM(D43:G43)</f>
+        <v>26.176620391695785</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>92</v>
+      </c>
+      <c r="D46" t="s">
+        <v>88</v>
+      </c>
+      <c r="E46" t="s">
+        <v>89</v>
+      </c>
+      <c r="F46" t="s">
+        <v>90</v>
+      </c>
+      <c r="G46" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>1</v>
+      </c>
+      <c r="B47">
+        <f>C28*A47</f>
+        <v>40.474219591825964</v>
+      </c>
+      <c r="C47" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D47" s="90">
         <v>7.0833333333333338E-3</v>
       </c>
-      <c r="J33">
-        <f t="shared" ref="J33:L36" si="9">D33/24</f>
+      <c r="E47" s="90">
         <v>0.01</v>
       </c>
-      <c r="K33">
-        <f t="shared" si="9"/>
+      <c r="F47" s="90">
         <v>1.8333333333333333E-2</v>
       </c>
-      <c r="L33">
-        <f t="shared" si="9"/>
+      <c r="G47" s="91">
         <v>2.5416666666666667E-2</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
+      <c r="I47">
+        <f>G47*B47</f>
+        <v>1.0287197479589099</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>0</v>
+      </c>
+      <c r="B48">
+        <f>D28*A48</f>
+        <v>0</v>
+      </c>
+      <c r="C48" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C34">
-        <v>1.64</v>
-      </c>
-      <c r="E34">
-        <f>1.49+0.62</f>
-        <v>2.11</v>
-      </c>
-      <c r="F34">
-        <v>8.06</v>
-      </c>
-      <c r="I34">
-        <f t="shared" ref="I34:I36" si="10">C34/24</f>
+      <c r="D48" s="92">
         <v>6.8333333333333329E-2</v>
       </c>
-      <c r="J34">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="K34">
-        <f t="shared" si="9"/>
-        <v>8.7916666666666657E-2</v>
-      </c>
-      <c r="L34">
-        <f t="shared" si="9"/>
-        <v>0.33583333333333337</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
+      <c r="E48" s="92">
+        <v>0</v>
+      </c>
+      <c r="F48" s="92">
+        <f>0.0879166666666667+0.335833333333333</f>
+        <v>0.42374999999999968</v>
+      </c>
+      <c r="G48" s="93"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>1</v>
+      </c>
+      <c r="B49">
+        <f>E28*A49</f>
+        <v>16.709979460820897</v>
+      </c>
+      <c r="C49" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C35">
-        <v>2.72</v>
-      </c>
-      <c r="D35">
-        <v>0.24</v>
-      </c>
-      <c r="E35">
-        <v>0.44</v>
-      </c>
-      <c r="F35">
-        <v>5.88</v>
-      </c>
-      <c r="I35">
-        <f t="shared" si="10"/>
+      <c r="D49" s="92">
         <v>0.11333333333333334</v>
       </c>
-      <c r="J35">
-        <f t="shared" si="9"/>
+      <c r="E49" s="92">
         <v>0.01</v>
       </c>
-      <c r="K35">
-        <f t="shared" si="9"/>
+      <c r="F49" s="92">
         <v>1.8333333333333333E-2</v>
       </c>
-      <c r="L35">
-        <f t="shared" si="9"/>
+      <c r="G49" s="93">
         <v>0.245</v>
       </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
+      <c r="I49">
+        <f>G49*B49</f>
+        <v>4.0939449679011197</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>1</v>
+      </c>
+      <c r="B50">
+        <f>G28*A50</f>
+        <v>5.8253510059213243</v>
+      </c>
+      <c r="C50" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="C36">
-        <v>4.54</v>
-      </c>
-      <c r="D36">
-        <v>1.23</v>
-      </c>
-      <c r="E36">
-        <v>0.88</v>
-      </c>
-      <c r="F36">
-        <v>14.28</v>
-      </c>
-      <c r="I36">
-        <f t="shared" si="10"/>
+      <c r="D50" s="94">
         <v>0.18916666666666668</v>
       </c>
-      <c r="J36">
-        <f t="shared" si="9"/>
+      <c r="E50" s="94">
         <v>5.1249999999999997E-2</v>
       </c>
-      <c r="K36">
-        <f t="shared" si="9"/>
+      <c r="F50" s="94">
         <v>3.6666666666666667E-2</v>
       </c>
-      <c r="L36">
-        <f t="shared" si="9"/>
+      <c r="G50" s="95">
         <v>0.59499999999999997</v>
       </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
-        <v>92</v>
-      </c>
-      <c r="C38" t="s">
-        <v>88</v>
-      </c>
-      <c r="D38" t="s">
-        <v>89</v>
-      </c>
-      <c r="E38" t="s">
-        <v>90</v>
-      </c>
-      <c r="F38" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
-        <v>22</v>
-      </c>
-      <c r="C39">
-        <f>C33*$B$28/24</f>
-        <v>0.14334619438771698</v>
-      </c>
-      <c r="D39">
-        <f t="shared" ref="D39:F39" si="11">D33*$B$28/24</f>
-        <v>0.2023710979591298</v>
-      </c>
-      <c r="E39">
-        <f t="shared" si="11"/>
-        <v>0.37101367959173803</v>
-      </c>
-      <c r="F39">
-        <f t="shared" si="11"/>
-        <v>0.51435987397945493</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
-        <v>23</v>
-      </c>
-      <c r="C40">
-        <f>C34*$C$28/24</f>
-        <v>0.84520789138424701</v>
-      </c>
-      <c r="D40">
-        <f t="shared" ref="D40:F40" si="12">D34*$C$28/24</f>
-        <v>0</v>
-      </c>
-      <c r="E40">
-        <f t="shared" si="12"/>
-        <v>1.0874321041590007</v>
-      </c>
-      <c r="F40">
-        <f t="shared" si="12"/>
-        <v>4.1538875637542878</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
-        <v>86</v>
-      </c>
-      <c r="C41">
-        <f>C35*$D$28/24</f>
-        <v>0.94689883611318415</v>
-      </c>
-      <c r="D41">
-        <f t="shared" ref="D41:F41" si="13">D35*$D$28/24</f>
-        <v>8.354989730410449E-2</v>
-      </c>
-      <c r="E41">
-        <f t="shared" si="13"/>
-        <v>0.15317481172419156</v>
-      </c>
-      <c r="F41">
-        <f t="shared" si="13"/>
-        <v>2.0469724839505599</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
-        <v>87</v>
-      </c>
-      <c r="C42" s="24">
-        <f>C36*$E$28/24</f>
-        <v>1.0747905604806258</v>
-      </c>
-      <c r="D42" s="24">
-        <f t="shared" ref="D42:F42" si="14">D36*$E$28/24</f>
-        <v>0.291187750967218</v>
-      </c>
-      <c r="E42" s="24">
+      <c r="I50">
+        <f>G50*B50</f>
+        <v>3.466083848523188</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D51">
+        <f>SUMPRODUCT($B$47:$B$50,D47:D50)</f>
+        <v>3.2824522929552531</v>
+      </c>
+      <c r="E51">
+        <f t="shared" ref="E51:G51" si="14">SUMPRODUCT($B$47:$B$50,E47:E50)</f>
+        <v>0.87039122957993653</v>
+      </c>
+      <c r="F51">
         <f t="shared" si="14"/>
-        <v>0.20832944784646493</v>
-      </c>
-      <c r="F42" s="24">
+        <v>1.2619731861823078</v>
+      </c>
+      <c r="G51">
         <f t="shared" si="14"/>
-        <v>3.3806187673267263</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C43">
-        <f>SUM(C39:C42)</f>
-        <v>3.010243482365774</v>
-      </c>
-      <c r="D43">
-        <f t="shared" ref="D43:F43" si="15">SUM(D39:D42)</f>
-        <v>0.57710874623045227</v>
-      </c>
-      <c r="E43">
-        <f t="shared" si="15"/>
-        <v>1.8199500433213953</v>
-      </c>
-      <c r="F43">
-        <f t="shared" si="15"/>
-        <v>10.095838689011028</v>
-      </c>
-      <c r="G43">
-        <f>SUM(C43:F43)</f>
-        <v>15.503140960928651</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
-        <v>92</v>
-      </c>
-      <c r="C46" t="s">
-        <v>88</v>
-      </c>
-      <c r="D46" t="s">
-        <v>89</v>
-      </c>
-      <c r="E46" t="s">
-        <v>90</v>
-      </c>
-      <c r="F46" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>20.399999999999999</v>
-      </c>
-      <c r="B47" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="C47" s="101">
-        <v>7.0833333333333338E-3</v>
-      </c>
-      <c r="D47" s="101">
-        <v>0.01</v>
-      </c>
-      <c r="E47" s="101">
-        <v>1.8333333333333333E-2</v>
-      </c>
-      <c r="F47" s="102">
-        <v>2.5416666666666667E-2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>12.4</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C48" s="103">
-        <v>6.8333333333333329E-2</v>
-      </c>
-      <c r="D48" s="103">
-        <v>0</v>
-      </c>
-      <c r="E48" s="103">
-        <v>8.7916666666666657E-2</v>
-      </c>
-      <c r="F48" s="104">
-        <v>0.33583333333333337</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>8.4</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C49" s="103">
-        <v>0.11333333333333334</v>
-      </c>
-      <c r="D49" s="103">
-        <v>0.01</v>
-      </c>
-      <c r="E49" s="103">
-        <v>1.8333333333333333E-2</v>
-      </c>
-      <c r="F49" s="104">
-        <v>0.245</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <v>5.7</v>
-      </c>
-      <c r="B50" s="29" t="s">
-        <v>87</v>
-      </c>
-      <c r="C50" s="105">
-        <v>0.18916666666666668</v>
-      </c>
-      <c r="D50" s="105">
-        <v>5.1249999999999997E-2</v>
-      </c>
-      <c r="E50" s="105">
-        <v>3.6666666666666667E-2</v>
-      </c>
-      <c r="F50" s="106">
-        <v>0.59499999999999997</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C51">
-        <f>SUMPRODUCT($A$47:$A$50,C47:C50)</f>
-        <v>3.0220833333333337</v>
-      </c>
-      <c r="D51">
-        <f t="shared" ref="D51:F51" si="16">SUMPRODUCT($A$47:$A$50,D47:D50)</f>
-        <v>0.580125</v>
-      </c>
-      <c r="E51">
-        <f t="shared" si="16"/>
-        <v>1.8271666666666664</v>
-      </c>
-      <c r="F51">
-        <f t="shared" si="16"/>
-        <v>10.132333333333335</v>
-      </c>
-      <c r="G51">
-        <f>SUM(C51:F51)</f>
-        <v>15.561708333333335</v>
+        <v>8.5887485643832164</v>
+      </c>
+      <c r="H51">
+        <f>SUM(D51:G51)</f>
+        <v>14.003565273100714</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="C1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>